<commit_message>
Inflation wired up to Excel (working example)
</commit_message>
<xml_diff>
--- a/examples/Qwack - YeildCurveExample (Frozen Data).xlsx
+++ b/examples/Qwack - YeildCurveExample (Frozen Data).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Qwack\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAFD43B-C02A-414F-B042-C9AC991E3CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6777C76-B8D1-4DF3-9F65-23C8750A746E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="92">
   <si>
     <t>3m</t>
   </si>
@@ -271,9 +271,6 @@
     <t>Infation Index</t>
   </si>
   <si>
-    <t>US.CPI</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -290,6 +287,63 @@
   </si>
   <si>
     <t>Act365</t>
+  </si>
+  <si>
+    <t>Inflation Swaps</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Tenor</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>USD.CPI</t>
+  </si>
+  <si>
+    <t>Funding Instrument Collection</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>ModelCPI</t>
+  </si>
+  <si>
+    <t>FicCPI</t>
+  </si>
+  <si>
+    <t>Solve Stages</t>
+  </si>
+  <si>
+    <t>CPI Fixings</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Curves</t>
+  </si>
+  <si>
+    <t>USD Libor</t>
+  </si>
+  <si>
+    <t>Lag</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>AssetFxModel</t>
+  </si>
+  <si>
+    <t>Porfolio</t>
+  </si>
+  <si>
+    <t>Cashflows</t>
   </si>
 </sst>
 </file>
@@ -300,7 +354,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,8 +369,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,7 +420,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -353,6 +429,39 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -370,6 +479,1092 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CPI!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CPI!$J$3:$J$35</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>43930</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44205</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44295</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44386</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44478</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44570</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44660</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44751</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44843</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44935</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45025</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45116</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45208</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45391</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45482</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45574</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45666</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45756</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45847</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45939</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>46031</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>46121</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>46212</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>46304</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>46396</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>46486</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>46577</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>46669</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>46761</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>46852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CPI!$M$3:$M$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>100.05308829634575</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101.56136075610513</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.08432470555356</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104.61791490204203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.12168591165967</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107.65295686520498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109.35558564506148</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>111.14293781232169</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>113.02471112207618</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>114.94820586348568</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>117.02564362611034</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>119.22338337900035</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>121.51481631861036</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>123.79859320175402</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>126.14512285807679</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>128.50509420877495</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130.89357541207272</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>133.27823562988155</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>135.75660866681818</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>138.35111982193467</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>141.07769688759015</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>143.86042465357392</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>146.82167910410232</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>149.88392218361739</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>153.02823461613627</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>156.13676504321063</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>159.36834522746165</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>162.6775589612019</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>166.04418259794028</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>169.34377748516795</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>172.74570841995714</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>176.20137882673822</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>179.68947192352954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-75A1-43AC-B153-E5E809566640}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="296818319"/>
+        <c:axId val="296822159"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="296818319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="47100"/>
+          <c:min val="43800"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296822159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="296822159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="80"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296818319"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9786967-DE07-7DB8-FDF2-B622829DC141}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1410,7 +2605,7 @@
   <dimension ref="B1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,7 +3580,7 @@
   <dimension ref="B1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,14 +3609,14 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("ZAR.JIBAR.3M","ZAR","3M","Act365F","Act365F","3M","JHB","0b","MF")</f>
-        <v>ZAR.JIBAR.3M¬19</v>
+        <v>ZAR.JIBAR.3M¬2</v>
       </c>
       <c r="I2" t="s">
         <v>25</v>
       </c>
       <c r="J2" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("USD.LIBOR.3M","USD","3M","Act360","Act360","6M","NYC","2b","MF")</f>
-        <v>USD.LIBOR.3M¬8</v>
+        <v>USD.LIBOR.3M¬2</v>
       </c>
       <c r="V2" s="3"/>
     </row>
@@ -2431,14 +3626,14 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("ZAR.OIS.1B","ZAR","3M","Act365F","Act365F","3M","JHB","0b","MF")</f>
-        <v>ZAR.OIS.1B¬12</v>
+        <v>ZAR.OIS.1B¬2</v>
       </c>
       <c r="I3" t="s">
         <v>31</v>
       </c>
       <c r="J3" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("USD.OIS.1B","USD","3M","Act360","Act360","3M","NYC","0b","MF")</f>
-        <v>USD.OIS.1B¬8</v>
+        <v>USD.OIS.1B¬2</v>
       </c>
       <c r="V3" t="s">
         <v>36</v>
@@ -2523,7 +3718,7 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B6,valDate,"0x3",index,"ZAR",E6,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_3m¬6</v>
+        <v>ZAROISFra_3m¬2</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -2540,7 +3735,7 @@
       </c>
       <c r="M6" t="str">
         <f ca="1">_xll.QIns_CreateFRA("USDOISFra_"&amp;I6,valDate,"0x3",J2,"USD",L6,1,"USD.LIBOR.3M","USD.OIS.1B",,,"USD.LIBOR.3M")</f>
-        <v>USDOISFra_3m¬6</v>
+        <v>USDOISFra_3m¬2</v>
       </c>
       <c r="O6" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P6,"F","JHB+NYC")</f>
@@ -2558,7 +3753,7 @@
       </c>
       <c r="S6" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P6,O6,"ZAR","USD",1000000,R6,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_1w¬6</v>
+        <v>ZARFwd_1w¬2</v>
       </c>
       <c r="U6" s="2">
         <f t="shared" ref="U6:U37" ca="1" si="0">EDATE(U5,3)</f>
@@ -2597,7 +3792,7 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B7,valDate,B7,index,"ZAR",E7,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_3x6¬6</v>
+        <v>ZAROISFra_3x6¬2</v>
       </c>
       <c r="I7" t="s">
         <v>39</v>
@@ -2615,7 +3810,7 @@
       </c>
       <c r="M7" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I7,valDate,I7,$J$2,L7,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDU8¬6</v>
+        <v>EDU8¬2</v>
       </c>
       <c r="O7" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P7,"MF","JHB+NYC")</f>
@@ -2633,7 +3828,7 @@
       </c>
       <c r="S7" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P7,O7,"ZAR","USD",1000000,R7,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_1m¬6</v>
+        <v>ZARFwd_1m¬2</v>
       </c>
       <c r="U7" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -2672,7 +3867,7 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B8,valDate,B8,index,"ZAR",E8,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_6x9¬6</v>
+        <v>ZAROISFra_6x9¬2</v>
       </c>
       <c r="I8" t="s">
         <v>40</v>
@@ -2690,7 +3885,7 @@
       </c>
       <c r="M8" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I8,valDate,I8,$J$2,L8,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDZ8¬6</v>
+        <v>EDZ8¬2</v>
       </c>
       <c r="O8" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P8,"MF","JHB+NYC")</f>
@@ -2708,7 +3903,7 @@
       </c>
       <c r="S8" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P8,O8,"ZAR","USD",1000000,R8,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_2m¬6</v>
+        <v>ZARFwd_2m¬2</v>
       </c>
       <c r="U8" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -2747,7 +3942,7 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B9,valDate,B9,index,"ZAR",E9,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_9x12¬6</v>
+        <v>ZAROISFra_9x12¬2</v>
       </c>
       <c r="I9" t="s">
         <v>42</v>
@@ -2765,7 +3960,7 @@
       </c>
       <c r="M9" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I9,valDate,I9,$J$2,L9,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDH9¬6</v>
+        <v>EDH9¬2</v>
       </c>
       <c r="O9" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P9,"MF","JHB+NYC")</f>
@@ -2783,7 +3978,7 @@
       </c>
       <c r="S9" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P9,O9,"ZAR","USD",1000000,R9,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_3m¬6</v>
+        <v>ZARFwd_3m¬2</v>
       </c>
       <c r="U9" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -2822,7 +4017,7 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B10,valDate,B10,index,"ZAR",E10,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_12x15¬6</v>
+        <v>ZAROISFra_12x15¬2</v>
       </c>
       <c r="I10" t="s">
         <v>41</v>
@@ -2840,7 +4035,7 @@
       </c>
       <c r="M10" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I10,valDate,I10,$J$2,L10,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDM9¬6</v>
+        <v>EDM9¬2</v>
       </c>
       <c r="O10" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P10,"MF","JHB+NYC")</f>
@@ -2858,7 +4053,7 @@
       </c>
       <c r="S10" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P10,O10,"ZAR","USD",1000000,R10,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_6m¬6</v>
+        <v>ZARFwd_6m¬2</v>
       </c>
       <c r="U10" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -2897,7 +4092,7 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B11,valDate,B11,index,"ZAR",E11,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_15x18¬6</v>
+        <v>ZAROISFra_15x18¬2</v>
       </c>
       <c r="I11" t="s">
         <v>43</v>
@@ -2915,7 +4110,7 @@
       </c>
       <c r="M11" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I11,valDate,I11,$J$2,L11,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDU9¬6</v>
+        <v>EDU9¬2</v>
       </c>
       <c r="O11" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P11,"MF","JHB+NYC")</f>
@@ -2933,7 +4128,7 @@
       </c>
       <c r="S11" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P11,O11,"ZAR","USD",1000000,R11,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_9m¬6</v>
+        <v>ZARFwd_9m¬2</v>
       </c>
       <c r="U11" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -2972,7 +4167,7 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B12,valDate,B12,index,E12,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_2y¬6</v>
+        <v>ZAROISSwap_2y¬2</v>
       </c>
       <c r="I12" t="s">
         <v>12</v>
@@ -2989,7 +4184,7 @@
       </c>
       <c r="M12" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I12,valDate,I12,$J$2,L12,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_2y¬6</v>
+        <v>USDOISSwap_2y¬2</v>
       </c>
       <c r="O12" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P12,"MF","JHB+NYC")</f>
@@ -3007,7 +4202,7 @@
       </c>
       <c r="S12" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P12,O12,"ZAR","USD",1000000,R12,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_12m¬6</v>
+        <v>ZARFwd_12m¬2</v>
       </c>
       <c r="U12" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3046,7 +4241,7 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B13,valDate,B13,index,E13,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_3y¬6</v>
+        <v>ZAROISSwap_3y¬2</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -3063,7 +4258,7 @@
       </c>
       <c r="M13" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I13,valDate,I13,$J$2,L13,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_3y¬6</v>
+        <v>USDOISSwap_3y¬2</v>
       </c>
       <c r="O13" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P13,"MF","JHB+NYC")</f>
@@ -3081,7 +4276,7 @@
       </c>
       <c r="S13" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P13,O13,"ZAR","USD",1000000,R13,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_15m¬6</v>
+        <v>ZARFwd_15m¬2</v>
       </c>
       <c r="U13" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3120,7 +4315,7 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B14,valDate,B14,index,E14,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_4y¬6</v>
+        <v>ZAROISSwap_4y¬2</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
@@ -3137,7 +4332,7 @@
       </c>
       <c r="M14" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I14,valDate,I14,$J$2,L14,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_4y¬6</v>
+        <v>USDOISSwap_4y¬2</v>
       </c>
       <c r="O14" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P14,"MF","JHB+NYC")</f>
@@ -3155,7 +4350,7 @@
       </c>
       <c r="S14" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P14,O14,"ZAR","USD",1000000,R14,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_18m¬6</v>
+        <v>ZARFwd_18m¬2</v>
       </c>
       <c r="U14" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3194,7 +4389,7 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B15,valDate,B15,index,E15,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_5y¬6</v>
+        <v>ZAROISSwap_5y¬2</v>
       </c>
       <c r="I15" t="s">
         <v>15</v>
@@ -3211,7 +4406,7 @@
       </c>
       <c r="M15" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I15,valDate,I15,$J$2,L15,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_5y¬6</v>
+        <v>USDOISSwap_5y¬2</v>
       </c>
       <c r="O15" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P15,"MF","JHB+NYC")</f>
@@ -3229,7 +4424,7 @@
       </c>
       <c r="S15" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P15,O15,"ZAR","USD",1000000,R15,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_2y¬6</v>
+        <v>ZARFwd_2y¬2</v>
       </c>
       <c r="U15" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3268,7 +4463,7 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B16,valDate,B16,index,E16,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_7y¬6</v>
+        <v>ZAROISSwap_7y¬2</v>
       </c>
       <c r="I16" t="s">
         <v>16</v>
@@ -3285,7 +4480,7 @@
       </c>
       <c r="M16" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I16,valDate,I16,$J$2,L16,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_7y¬6</v>
+        <v>USDOISSwap_7y¬2</v>
       </c>
       <c r="O16" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P16,"MF","JHB+NYC")</f>
@@ -3303,7 +4498,7 @@
       </c>
       <c r="S16" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P16,O16,"ZAR","USD",1000000,R16,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_3y¬6</v>
+        <v>ZARFwd_3y¬2</v>
       </c>
       <c r="U16" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3342,7 +4537,7 @@
       </c>
       <c r="F17" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B17,valDate,B17,index,E17,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_10y¬6</v>
+        <v>ZAROISSwap_10y¬2</v>
       </c>
       <c r="I17" t="s">
         <v>17</v>
@@ -3359,7 +4554,7 @@
       </c>
       <c r="M17" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I17,valDate,I17,$J$2,L17,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_10y¬6</v>
+        <v>USDOISSwap_10y¬2</v>
       </c>
       <c r="O17" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P17,"MF","JHB+NYC")</f>
@@ -3377,7 +4572,7 @@
       </c>
       <c r="S17" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P17,O17,"ZAR","USD",1000000,R17,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_4y¬6</v>
+        <v>ZARFwd_4y¬2</v>
       </c>
       <c r="U17" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3409,7 +4604,7 @@
       </c>
       <c r="F18" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B18,valDate,B18,oisIndex,index,E18,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_3m¬8</v>
+        <v>ZAROISBasis_3m¬2</v>
       </c>
       <c r="I18" t="s">
         <v>0</v>
@@ -3419,7 +4614,7 @@
       </c>
       <c r="M18" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I18,valDate,I18,$J$3,$J$2,L18,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_3m¬8</v>
+        <v>USDOISBasis_3m¬2</v>
       </c>
       <c r="O18" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P18,"MF","JHB+NYC")</f>
@@ -3437,7 +4632,7 @@
       </c>
       <c r="S18" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P18,O18,"ZAR","USD",1000000,R18,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_5y¬6</v>
+        <v>ZARFwd_5y¬2</v>
       </c>
       <c r="U18" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3469,7 +4664,7 @@
       </c>
       <c r="F19" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B19,valDate,B19,oisIndex,index,E19,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_6m¬8</v>
+        <v>ZAROISBasis_6m¬2</v>
       </c>
       <c r="I19" t="s">
         <v>32</v>
@@ -3479,7 +4674,7 @@
       </c>
       <c r="M19" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I19,valDate,I19,$J$3,$J$2,L19,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_6m¬8</v>
+        <v>USDOISBasis_6m¬2</v>
       </c>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
@@ -3513,7 +4708,7 @@
       </c>
       <c r="F20" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B20,valDate,B20,oisIndex,index,E20,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_9m¬8</v>
+        <v>ZAROISBasis_9m¬2</v>
       </c>
       <c r="I20" t="s">
         <v>33</v>
@@ -3523,7 +4718,7 @@
       </c>
       <c r="M20" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I20,valDate,I20,$J$3,$J$2,L20,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_9m¬8</v>
+        <v>USDOISBasis_9m¬2</v>
       </c>
       <c r="U20" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3555,7 +4750,7 @@
       </c>
       <c r="F21" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B21,valDate,B21,oisIndex,index,E21,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_1y¬8</v>
+        <v>ZAROISBasis_1y¬2</v>
       </c>
       <c r="I21" t="s">
         <v>34</v>
@@ -3565,7 +4760,7 @@
       </c>
       <c r="M21" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I21,valDate,I21,$J$3,$J$2,L21,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_1y¬8</v>
+        <v>USDOISBasis_1y¬2</v>
       </c>
       <c r="U21" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3597,7 +4792,7 @@
       </c>
       <c r="F22" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B22,valDate,B22,oisIndex,index,E22,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_18m¬8</v>
+        <v>ZAROISBasis_18m¬2</v>
       </c>
       <c r="I22" t="s">
         <v>35</v>
@@ -3607,7 +4802,7 @@
       </c>
       <c r="M22" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I22,valDate,I22,$J$3,$J$2,L22,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_18m¬8</v>
+        <v>USDOISBasis_18m¬2</v>
       </c>
       <c r="U22" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3639,7 +4834,7 @@
       </c>
       <c r="F23" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B23,valDate,B23,oisIndex,index,E23,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_2y¬8</v>
+        <v>ZAROISBasis_2y¬2</v>
       </c>
       <c r="I23" t="s">
         <v>12</v>
@@ -3649,7 +4844,7 @@
       </c>
       <c r="M23" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I23,valDate,I23,$J$3,$J$2,L23,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_2y¬8</v>
+        <v>USDOISBasis_2y¬2</v>
       </c>
       <c r="U23" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3681,7 +4876,7 @@
       </c>
       <c r="F24" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B24,valDate,B24,oisIndex,index,E24,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_5y¬8</v>
+        <v>ZAROISBasis_5y¬2</v>
       </c>
       <c r="I24" t="s">
         <v>15</v>
@@ -3691,7 +4886,7 @@
       </c>
       <c r="M24" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I24,valDate,I24,$J$3,$J$2,L24,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_5y¬8</v>
+        <v>USDOISBasis_5y¬2</v>
       </c>
       <c r="U24" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3723,7 +4918,7 @@
       </c>
       <c r="F25" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B25,valDate,B25,oisIndex,index,E25,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_10y¬8</v>
+        <v>ZAROISBasis_10y¬2</v>
       </c>
       <c r="I25" t="s">
         <v>17</v>
@@ -3733,7 +4928,7 @@
       </c>
       <c r="M25" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I25,valDate,I25,$J$3,$J$2,L25,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_10y¬8</v>
+        <v>USDOISBasis_10y¬2</v>
       </c>
       <c r="U25" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3784,7 +4979,7 @@
       </c>
       <c r="C27" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_ZAR",F6:F25)</f>
-        <v>FundingInstruments_ZAR¬8</v>
+        <v>FundingInstruments_ZAR¬2</v>
       </c>
       <c r="G27" t="s">
         <v>53</v>
@@ -3794,7 +4989,7 @@
       </c>
       <c r="J27" t="str">
         <f ca="1">_xll.QIns_CreateFxPair("USDZAR","ZAR","USD","NYC+JHB","2b")</f>
-        <v>USDZAR¬8</v>
+        <v>USDZAR¬2</v>
       </c>
       <c r="L27" t="s">
         <v>63</v>
@@ -3830,7 +5025,7 @@
       </c>
       <c r="C28" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_USD",M6:M25)</f>
-        <v>FundingInstruments_USD¬8</v>
+        <v>FundingInstruments_USD¬2</v>
       </c>
       <c r="G28" t="s">
         <v>54</v>
@@ -3840,7 +5035,7 @@
       </c>
       <c r="J28" t="str">
         <f ca="1">_xll.QIns_CreateFxMatrix("fxMatrix","USD",valDate,L27:M27,J27,L29:M30)</f>
-        <v>fxMatrix¬8</v>
+        <v>fxMatrix¬2</v>
       </c>
       <c r="U28" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3869,7 +5064,7 @@
       </c>
       <c r="C29" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_XCY",S6:S18)</f>
-        <v>FundingInstruments_XCY¬8</v>
+        <v>FundingInstruments_XCY¬2</v>
       </c>
       <c r="G29" t="s">
         <v>55</v>
@@ -3910,7 +5105,7 @@
       </c>
       <c r="C30" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstrumentsComplex",C27:C29)</f>
-        <v>FundingInstrumentsComplex¬8</v>
+        <v>FundingInstrumentsComplex¬2</v>
       </c>
       <c r="G30" t="s">
         <v>56</v>
@@ -3979,7 +5174,7 @@
       </c>
       <c r="C32" t="str">
         <f ca="1">_xll.QCurves_CreateFundingModel("ModelComplex",valDate,C30,G27:H31,J28)</f>
-        <v>ModelComplex¬6</v>
+        <v>ModelComplex¬2</v>
       </c>
       <c r="U32" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4012,7 +5207,7 @@
       </c>
       <c r="D33" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C33,"curve.complex."&amp;C33)</f>
-        <v>curve.complex.ZAR.JIBAR.3M¬6</v>
+        <v>curve.complex.ZAR.JIBAR.3M¬2</v>
       </c>
       <c r="U33" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4045,7 +5240,7 @@
       </c>
       <c r="D34" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C34,"curve.complex."&amp;C34)</f>
-        <v>curve.complex.ZAR.OIS.1B¬6</v>
+        <v>curve.complex.ZAR.OIS.1B¬2</v>
       </c>
       <c r="U34" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4078,7 +5273,7 @@
       </c>
       <c r="D35" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C35,"curve.complex."&amp;C35)</f>
-        <v>curve.complex.USD.LIBOR.3M¬6</v>
+        <v>curve.complex.USD.LIBOR.3M¬2</v>
       </c>
       <c r="U35" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4111,7 +5306,7 @@
       </c>
       <c r="D36" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C36,"curve.complex."&amp;C36)</f>
-        <v>curve.complex.USD.OIS.1B¬6</v>
+        <v>curve.complex.USD.OIS.1B¬2</v>
       </c>
       <c r="U36" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4144,7 +5339,7 @@
       </c>
       <c r="D37" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C37,"curve.complex."&amp;C37)</f>
-        <v>curve.complex.ZAR.DISC.[USD.OIS.1B]¬6</v>
+        <v>curve.complex.ZAR.DISC.[USD.OIS.1B]¬2</v>
       </c>
       <c r="U37" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4165,59 +5360,1218 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8176C107-E78D-42F6-9C95-7C92D15AD2A8}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="str" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">_xll.QIns_CreateInflationIndex(B3,B4,"Linear",B5,B6,"1y","USD","-3m","P")</f>
-        <v>US.CPI¬0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>68</v>
+      <c r="K1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" aca="1" ref="B2" ca="1">_xll.QIns_CreateInflationIndex(B3,B4,"Linear",B6,B7,"1y","USD",B5,"P")</f>
+        <v>USD.CPI¬30</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>71</v>
+        <v>77</v>
+      </c>
+      <c r="J3" s="2">
+        <f ca="1">valDate</f>
+        <v>43930</v>
+      </c>
+      <c r="K3" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J3)</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J3,J4,"Linear","Act365F")</f>
+        <v>1.329593611111116E-2</v>
+      </c>
+      <c r="M3" cm="1">
+        <f t="array" aca="1" ref="M3" ca="1">_xll.QCurves_GetCpiForecast($B$30,J3,3)</f>
+        <v>100.05308829634575</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="J4" s="2">
+        <f ca="1">EDATE(J3,3)</f>
+        <v>44021</v>
+      </c>
+      <c r="K4" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J4)</f>
+        <v>0.99669607488388912</v>
+      </c>
+      <c r="L4" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J4,J5,"Linear","Act365F")</f>
+        <v>1.0853461188319216E-2</v>
+      </c>
+      <c r="M4" cm="1">
+        <f t="array" aca="1" ref="M4" ca="1">_xll.QCurves_GetCpiForecast($B$30,J4,3)</f>
+        <v>101.56136075610513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="str">
+        <f ca="1">"-3m"</f>
+        <v>-3m</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" ref="J5:J35" ca="1" si="0">EDATE(J4,3)</f>
+        <v>44113</v>
+      </c>
+      <c r="K5" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J5)</f>
+        <v>0.99397688519022931</v>
+      </c>
+      <c r="L5" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J5,J6,"Linear","Act365F")</f>
+        <v>8.3989074440587643E-3</v>
+      </c>
+      <c r="M5" cm="1">
+        <f t="array" aca="1" ref="M5" ca="1">_xll.QCurves_GetCpiForecast($B$30,J5,3)</f>
+        <v>103.08432470555356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44205</v>
+      </c>
+      <c r="K6" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J6)</f>
+        <v>0.99187709636447929</v>
+      </c>
+      <c r="L6" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J6,J7,"Linear","Act365F")</f>
+        <v>5.9724257990548448E-3</v>
+      </c>
+      <c r="M6" cm="1">
+        <f t="array" aca="1" ref="M6" ca="1">_xll.QCurves_GetCpiForecast($B$30,J6,3)</f>
+        <v>104.61791490204203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="J7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44295</v>
+      </c>
+      <c r="K7" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J7)</f>
+        <v>0.99041855357294528</v>
+      </c>
+      <c r="L7" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J7,J8,"Linear","Act365F")</f>
+        <v>3.5609225435252819E-3</v>
+      </c>
+      <c r="M7" cm="1">
+        <f t="array" aca="1" ref="M7" ca="1">_xll.QCurves_GetCpiForecast($B$30,J7,3)</f>
+        <v>106.12168591165967</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44386</v>
+      </c>
+      <c r="K8" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J8)</f>
+        <v>0.98954004818296748</v>
+      </c>
+      <c r="L8" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J8,J9,"Linear","Act365F")</f>
+        <v>1.1241970334315312E-3</v>
+      </c>
+      <c r="M8" cm="1">
+        <f t="array" aca="1" ref="M8" ca="1">_xll.QCurves_GetCpiForecast($B$30,J8,3)</f>
+        <v>107.65295686520498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J9" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44478</v>
+      </c>
+      <c r="K9" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J9)</f>
+        <v>0.98925973228493413</v>
+      </c>
+      <c r="L9" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J9,J10,"Linear","Act365F")</f>
+        <v>-1.3243538117687285E-3</v>
+      </c>
+      <c r="M9" cm="1">
+        <f t="array" aca="1" ref="M9" ca="1">_xll.QCurves_GetCpiForecast($B$30,J9,3)</f>
+        <v>109.35558564506148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>73</v>
       </c>
+      <c r="E10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="str" cm="1">
+        <f t="array" aca="1" ref="F10" ca="1">_xll.QCurves_CreateFixingDictionary(E10,"USD.CPI",E12:F14)</f>
+        <v>CPI Fixings¬31</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44570</v>
+      </c>
+      <c r="K10" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J10)</f>
+        <v>0.9895900670759552</v>
+      </c>
+      <c r="L10" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J10,J11,"Linear","Act365F")</f>
+        <v>-3.7448422044676728E-3</v>
+      </c>
+      <c r="M10" cm="1">
+        <f t="array" aca="1" ref="M10" ca="1">_xll.QCurves_GetCpiForecast($B$30,J10,3)</f>
+        <v>111.14293781232169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44660</v>
+      </c>
+      <c r="K11" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J11)</f>
+        <v>0.99050468498643585</v>
+      </c>
+      <c r="L11" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J11,J12,"Linear","Act365F")</f>
+        <v>4.6165208548161734E-3</v>
+      </c>
+      <c r="M11" cm="1">
+        <f t="array" aca="1" ref="M11" ca="1">_xll.QCurves_GetCpiForecast($B$30,J11,3)</f>
+        <v>113.02471112207618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="C12" t="str" cm="1">
+        <f t="array" aca="1" ref="C12" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A12,ComplexBuild!valDate,A12,$B$2,B12,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
+        <v>InfSwap6m¬30</v>
+      </c>
+      <c r="E12" s="17">
+        <v>43891</v>
+      </c>
+      <c r="F12">
+        <v>103</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44751</v>
+      </c>
+      <c r="K12" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J12)</f>
+        <v>0.98936595621968537</v>
+      </c>
+      <c r="L12" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J12,J13,"Linear","Act365F")</f>
+        <v>4.8510727063655334E-3</v>
+      </c>
+      <c r="M12" cm="1">
+        <f t="array" aca="1" ref="M12" ca="1">_xll.QCurves_GetCpiForecast($B$30,J12,3)</f>
+        <v>114.94820586348568</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="10">
+        <f ca="1">B12+0.005</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="C13" t="str" cm="1">
+        <f t="array" aca="1" ref="C13" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A13,ComplexBuild!valDate,A13,$B$2,B13,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
+        <v>InfSwap1y¬30</v>
+      </c>
+      <c r="E13" s="17">
+        <v>43862</v>
+      </c>
+      <c r="F13">
+        <v>102</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44843</v>
+      </c>
+      <c r="K13" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J13)</f>
+        <v>0.98815770009348602</v>
+      </c>
+      <c r="L13" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J13,J14,"Linear","Act365F")</f>
+        <v>4.8702643663097681E-3</v>
+      </c>
+      <c r="M13" cm="1">
+        <f t="array" aca="1" ref="M13" ca="1">_xll.QCurves_GetCpiForecast($B$30,J13,3)</f>
+        <v>117.02564362611034</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10">
+        <f t="shared" ref="B14:B16" ca="1" si="1">B13+0.005</f>
+        <v>0.06</v>
+      </c>
+      <c r="C14" t="str" cm="1">
+        <f t="array" aca="1" ref="C14" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A14,ComplexBuild!valDate,A14,$B$2,B14,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
+        <v>InfSwap2y¬30</v>
+      </c>
+      <c r="E14" s="17">
+        <v>43831</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44935</v>
+      </c>
+      <c r="K14" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J14)</f>
+        <v>0.98694615116806661</v>
+      </c>
+      <c r="L14" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J14,J15,"Linear","Act365F")</f>
+        <v>4.8891820475031661E-3</v>
+      </c>
+      <c r="M14" cm="1">
+        <f t="array" aca="1" ref="M14" ca="1">_xll.QCurves_GetCpiForecast($B$30,J14,3)</f>
+        <v>119.22338337900035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C15" t="str" cm="1">
+        <f t="array" aca="1" ref="C15" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A15,ComplexBuild!valDate,A15,$B$2,B15,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
+        <v>InfSwap3y¬30</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45025</v>
+      </c>
+      <c r="K15" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J15)</f>
+        <v>0.98575776917644486</v>
+      </c>
+      <c r="L15" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J15,J16,"Linear","Act365F")</f>
+        <v>6.3091638772783849E-3</v>
+      </c>
+      <c r="M15" cm="1">
+        <f t="array" aca="1" ref="M15" ca="1">_xll.QCurves_GetCpiForecast($B$30,J15,3)</f>
+        <v>121.51481631861036</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C16" t="str" cm="1">
+        <f t="array" aca="1" ref="C16" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A16,ComplexBuild!valDate,A16,$B$2,B16,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
+        <v>InfSwap5y¬30</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45116</v>
+      </c>
+      <c r="K16" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J16)</f>
+        <v>0.98420963731310829</v>
+      </c>
+      <c r="L16" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J16,J17,"Linear","Act365F")</f>
+        <v>6.5613257933532371E-3</v>
+      </c>
+      <c r="M16" cm="1">
+        <f t="array" aca="1" ref="M16" ca="1">_xll.QCurves_GetCpiForecast($B$30,J16,3)</f>
+        <v>123.79859320175402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C17" t="str" cm="1">
+        <f t="array" aca="1" ref="C17" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A17,ComplexBuild!valDate,A17,$B$2,B17,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
+        <v>InfSwap10y¬30</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45208</v>
+      </c>
+      <c r="K17" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J17)</f>
+        <v>0.98258462547215442</v>
+      </c>
+      <c r="L17" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J17,J18,"Linear","Act365F")</f>
+        <v>6.80037086562539E-3</v>
+      </c>
+      <c r="M17" cm="1">
+        <f t="array" aca="1" ref="M17" ca="1">_xll.QCurves_GetCpiForecast($B$30,J17,3)</f>
+        <v>126.14512285807679</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="21">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="C18" s="19" t="str" cm="1">
+        <f t="array" aca="1" ref="C18" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A18,ComplexBuild!valDate,A18,$B$2,B18,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
+        <v>InfSwap4y¬19</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45300</v>
+      </c>
+      <c r="K18" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J18)</f>
+        <v>0.98090329240969876</v>
+      </c>
+      <c r="L18" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J18,J19,"Linear","Act365F")</f>
+        <v>7.0380632261232545E-3</v>
+      </c>
+      <c r="M18" cm="1">
+        <f t="array" aca="1" ref="M18" ca="1">_xll.QCurves_GetCpiForecast($B$30,J18,3)</f>
+        <v>128.50509420877495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45391</v>
+      </c>
+      <c r="K19" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J19)</f>
+        <v>0.97918512096307153</v>
+      </c>
+      <c r="L19" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J19,J20,"Linear","Act365F")</f>
+        <v>7.8483692645597777E-3</v>
+      </c>
+      <c r="M19" cm="1">
+        <f t="array" aca="1" ref="M19" ca="1">_xll.QCurves_GetCpiForecast($B$30,J19,3)</f>
+        <v>130.89357541207272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="str">
+        <f ca="1">ComplexBuild!C28</f>
+        <v>FundingInstruments_USD¬2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45482</v>
+      </c>
+      <c r="K20" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J20)</f>
+        <v>0.97727287478823477</v>
+      </c>
+      <c r="L20" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J20,J21,"Linear","Act365F")</f>
+        <v>8.1539496965475442E-3</v>
+      </c>
+      <c r="M20" cm="1">
+        <f t="array" aca="1" ref="M20" ca="1">_xll.QCurves_GetCpiForecast($B$30,J20,3)</f>
+        <v>133.27823562988155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" t="str" cm="1">
+        <f t="array" aca="1" ref="B21" ca="1">_xll.QIns_CreateFundingInstrumentCollection(A21,C12:C17)</f>
+        <v>CPI¬30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45574</v>
+      </c>
+      <c r="K21" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J21)</f>
+        <v>0.97526846197147277</v>
+      </c>
+      <c r="L21" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J21,J22,"Linear","Act365F")</f>
+        <v>8.4611388513162224E-3</v>
+      </c>
+      <c r="M21" cm="1">
+        <f t="array" aca="1" ref="M21" ca="1">_xll.QCurves_GetCpiForecast($B$30,J21,3)</f>
+        <v>135.75660866681818</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="str">
+        <f ca="1">_xll.QIns_CreateFundingInstrumentCollection(A22,B20:B21)</f>
+        <v>FicCPI¬30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45666</v>
+      </c>
+      <c r="K22" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J22)</f>
+        <v>0.97319296193923055</v>
+      </c>
+      <c r="L22" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J22,J23,"Linear","Act365F")</f>
+        <v>8.7648020218674943E-3</v>
+      </c>
+      <c r="M22" cm="1">
+        <f t="array" aca="1" ref="M22" ca="1">_xll.QCurves_GetCpiForecast($B$30,J22,3)</f>
+        <v>138.35111982193467</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J23" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45756</v>
+      </c>
+      <c r="K23" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J23)</f>
+        <v>0.97109424852837223</v>
+      </c>
+      <c r="L23" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J23,J24,"Linear","Act365F")</f>
+        <v>8.9084999722346507E-3</v>
+      </c>
+      <c r="M23" cm="1">
+        <f t="array" aca="1" ref="M23" ca="1">_xll.QCurves_GetCpiForecast($B$30,J23,3)</f>
+        <v>141.07769688759015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45847</v>
+      </c>
+      <c r="K24" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J24)</f>
+        <v>0.9689422053326282</v>
+      </c>
+      <c r="L24" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J24,J25,"Linear","Act365F")</f>
+        <v>9.1990422107138606E-3</v>
+      </c>
+      <c r="M24" cm="1">
+        <f t="array" aca="1" ref="M24" ca="1">_xll.QCurves_GetCpiForecast($B$30,J24,3)</f>
+        <v>143.86042465357392</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="P24" t="str" cm="1">
+        <f t="array" aca="1" ref="P24" ca="1">_xll.QIns_AssetPortfolioExpectedFlows("CashflowResult",B34,B33)</f>
+        <v>CashflowResult¬7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="str" cm="1">
+        <f t="array" aca="1" ref="B25" ca="1">_xll.QCurves_CreateFundingModel(A25,valDate,B22,E20:F22,,,F10)</f>
+        <v>ModelCPI¬31</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>45939</v>
+      </c>
+      <c r="K25" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J25)</f>
+        <v>0.96670075236166508</v>
+      </c>
+      <c r="L25" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J25,J26,"Linear","Act365F")</f>
+        <v>9.4910842711828682E-3</v>
+      </c>
+      <c r="M25" cm="1">
+        <f t="array" aca="1" ref="M25" ca="1">_xll.QCurves_GetCpiForecast($B$30,J25,3)</f>
+        <v>146.82167910410232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J26" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46031</v>
+      </c>
+      <c r="K26" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J26)</f>
+        <v>0.96439365916425557</v>
+      </c>
+      <c r="L26" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J26,J27,"Linear","Act365F")</f>
+        <v>9.7797112314272662E-3</v>
+      </c>
+      <c r="M26" cm="1">
+        <f t="array" aca="1" ref="M26" ca="1">_xll.QCurves_GetCpiForecast($B$30,J26,3)</f>
+        <v>149.88392218361739</v>
+      </c>
+      <c r="O26" s="14" t="str">
+        <f t="array" aca="1" ref="O26:S40" ca="1">_xll.QCube_DisplayCube(P24)</f>
+        <v>TradeId</v>
+      </c>
+      <c r="P26" s="14" t="str">
+        <f ca="1"/>
+        <v>Currency</v>
+      </c>
+      <c r="Q26" s="14" t="str">
+        <f ca="1"/>
+        <v>TradeType</v>
+      </c>
+      <c r="R26" s="14" t="str">
+        <f ca="1"/>
+        <v>PayDate</v>
+      </c>
+      <c r="S26" s="14" t="str">
+        <f ca="1"/>
+        <v>Value</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46121</v>
+      </c>
+      <c r="K27" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J27)</f>
+        <v>0.96207368039716601</v>
+      </c>
+      <c r="L27" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J27,J28,"Linear","Act365F")</f>
+        <v>1.0067156644269194E-2</v>
+      </c>
+      <c r="M27" cm="1">
+        <f t="array" aca="1" ref="M27" ca="1">_xll.QCurves_GetCpiForecast($B$30,J27,3)</f>
+        <v>153.02823461613627</v>
+      </c>
+      <c r="O27" t="str">
+        <f ca="1"/>
+        <v>InfSwap6m</v>
+      </c>
+      <c r="P27" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q27" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R27" s="2">
+        <f ca="1"/>
+        <v>44113</v>
+      </c>
+      <c r="S27" s="4">
+        <f ca="1"/>
+        <v>24695.07659595993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="array" aca="1" ref="A28:A30" ca="1">_xll.QCurves_ListCurvesInModel(B25)</f>
+        <v>USD.LIBOR.3M</v>
+      </c>
+      <c r="B28" t="str">
+        <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A28,"curve.cpiBuild."&amp;A28)</f>
+        <v>curve.cpiBuild.USD.LIBOR.3M¬30</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46212</v>
+      </c>
+      <c r="K28" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J28)</f>
+        <v>0.95966502305936319</v>
+      </c>
+      <c r="L28" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J28,J29,"Linear","Act365F")</f>
+        <v>1.0357813597547285E-2</v>
+      </c>
+      <c r="M28" cm="1">
+        <f t="array" aca="1" ref="M28" ca="1">_xll.QCurves_GetCpiForecast($B$30,J28,3)</f>
+        <v>156.13676504321063</v>
+      </c>
+      <c r="O28" t="str">
+        <f ca="1"/>
+        <v>InfSwap6m</v>
+      </c>
+      <c r="P28" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q28" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R28" s="2">
+        <f ca="1"/>
+        <v>44113</v>
+      </c>
+      <c r="S28" s="4">
+        <f ca="1"/>
+        <v>-24695.07659595993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f ca="1"/>
+        <v>USD.OIS.1B</v>
+      </c>
+      <c r="B29" t="str">
+        <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A29,"curve.cpiBuild."&amp;A29)</f>
+        <v>curve.cpiBuild.USD.OIS.1B¬30</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46304</v>
+      </c>
+      <c r="K29" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J29)</f>
+        <v>0.95716611447307476</v>
+      </c>
+      <c r="L29" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J29,J30,"Linear","Act365F")</f>
+        <v>1.0649940758556239E-2</v>
+      </c>
+      <c r="M29" cm="1">
+        <f t="array" aca="1" ref="M29" ca="1">_xll.QCurves_GetCpiForecast($B$30,J29,3)</f>
+        <v>159.36834522746165</v>
+      </c>
+      <c r="O29" t="str">
+        <f ca="1"/>
+        <v>InfSwap1y</v>
+      </c>
+      <c r="P29" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q29" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R29" s="2">
+        <f ca="1"/>
+        <v>44295</v>
+      </c>
+      <c r="S29" s="4">
+        <f ca="1"/>
+        <v>54887.533913118066</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f ca="1"/>
+        <v>USD.CPI</v>
+      </c>
+      <c r="B30" t="str">
+        <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A30,"curve.cpiBuild."&amp;A30)</f>
+        <v>curve.cpiBuild.USD.CPI¬31</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46396</v>
+      </c>
+      <c r="K30" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J30)</f>
+        <v>0.95460360649813214</v>
+      </c>
+      <c r="L30" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J30,J31,"Linear","Act365F")</f>
+        <v>1.0938586201982145E-2</v>
+      </c>
+      <c r="M30" cm="1">
+        <f t="array" aca="1" ref="M30" ca="1">_xll.QCurves_GetCpiForecast($B$30,J30,3)</f>
+        <v>162.6775589612019</v>
+      </c>
+      <c r="O30" t="str">
+        <f ca="1"/>
+        <v>InfSwap1y</v>
+      </c>
+      <c r="P30" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q30" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R30" s="2">
+        <f ca="1"/>
+        <v>44295</v>
+      </c>
+      <c r="S30" s="4">
+        <f ca="1"/>
+        <v>-54887.533913118066</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J31" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46486</v>
+      </c>
+      <c r="K31" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J31)</f>
+        <v>0.95203578923972831</v>
+      </c>
+      <c r="L31" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J31,J32,"Linear","Act365F")</f>
+        <v>1.174513824912918E-2</v>
+      </c>
+      <c r="M31" cm="1">
+        <f t="array" aca="1" ref="M31" ca="1">_xll.QCurves_GetCpiForecast($B$30,J31,3)</f>
+        <v>166.04418259794028</v>
+      </c>
+      <c r="O31" t="str">
+        <f ca="1"/>
+        <v>InfSwap2y</v>
+      </c>
+      <c r="P31" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q31" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R31" s="2">
+        <f ca="1"/>
+        <v>44659</v>
+      </c>
+      <c r="S31" s="4">
+        <f ca="1"/>
+        <v>123290.30664938733</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46577</v>
+      </c>
+      <c r="K32" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J32)</f>
+        <v>0.94925613949209153</v>
+      </c>
+      <c r="L32" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J32,J33,"Linear","Act365F")</f>
+        <v>1.2071854462021157E-2</v>
+      </c>
+      <c r="M32" cm="1">
+        <f t="array" aca="1" ref="M32" ca="1">_xll.QCurves_GetCpiForecast($B$30,J32,3)</f>
+        <v>169.34377748516795</v>
+      </c>
+      <c r="O32" t="str">
+        <f ca="1"/>
+        <v>InfSwap2y</v>
+      </c>
+      <c r="P32" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q32" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R32" s="2">
+        <f ca="1"/>
+        <v>44659</v>
+      </c>
+      <c r="S32" s="4">
+        <f ca="1"/>
+        <v>-123290.30664938757</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f ca="1">A32</f>
+        <v>AssetFxModel</v>
+      </c>
+      <c r="B33" t="str" cm="1">
+        <f t="array" aca="1" ref="B33" ca="1">_xll.QCurves_CreateAssetFxModel(A33,valDate,,,B25)</f>
+        <v>AssetFxModel¬21</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46669</v>
+      </c>
+      <c r="K33" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J33)</f>
+        <v>0.94637653450372528</v>
+      </c>
+      <c r="L33" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J33,J34,"Linear","Act365F")</f>
+        <v>1.2400193204532005E-2</v>
+      </c>
+      <c r="M33" cm="1">
+        <f t="array" aca="1" ref="M33" ca="1">_xll.QCurves_GetCpiForecast($B$30,J33,3)</f>
+        <v>172.74570841995714</v>
+      </c>
+      <c r="O33" t="str">
+        <f ca="1"/>
+        <v>InfSwap3y</v>
+      </c>
+      <c r="P33" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q33" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R33" s="2">
+        <f ca="1"/>
+        <v>45023</v>
+      </c>
+      <c r="S33" s="4">
+        <f ca="1"/>
+        <v>207381.46579058992</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="str" cm="1">
+        <f t="array" aca="1" ref="B34" ca="1">_xll.QIns_CreatePortfolio(A34,C12:C18)</f>
+        <v>Porfolio¬22</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46761</v>
+      </c>
+      <c r="K34" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J34)</f>
+        <v>0.94342782428126781</v>
+      </c>
+      <c r="L34" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J34,J35,"Linear","Act365F")</f>
+        <v>1.2726552729230234E-2</v>
+      </c>
+      <c r="M34" cm="1">
+        <f t="array" aca="1" ref="M34" ca="1">_xll.QCurves_GetCpiForecast($B$30,J34,3)</f>
+        <v>176.20137882673822</v>
+      </c>
+      <c r="O34" t="str">
+        <f ca="1"/>
+        <v>InfSwap3y</v>
+      </c>
+      <c r="P34" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q34" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R34" s="2">
+        <f ca="1"/>
+        <v>45023</v>
+      </c>
+      <c r="S34" s="4">
+        <f ca="1"/>
+        <v>-207381.46579058969</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J35" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>46852</v>
+      </c>
+      <c r="K35" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J35)</f>
+        <v>0.94044386983374129</v>
+      </c>
+      <c r="L35" s="1"/>
+      <c r="M35" cm="1">
+        <f t="array" aca="1" ref="M35" ca="1">_xll.QCurves_GetCpiForecast($B$30,J35,3)</f>
+        <v>179.68947192352954</v>
+      </c>
+      <c r="O35" t="str">
+        <f ca="1"/>
+        <v>InfSwap5y</v>
+      </c>
+      <c r="P35" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q35" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R35" s="2">
+        <f ca="1"/>
+        <v>45756</v>
+      </c>
+      <c r="S35" s="4">
+        <f ca="1"/>
+        <v>402362.79212316248</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O36" t="str">
+        <f ca="1"/>
+        <v>InfSwap5y</v>
+      </c>
+      <c r="P36" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q36" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R36" s="2">
+        <f ca="1"/>
+        <v>45756</v>
+      </c>
+      <c r="S36" s="4">
+        <f ca="1"/>
+        <v>-402362.79212316248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O37" t="str">
+        <f ca="1"/>
+        <v>InfSwap10y</v>
+      </c>
+      <c r="P37" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q37" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R37" s="2">
+        <f ca="1"/>
+        <v>47582</v>
+      </c>
+      <c r="S37" s="4">
+        <f ca="1"/>
+        <v>1060734.7898047399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O38" t="str">
+        <f ca="1"/>
+        <v>InfSwap10y</v>
+      </c>
+      <c r="P38" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q38" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R38" s="2">
+        <f ca="1"/>
+        <v>47582</v>
+      </c>
+      <c r="S38" s="4">
+        <f ca="1"/>
+        <v>-1060734.7898047403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O39" s="6" t="str">
+        <f ca="1"/>
+        <v>InfSwap4y</v>
+      </c>
+      <c r="P39" s="6" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q39" s="6" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R39" s="7">
+        <f ca="1"/>
+        <v>45391</v>
+      </c>
+      <c r="S39" s="22">
+        <f ca="1"/>
+        <v>301128.98023929156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O40" s="6" t="str">
+        <f ca="1"/>
+        <v>InfSwap4y</v>
+      </c>
+      <c r="P40" s="6" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="Q40" s="6" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="R40" s="7">
+        <f ca="1"/>
+        <v>45391</v>
+      </c>
+      <c r="S40" s="22">
+        <f ca="1"/>
+        <v>-298588.44691406208</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More working inflation functionality
</commit_message>
<xml_diff>
--- a/examples/Qwack - YeildCurveExample (Frozen Data).xlsx
+++ b/examples/Qwack - YeildCurveExample (Frozen Data).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Qwack\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6777C76-B8D1-4DF3-9F65-23C8750A746E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E644BA9-7B05-452A-BF58-122B77304237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="101">
   <si>
     <t>3m</t>
   </si>
@@ -344,15 +344,45 @@
   </si>
   <si>
     <t>Cashflows</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Fixed Rate</t>
+  </si>
+  <si>
+    <t>TradeObj</t>
+  </si>
+  <si>
+    <t>BenchmarkRisk</t>
+  </si>
+  <si>
+    <t>Fx Matrix</t>
+  </si>
+  <si>
+    <t>ValDate</t>
+  </si>
+  <si>
+    <t>Size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -406,12 +436,49 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -420,7 +487,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -451,17 +518,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -672,103 +745,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>100.05308829634575</c:v>
+                  <c:v>100.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101.56136075610513</c:v>
+                  <c:v>101.84216235277678</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103.08432470555356</c:v>
+                  <c:v>103.08432470555357</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>104.61791490204203</c:v>
+                  <c:v>104.60300530860663</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>106.12168591165967</c:v>
+                  <c:v>106.12168591165968</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>107.65295686520498</c:v>
+                  <c:v>107.81948182466114</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>109.35558564506148</c:v>
+                  <c:v>109.54101684366961</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>111.14293781232169</c:v>
+                  <c:v>111.28146982991993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>113.02471112207618</c:v>
+                  <c:v>113.02192281617025</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>114.94820586348568</c:v>
+                  <c:v>115.19136548128431</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>117.02564362611034</c:v>
+                  <c:v>117.39564062318617</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>119.22338337900035</c:v>
+                  <c:v>119.6241385688452</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>121.51481631861036</c:v>
+                  <c:v>121.85263651450421</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>123.79859320175402</c:v>
+                  <c:v>124.21778335068639</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>126.14512285807679</c:v>
+                  <c:v>126.61131241754792</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>128.50509420877495</c:v>
+                  <c:v>129.03114400162772</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>130.89357541207272</c:v>
+                  <c:v>131.45097558570751</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>133.27823562988155</c:v>
+                  <c:v>133.84450465256904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>135.75660866681818</c:v>
+                  <c:v>136.23803371943058</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>138.35111982193467</c:v>
+                  <c:v>138.65786530351036</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>141.07769688759015</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>143.86042465357392</c:v>
+                  <c:v>144.3421547556126</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>146.82167910410232</c:v>
+                  <c:v>147.64288437772422</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>149.88392218361739</c:v>
+                  <c:v>150.97988575392495</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>153.02823461613627</c:v>
+                  <c:v>154.31688713012568</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>156.13676504321063</c:v>
+                  <c:v>157.58134499814813</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>159.36834522746165</c:v>
+                  <c:v>160.88207462025971</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>162.6775589612019</c:v>
+                  <c:v>164.21907599646045</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>166.04418259794028</c:v>
+                  <c:v>167.55607737266118</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>169.34377748516795</c:v>
+                  <c:v>170.82053524068365</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>172.74570841995714</c:v>
+                  <c:v>174.12126486279524</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>176.20137882673822</c:v>
+                  <c:v>177.45826623899598</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>179.68947192352954</c:v>
+                  <c:v>180.79526761519671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1530,16 +1603,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3580,7 +3653,7 @@
   <dimension ref="B1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3609,14 +3682,14 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("ZAR.JIBAR.3M","ZAR","3M","Act365F","Act365F","3M","JHB","0b","MF")</f>
-        <v>ZAR.JIBAR.3M¬2</v>
+        <v>ZAR.JIBAR.3M¬0</v>
       </c>
       <c r="I2" t="s">
         <v>25</v>
       </c>
       <c r="J2" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("USD.LIBOR.3M","USD","3M","Act360","Act360","6M","NYC","2b","MF")</f>
-        <v>USD.LIBOR.3M¬2</v>
+        <v>USD.LIBOR.3M¬0</v>
       </c>
       <c r="V2" s="3"/>
     </row>
@@ -3626,14 +3699,14 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("ZAR.OIS.1B","ZAR","3M","Act365F","Act365F","3M","JHB","0b","MF")</f>
-        <v>ZAR.OIS.1B¬2</v>
+        <v>ZAR.OIS.1B¬0</v>
       </c>
       <c r="I3" t="s">
         <v>31</v>
       </c>
       <c r="J3" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("USD.OIS.1B","USD","3M","Act360","Act360","3M","NYC","0b","MF")</f>
-        <v>USD.OIS.1B¬2</v>
+        <v>USD.OIS.1B¬0</v>
       </c>
       <c r="V3" t="s">
         <v>36</v>
@@ -3718,7 +3791,7 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B6,valDate,"0x3",index,"ZAR",E6,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_3m¬2</v>
+        <v>ZAROISFra_3m¬0</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -3735,7 +3808,7 @@
       </c>
       <c r="M6" t="str">
         <f ca="1">_xll.QIns_CreateFRA("USDOISFra_"&amp;I6,valDate,"0x3",J2,"USD",L6,1,"USD.LIBOR.3M","USD.OIS.1B",,,"USD.LIBOR.3M")</f>
-        <v>USDOISFra_3m¬2</v>
+        <v>USDOISFra_3m¬0</v>
       </c>
       <c r="O6" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P6,"F","JHB+NYC")</f>
@@ -3753,7 +3826,7 @@
       </c>
       <c r="S6" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P6,O6,"ZAR","USD",1000000,R6,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_1w¬2</v>
+        <v>ZARFwd_1w¬0</v>
       </c>
       <c r="U6" s="2">
         <f t="shared" ref="U6:U37" ca="1" si="0">EDATE(U5,3)</f>
@@ -3792,7 +3865,7 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B7,valDate,B7,index,"ZAR",E7,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_3x6¬2</v>
+        <v>ZAROISFra_3x6¬0</v>
       </c>
       <c r="I7" t="s">
         <v>39</v>
@@ -3810,7 +3883,7 @@
       </c>
       <c r="M7" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I7,valDate,I7,$J$2,L7,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDU8¬2</v>
+        <v>EDU8¬0</v>
       </c>
       <c r="O7" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P7,"MF","JHB+NYC")</f>
@@ -3828,7 +3901,7 @@
       </c>
       <c r="S7" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P7,O7,"ZAR","USD",1000000,R7,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_1m¬2</v>
+        <v>ZARFwd_1m¬0</v>
       </c>
       <c r="U7" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3867,25 +3940,25 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B8,valDate,B8,index,"ZAR",E8,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_6x9¬2</v>
+        <v>ZAROISFra_6x9¬0</v>
       </c>
       <c r="I8" t="s">
         <v>40</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" ref="J8:J11" ca="1" si="3">I8&amp;" Comdty"</f>
+        <f ca="1">I8&amp;" Comdty"</f>
         <v>EDZ8 Comdty</v>
       </c>
       <c r="K8" s="6">
         <v>98.614999999999995</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" ref="L8:L11" ca="1" si="4">K8</f>
+        <f ca="1">K8</f>
         <v>98.614999999999995</v>
       </c>
       <c r="M8" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I8,valDate,I8,$J$2,L8,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDZ8¬2</v>
+        <v>EDZ8¬0</v>
       </c>
       <c r="O8" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P8,"MF","JHB+NYC")</f>
@@ -3903,7 +3976,7 @@
       </c>
       <c r="S8" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P8,O8,"ZAR","USD",1000000,R8,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_2m¬2</v>
+        <v>ZARFwd_2m¬0</v>
       </c>
       <c r="U8" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3942,25 +4015,25 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B9,valDate,B9,index,"ZAR",E9,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_9x12¬2</v>
+        <v>ZAROISFra_9x12¬0</v>
       </c>
       <c r="I9" t="s">
         <v>42</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">I9&amp;" Comdty"</f>
         <v>EDH9 Comdty</v>
       </c>
       <c r="K9" s="6">
         <v>98.614999999999995</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">K9</f>
         <v>98.614999999999995</v>
       </c>
       <c r="M9" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I9,valDate,I9,$J$2,L9,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDH9¬2</v>
+        <v>EDH9¬0</v>
       </c>
       <c r="O9" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P9,"MF","JHB+NYC")</f>
@@ -3978,7 +4051,7 @@
       </c>
       <c r="S9" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P9,O9,"ZAR","USD",1000000,R9,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_3m¬2</v>
+        <v>ZARFwd_3m¬0</v>
       </c>
       <c r="U9" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4017,25 +4090,25 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B10,valDate,B10,index,"ZAR",E10,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_12x15¬2</v>
+        <v>ZAROISFra_12x15¬0</v>
       </c>
       <c r="I10" t="s">
         <v>41</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">I10&amp;" Comdty"</f>
         <v>EDM9 Comdty</v>
       </c>
       <c r="K10" s="6">
         <v>98.605000000000004</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">K10</f>
         <v>98.605000000000004</v>
       </c>
       <c r="M10" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I10,valDate,I10,$J$2,L10,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDM9¬2</v>
+        <v>EDM9¬0</v>
       </c>
       <c r="O10" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P10,"MF","JHB+NYC")</f>
@@ -4053,7 +4126,7 @@
       </c>
       <c r="S10" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P10,O10,"ZAR","USD",1000000,R10,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_6m¬2</v>
+        <v>ZARFwd_6m¬0</v>
       </c>
       <c r="U10" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4092,25 +4165,25 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B11,valDate,B11,index,"ZAR",E11,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_15x18¬2</v>
+        <v>ZAROISFra_15x18¬0</v>
       </c>
       <c r="I11" t="s">
         <v>43</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f ca="1">I11&amp;" Comdty"</f>
         <v>EDU9 Comdty</v>
       </c>
       <c r="K11" s="6">
         <v>98.594999999999999</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">K11</f>
         <v>98.594999999999999</v>
       </c>
       <c r="M11" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I11,valDate,I11,$J$2,L11,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDU9¬2</v>
+        <v>EDU9¬0</v>
       </c>
       <c r="O11" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P11,"MF","JHB+NYC")</f>
@@ -4128,7 +4201,7 @@
       </c>
       <c r="S11" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P11,O11,"ZAR","USD",1000000,R11,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_9m¬2</v>
+        <v>ZARFwd_9m¬0</v>
       </c>
       <c r="U11" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4167,7 +4240,7 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B12,valDate,B12,index,E12,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_2y¬2</v>
+        <v>ZAROISSwap_2y¬0</v>
       </c>
       <c r="I12" t="s">
         <v>12</v>
@@ -4179,12 +4252,12 @@
         <v>0.4677</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" ref="L12:L17" ca="1" si="5">K12/100</f>
+        <f t="shared" ref="L12:L17" ca="1" si="3">K12/100</f>
         <v>4.6769999999999997E-3</v>
       </c>
       <c r="M12" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I12,valDate,I12,$J$2,L12,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_2y¬2</v>
+        <v>USDOISSwap_2y¬0</v>
       </c>
       <c r="O12" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P12,"MF","JHB+NYC")</f>
@@ -4202,7 +4275,7 @@
       </c>
       <c r="S12" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P12,O12,"ZAR","USD",1000000,R12,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_12m¬2</v>
+        <v>ZARFwd_12m¬0</v>
       </c>
       <c r="U12" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4241,7 +4314,7 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B13,valDate,B13,index,E13,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_3y¬2</v>
+        <v>ZAROISSwap_3y¬0</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -4253,12 +4326,12 @@
         <v>0.47160000000000002</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>4.7160000000000006E-3</v>
       </c>
       <c r="M13" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I13,valDate,I13,$J$2,L13,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_3y¬2</v>
+        <v>USDOISSwap_3y¬0</v>
       </c>
       <c r="O13" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P13,"MF","JHB+NYC")</f>
@@ -4276,7 +4349,7 @@
       </c>
       <c r="S13" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P13,O13,"ZAR","USD",1000000,R13,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_15m¬2</v>
+        <v>ZARFwd_15m¬0</v>
       </c>
       <c r="U13" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4315,7 +4388,7 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B14,valDate,B14,index,E14,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_4y¬2</v>
+        <v>ZAROISSwap_4y¬0</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
@@ -4327,12 +4400,12 @@
         <v>0.51839999999999997</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.1839999999999994E-3</v>
       </c>
       <c r="M14" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I14,valDate,I14,$J$2,L14,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_4y¬2</v>
+        <v>USDOISSwap_4y¬0</v>
       </c>
       <c r="O14" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P14,"MF","JHB+NYC")</f>
@@ -4350,7 +4423,7 @@
       </c>
       <c r="S14" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P14,O14,"ZAR","USD",1000000,R14,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_18m¬2</v>
+        <v>ZARFwd_18m¬0</v>
       </c>
       <c r="U14" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4389,7 +4462,7 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B15,valDate,B15,index,E15,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_5y¬2</v>
+        <v>ZAROISSwap_5y¬0</v>
       </c>
       <c r="I15" t="s">
         <v>15</v>
@@ -4401,12 +4474,12 @@
         <v>0.57820000000000005</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>5.7820000000000007E-3</v>
       </c>
       <c r="M15" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I15,valDate,I15,$J$2,L15,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_5y¬2</v>
+        <v>USDOISSwap_5y¬0</v>
       </c>
       <c r="O15" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P15,"MF","JHB+NYC")</f>
@@ -4424,7 +4497,7 @@
       </c>
       <c r="S15" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P15,O15,"ZAR","USD",1000000,R15,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_2y¬2</v>
+        <v>ZARFwd_2y¬0</v>
       </c>
       <c r="U15" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4463,7 +4536,7 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B16,valDate,B16,index,E16,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_7y¬2</v>
+        <v>ZAROISSwap_7y¬0</v>
       </c>
       <c r="I16" t="s">
         <v>16</v>
@@ -4475,12 +4548,12 @@
         <v>0.69269999999999998</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>6.927E-3</v>
       </c>
       <c r="M16" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I16,valDate,I16,$J$2,L16,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_7y¬2</v>
+        <v>USDOISSwap_7y¬0</v>
       </c>
       <c r="O16" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P16,"MF","JHB+NYC")</f>
@@ -4498,7 +4571,7 @@
       </c>
       <c r="S16" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P16,O16,"ZAR","USD",1000000,R16,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_3y¬2</v>
+        <v>ZARFwd_3y¬0</v>
       </c>
       <c r="U16" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4537,7 +4610,7 @@
       </c>
       <c r="F17" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B17,valDate,B17,index,E17,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_10y¬2</v>
+        <v>ZAROISSwap_10y¬0</v>
       </c>
       <c r="I17" t="s">
         <v>17</v>
@@ -4549,12 +4622,12 @@
         <v>0.8155</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>8.1550000000000008E-3</v>
       </c>
       <c r="M17" t="str">
         <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I17,valDate,I17,$J$2,L17,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_10y¬2</v>
+        <v>USDOISSwap_10y¬0</v>
       </c>
       <c r="O17" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P17,"MF","JHB+NYC")</f>
@@ -4572,7 +4645,7 @@
       </c>
       <c r="S17" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P17,O17,"ZAR","USD",1000000,R17,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_4y¬2</v>
+        <v>ZARFwd_4y¬0</v>
       </c>
       <c r="U17" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4604,7 +4677,7 @@
       </c>
       <c r="F18" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B18,valDate,B18,oisIndex,index,E18,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_3m¬2</v>
+        <v>ZAROISBasis_3m¬0</v>
       </c>
       <c r="I18" t="s">
         <v>0</v>
@@ -4614,7 +4687,7 @@
       </c>
       <c r="M18" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I18,valDate,I18,$J$3,$J$2,L18,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_3m¬2</v>
+        <v>USDOISBasis_3m¬0</v>
       </c>
       <c r="O18" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P18,"MF","JHB+NYC")</f>
@@ -4632,7 +4705,7 @@
       </c>
       <c r="S18" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P18,O18,"ZAR","USD",1000000,R18,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_5y¬2</v>
+        <v>ZARFwd_5y¬0</v>
       </c>
       <c r="U18" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4664,7 +4737,7 @@
       </c>
       <c r="F19" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B19,valDate,B19,oisIndex,index,E19,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_6m¬2</v>
+        <v>ZAROISBasis_6m¬0</v>
       </c>
       <c r="I19" t="s">
         <v>32</v>
@@ -4674,7 +4747,7 @@
       </c>
       <c r="M19" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I19,valDate,I19,$J$3,$J$2,L19,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_6m¬2</v>
+        <v>USDOISBasis_6m¬0</v>
       </c>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
@@ -4708,7 +4781,7 @@
       </c>
       <c r="F20" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B20,valDate,B20,oisIndex,index,E20,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_9m¬2</v>
+        <v>ZAROISBasis_9m¬0</v>
       </c>
       <c r="I20" t="s">
         <v>33</v>
@@ -4718,7 +4791,7 @@
       </c>
       <c r="M20" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I20,valDate,I20,$J$3,$J$2,L20,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_9m¬2</v>
+        <v>USDOISBasis_9m¬0</v>
       </c>
       <c r="U20" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4750,7 +4823,7 @@
       </c>
       <c r="F21" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B21,valDate,B21,oisIndex,index,E21,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_1y¬2</v>
+        <v>ZAROISBasis_1y¬0</v>
       </c>
       <c r="I21" t="s">
         <v>34</v>
@@ -4760,7 +4833,7 @@
       </c>
       <c r="M21" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I21,valDate,I21,$J$3,$J$2,L21,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_1y¬2</v>
+        <v>USDOISBasis_1y¬0</v>
       </c>
       <c r="U21" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4792,7 +4865,7 @@
       </c>
       <c r="F22" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B22,valDate,B22,oisIndex,index,E22,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_18m¬2</v>
+        <v>ZAROISBasis_18m¬0</v>
       </c>
       <c r="I22" t="s">
         <v>35</v>
@@ -4802,7 +4875,7 @@
       </c>
       <c r="M22" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I22,valDate,I22,$J$3,$J$2,L22,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_18m¬2</v>
+        <v>USDOISBasis_18m¬0</v>
       </c>
       <c r="U22" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4834,7 +4907,7 @@
       </c>
       <c r="F23" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B23,valDate,B23,oisIndex,index,E23,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_2y¬2</v>
+        <v>ZAROISBasis_2y¬0</v>
       </c>
       <c r="I23" t="s">
         <v>12</v>
@@ -4844,7 +4917,7 @@
       </c>
       <c r="M23" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I23,valDate,I23,$J$3,$J$2,L23,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_2y¬2</v>
+        <v>USDOISBasis_2y¬0</v>
       </c>
       <c r="U23" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4876,7 +4949,7 @@
       </c>
       <c r="F24" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B24,valDate,B24,oisIndex,index,E24,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_5y¬2</v>
+        <v>ZAROISBasis_5y¬0</v>
       </c>
       <c r="I24" t="s">
         <v>15</v>
@@ -4886,7 +4959,7 @@
       </c>
       <c r="M24" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I24,valDate,I24,$J$3,$J$2,L24,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_5y¬2</v>
+        <v>USDOISBasis_5y¬0</v>
       </c>
       <c r="U24" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4918,7 +4991,7 @@
       </c>
       <c r="F25" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B25,valDate,B25,oisIndex,index,E25,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_10y¬2</v>
+        <v>ZAROISBasis_10y¬0</v>
       </c>
       <c r="I25" t="s">
         <v>17</v>
@@ -4928,7 +5001,7 @@
       </c>
       <c r="M25" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I25,valDate,I25,$J$3,$J$2,L25,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_10y¬2</v>
+        <v>USDOISBasis_10y¬0</v>
       </c>
       <c r="U25" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4979,7 +5052,7 @@
       </c>
       <c r="C27" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_ZAR",F6:F25)</f>
-        <v>FundingInstruments_ZAR¬2</v>
+        <v>FundingInstruments_ZAR¬0</v>
       </c>
       <c r="G27" t="s">
         <v>53</v>
@@ -4989,7 +5062,7 @@
       </c>
       <c r="J27" t="str">
         <f ca="1">_xll.QIns_CreateFxPair("USDZAR","ZAR","USD","NYC+JHB","2b")</f>
-        <v>USDZAR¬2</v>
+        <v>USDZAR¬0</v>
       </c>
       <c r="L27" t="s">
         <v>63</v>
@@ -5025,7 +5098,7 @@
       </c>
       <c r="C28" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_USD",M6:M25)</f>
-        <v>FundingInstruments_USD¬2</v>
+        <v>FundingInstruments_USD¬0</v>
       </c>
       <c r="G28" t="s">
         <v>54</v>
@@ -5035,7 +5108,7 @@
       </c>
       <c r="J28" t="str">
         <f ca="1">_xll.QIns_CreateFxMatrix("fxMatrix","USD",valDate,L27:M27,J27,L29:M30)</f>
-        <v>fxMatrix¬2</v>
+        <v>fxMatrix¬0</v>
       </c>
       <c r="U28" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5064,7 +5137,7 @@
       </c>
       <c r="C29" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_XCY",S6:S18)</f>
-        <v>FundingInstruments_XCY¬2</v>
+        <v>FundingInstruments_XCY¬0</v>
       </c>
       <c r="G29" t="s">
         <v>55</v>
@@ -5105,7 +5178,7 @@
       </c>
       <c r="C30" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstrumentsComplex",C27:C29)</f>
-        <v>FundingInstrumentsComplex¬2</v>
+        <v>FundingInstrumentsComplex¬0</v>
       </c>
       <c r="G30" t="s">
         <v>56</v>
@@ -5174,7 +5247,7 @@
       </c>
       <c r="C32" t="str">
         <f ca="1">_xll.QCurves_CreateFundingModel("ModelComplex",valDate,C30,G27:H31,J28)</f>
-        <v>ModelComplex¬2</v>
+        <v>ModelComplex¬0</v>
       </c>
       <c r="U32" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5207,7 +5280,7 @@
       </c>
       <c r="D33" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C33,"curve.complex."&amp;C33)</f>
-        <v>curve.complex.ZAR.JIBAR.3M¬2</v>
+        <v>curve.complex.ZAR.JIBAR.3M¬0</v>
       </c>
       <c r="U33" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5240,7 +5313,7 @@
       </c>
       <c r="D34" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C34,"curve.complex."&amp;C34)</f>
-        <v>curve.complex.ZAR.OIS.1B¬2</v>
+        <v>curve.complex.ZAR.OIS.1B¬0</v>
       </c>
       <c r="U34" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5273,7 +5346,7 @@
       </c>
       <c r="D35" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C35,"curve.complex."&amp;C35)</f>
-        <v>curve.complex.USD.LIBOR.3M¬2</v>
+        <v>curve.complex.USD.LIBOR.3M¬0</v>
       </c>
       <c r="U35" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5306,7 +5379,7 @@
       </c>
       <c r="D36" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C36,"curve.complex."&amp;C36)</f>
-        <v>curve.complex.USD.OIS.1B¬2</v>
+        <v>curve.complex.USD.OIS.1B¬0</v>
       </c>
       <c r="U36" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5339,7 +5412,7 @@
       </c>
       <c r="D37" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C37,"curve.complex."&amp;C37)</f>
-        <v>curve.complex.ZAR.DISC.[USD.OIS.1B]¬2</v>
+        <v>curve.complex.ZAR.DISC.[USD.OIS.1B]¬0</v>
       </c>
       <c r="U37" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5360,42 +5433,69 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8176C107-E78D-42F6-9C95-7C92D15AD2A8}">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.42578125" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="2">
+        <f ca="1">valDate</f>
+        <v>43930</v>
+      </c>
+      <c r="K1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="18"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>74</v>
       </c>
       <c r="B2" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_xll.QIns_CreateInflationIndex(B3,B4,"Linear",B6,B7,"1y","USD",B5,"P")</f>
-        <v>USD.CPI¬30</v>
+        <v>USD.CPI¬79</v>
+      </c>
+      <c r="E2" s="2">
+        <f ca="1">EDATE(E1,-3)</f>
+        <v>43839</v>
+      </c>
+      <c r="F2">
+        <f ca="1">9/30</f>
+        <v>0.3</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>88</v>
@@ -5410,12 +5510,16 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
+      </c>
+      <c r="F3">
+        <f ca="1">F13-F14</f>
+        <v>2</v>
       </c>
       <c r="J3" s="2">
         <f ca="1">valDate</f>
@@ -5430,16 +5534,27 @@
         <v>1.329593611111116E-2</v>
       </c>
       <c r="M3" cm="1">
-        <f t="array" aca="1" ref="M3" ca="1">_xll.QCurves_GetCpiForecast($B$30,J3,3)</f>
-        <v>100.05308829634575</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M3" ca="1">_xll.QCurves_GetCpiForecast($B$30,J3,-3)</f>
+        <v>100.6</v>
+      </c>
+      <c r="N3">
+        <v>100.6</v>
+      </c>
+      <c r="O3" s="26">
+        <f ca="1">M3-N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>70</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
+      </c>
+      <c r="F4">
+        <f ca="1">F14+F3*F2</f>
+        <v>100.6</v>
       </c>
       <c r="J4" s="2">
         <f ca="1">EDATE(J3,3)</f>
@@ -5454,11 +5569,18 @@
         <v>1.0853461188319216E-2</v>
       </c>
       <c r="M4" cm="1">
-        <f t="array" aca="1" ref="M4" ca="1">_xll.QCurves_GetCpiForecast($B$30,J4,3)</f>
-        <v>101.56136075610513</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M4" ca="1">_xll.QCurves_GetCpiForecast($B$30,J4,-3)</f>
+        <v>101.84216235277678</v>
+      </c>
+      <c r="N4">
+        <v>101.84216235277678</v>
+      </c>
+      <c r="O4" s="26">
+        <f t="shared" ref="O4:O35" ca="1" si="0">M4-N4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>87</v>
       </c>
@@ -5467,7 +5589,7 @@
         <v>-3m</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" ref="J5:J35" ca="1" si="0">EDATE(J4,3)</f>
+        <f t="shared" ref="J5:J50" ca="1" si="1">EDATE(J4,3)</f>
         <v>44113</v>
       </c>
       <c r="K5" s="1">
@@ -5479,11 +5601,18 @@
         <v>8.3989074440587643E-3</v>
       </c>
       <c r="M5" cm="1">
-        <f t="array" aca="1" ref="M5" ca="1">_xll.QCurves_GetCpiForecast($B$30,J5,3)</f>
-        <v>103.08432470555356</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M5" ca="1">_xll.QCurves_GetCpiForecast($B$30,J5,-3)</f>
+        <v>103.08432470555357</v>
+      </c>
+      <c r="N5">
+        <v>103.08432470555357</v>
+      </c>
+      <c r="O5" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>68</v>
       </c>
@@ -5491,7 +5620,7 @@
         <v>71</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44205</v>
       </c>
       <c r="K6" s="1">
@@ -5503,37 +5632,58 @@
         <v>5.9724257990548448E-3</v>
       </c>
       <c r="M6" cm="1">
-        <f t="array" aca="1" ref="M6" ca="1">_xll.QCurves_GetCpiForecast($B$30,J6,3)</f>
-        <v>104.61791490204203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M6" ca="1">_xll.QCurves_GetCpiForecast($B$30,J6,-3)</f>
+        <v>104.60300530860663</v>
+      </c>
+      <c r="N6">
+        <v>104.60300530860663</v>
+      </c>
+      <c r="O6" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="2">
-        <f t="shared" ca="1" si="0"/>
+      <c r="G7">
+        <f ca="1">M7/M3-1</f>
+        <v>5.488753391311807E-2</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="23">
+        <f t="shared" ca="1" si="1"/>
         <v>44295</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="24">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J7)</f>
         <v>0.99041855357294528</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="24">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J7,J8,"Linear","Act365F")</f>
         <v>3.5609225435252819E-3</v>
       </c>
-      <c r="M7" cm="1">
-        <f t="array" aca="1" ref="M7" ca="1">_xll.QCurves_GetCpiForecast($B$30,J7,3)</f>
-        <v>106.12168591165967</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="25" cm="1">
+        <f t="array" aca="1" ref="M7" ca="1">_xll.QCurves_GetCpiForecast($B$30,J7,-3)</f>
+        <v>106.12168591165968</v>
+      </c>
+      <c r="N7">
+        <v>106.12168591165968</v>
+      </c>
+      <c r="O7" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J8" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44386</v>
       </c>
       <c r="K8" s="1">
@@ -5545,13 +5695,20 @@
         <v>1.1241970334315312E-3</v>
       </c>
       <c r="M8" cm="1">
-        <f t="array" aca="1" ref="M8" ca="1">_xll.QCurves_GetCpiForecast($B$30,J8,3)</f>
-        <v>107.65295686520498</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M8" ca="1">_xll.QCurves_GetCpiForecast($B$30,J8,-3)</f>
+        <v>107.81948182466114</v>
+      </c>
+      <c r="N8">
+        <v>107.81948182466114</v>
+      </c>
+      <c r="O8" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J9" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44478</v>
       </c>
       <c r="K9" s="1">
@@ -5563,11 +5720,18 @@
         <v>-1.3243538117687285E-3</v>
       </c>
       <c r="M9" cm="1">
-        <f t="array" aca="1" ref="M9" ca="1">_xll.QCurves_GetCpiForecast($B$30,J9,3)</f>
-        <v>109.35558564506148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M9" ca="1">_xll.QCurves_GetCpiForecast($B$30,J9,-3)</f>
+        <v>109.54101684366961</v>
+      </c>
+      <c r="N9">
+        <v>109.54101684366961</v>
+      </c>
+      <c r="O9" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>73</v>
       </c>
@@ -5576,10 +5740,10 @@
       </c>
       <c r="F10" t="str" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">_xll.QCurves_CreateFixingDictionary(E10,"USD.CPI",E12:F14)</f>
-        <v>CPI Fixings¬31</v>
+        <v>CPI Fixings¬78</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44570</v>
       </c>
       <c r="K10" s="1">
@@ -5591,11 +5755,18 @@
         <v>-3.7448422044676728E-3</v>
       </c>
       <c r="M10" cm="1">
-        <f t="array" aca="1" ref="M10" ca="1">_xll.QCurves_GetCpiForecast($B$30,J10,3)</f>
-        <v>111.14293781232169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M10" ca="1">_xll.QCurves_GetCpiForecast($B$30,J10,-3)</f>
+        <v>111.28146982991993</v>
+      </c>
+      <c r="N10">
+        <v>111.28146982991993</v>
+      </c>
+      <c r="O10" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>75</v>
       </c>
@@ -5611,33 +5782,49 @@
       <c r="F11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="2">
-        <f t="shared" ca="1" si="0"/>
+      <c r="I11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="23">
+        <f t="shared" ca="1" si="1"/>
         <v>44660</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="24">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J11)</f>
         <v>0.99050468498643585</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="24">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J11,J12,"Linear","Act365F")</f>
         <v>4.6165208548161734E-3</v>
       </c>
-      <c r="M11" cm="1">
-        <f t="array" aca="1" ref="M11" ca="1">_xll.QCurves_GetCpiForecast($B$30,J11,3)</f>
-        <v>113.02471112207618</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="10">
-        <v>0.05</v>
+      <c r="M11" s="25" cm="1">
+        <f t="array" aca="1" ref="M11" ca="1">_xll.QCurves_GetCpiForecast($B$30,J11,-3)</f>
+        <v>113.02192281617025</v>
+      </c>
+      <c r="N11">
+        <v>113.02192281617025</v>
+      </c>
+      <c r="O11" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f ca="1">valDate</f>
+        <v>43930</v>
+      </c>
+      <c r="B12">
+        <f ca="1">F4</f>
+        <v>100.6</v>
       </c>
       <c r="C12" t="str" cm="1">
-        <f t="array" aca="1" ref="C12" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A12,ComplexBuild!valDate,A12,$B$2,B12,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
-        <v>InfSwap6m¬30</v>
+        <f t="array" aca="1" ref="C12" ca="1">_xll.QIns_CreateInflationFwd("InfFwd0",A12,B2,B12,100000000,"USD.CPI","USD.OIS.1B","USD.CPI",D12)</f>
+        <v>InfFwd0¬82</v>
+      </c>
+      <c r="D12" s="2" cm="1">
+        <f t="array" aca="1" ref="D12" ca="1">_xll.QDates_AddPeriod(valDate,$B$5,"P","USD")</f>
+        <v>43839</v>
       </c>
       <c r="E12" s="17">
         <v>43891</v>
@@ -5646,7 +5833,7 @@
         <v>103</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44751</v>
       </c>
       <c r="K12" s="1">
@@ -5658,21 +5845,31 @@
         <v>4.8510727063655334E-3</v>
       </c>
       <c r="M12" cm="1">
-        <f t="array" aca="1" ref="M12" ca="1">_xll.QCurves_GetCpiForecast($B$30,J12,3)</f>
-        <v>114.94820586348568</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M12" ca="1">_xll.QCurves_GetCpiForecast($B$30,J12,-3)</f>
+        <v>115.19136548128431</v>
+      </c>
+      <c r="N12">
+        <v>115.10809080132813</v>
+      </c>
+      <c r="O12" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.3274679956176101E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="10">
-        <f ca="1">B12+0.005</f>
-        <v>5.5E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C13" t="str" cm="1">
-        <f t="array" aca="1" ref="C13" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A13,ComplexBuild!valDate,A13,$B$2,B13,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
-        <v>InfSwap1y¬30</v>
+        <f t="array" aca="1" ref="C13" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A13,ComplexBuild!valDate,A13,$B$2,B13,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D13)</f>
+        <v>InfSwap6m¬79</v>
+      </c>
+      <c r="D13" s="2" cm="1">
+        <f t="array" aca="1" ref="D13" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A13),$B$5)</f>
+        <v>44021</v>
       </c>
       <c r="E13" s="17">
         <v>43862</v>
@@ -5681,7 +5878,7 @@
         <v>102</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44843</v>
       </c>
       <c r="K13" s="1">
@@ -5693,21 +5890,31 @@
         <v>4.8702643663097681E-3</v>
       </c>
       <c r="M13" cm="1">
-        <f t="array" aca="1" ref="M13" ca="1">_xll.QCurves_GetCpiForecast($B$30,J13,3)</f>
-        <v>117.02564362611034</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M13" ca="1">_xll.QCurves_GetCpiForecast($B$30,J13,-3)</f>
+        <v>117.39564062318617</v>
+      </c>
+      <c r="N13">
+        <v>117.22625235372986</v>
+      </c>
+      <c r="O13" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16938826945630581</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B14" s="10">
-        <f t="shared" ref="B14:B16" ca="1" si="1">B13+0.005</f>
-        <v>0.06</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C14" t="str" cm="1">
-        <f t="array" aca="1" ref="C14" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A14,ComplexBuild!valDate,A14,$B$2,B14,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
-        <v>InfSwap2y¬30</v>
+        <f t="array" aca="1" ref="C14" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A14,ComplexBuild!valDate,A14,$B$2,B14,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D14)</f>
+        <v>InfSwap1y¬78</v>
+      </c>
+      <c r="D14" s="2" cm="1">
+        <f t="array" aca="1" ref="D14" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A14),$B$5)</f>
+        <v>44207</v>
       </c>
       <c r="E14" s="17">
         <v>43831</v>
@@ -5716,7 +5923,7 @@
         <v>100</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44935</v>
       </c>
       <c r="K14" s="1">
@@ -5728,53 +5935,76 @@
         <v>4.8891820475031661E-3</v>
       </c>
       <c r="M14" cm="1">
-        <f t="array" aca="1" ref="M14" ca="1">_xll.QCurves_GetCpiForecast($B$30,J14,3)</f>
-        <v>119.22338337900035</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M14" ca="1">_xll.QCurves_GetCpiForecast($B$30,J14,-3)</f>
+        <v>119.6241385688452</v>
+      </c>
+      <c r="N14">
+        <v>119.36769040670744</v>
+      </c>
+      <c r="O14" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25644816213775812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="C15" t="str" cm="1">
+        <f t="array" aca="1" ref="C15" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A15,ComplexBuild!valDate,A15,$B$2,B15,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D15)</f>
+        <v>InfSwap2y¬78</v>
+      </c>
+      <c r="D15" s="2" cm="1">
+        <f t="array" aca="1" ref="D15" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A15),$B$5)</f>
+        <v>44572</v>
+      </c>
+      <c r="I15" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="10">
-        <f t="shared" ca="1" si="1"/>
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="C15" t="str" cm="1">
-        <f t="array" aca="1" ref="C15" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A15,ComplexBuild!valDate,A15,$B$2,B15,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
-        <v>InfSwap3y¬30</v>
-      </c>
-      <c r="J15" s="2">
-        <f t="shared" ca="1" si="0"/>
+      <c r="J15" s="23">
+        <f t="shared" ca="1" si="1"/>
         <v>45025</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="24">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J15)</f>
         <v>0.98575776917644486</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="24">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J15,J16,"Linear","Act365F")</f>
         <v>6.3091638772783849E-3</v>
       </c>
-      <c r="M15" cm="1">
-        <f t="array" aca="1" ref="M15" ca="1">_xll.QCurves_GetCpiForecast($B$30,J15,3)</f>
-        <v>121.51481631861036</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="25" cm="1">
+        <f t="array" aca="1" ref="M15" ca="1">_xll.QCurves_GetCpiForecast($B$30,J15,-3)</f>
+        <v>121.85263651450421</v>
+      </c>
+      <c r="N15">
+        <v>121.509128459685</v>
+      </c>
+      <c r="O15" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34350805481921043</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="10">
-        <f t="shared" ca="1" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="C16" t="str" cm="1">
-        <f t="array" aca="1" ref="C16" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A16,ComplexBuild!valDate,A16,$B$2,B16,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
-        <v>InfSwap5y¬30</v>
+        <f t="array" aca="1" ref="C16" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A16,ComplexBuild!valDate,A16,$B$2,B16,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D16)</f>
+        <v>InfSwap3y¬78</v>
+      </c>
+      <c r="D16" s="2" cm="1">
+        <f t="array" aca="1" ref="D16" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A16),$B$5)</f>
+        <v>44936</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45116</v>
       </c>
       <c r="K16" s="1">
@@ -5786,23 +6016,34 @@
         <v>6.5613257933532371E-3</v>
       </c>
       <c r="M16" cm="1">
-        <f t="array" aca="1" ref="M16" ca="1">_xll.QCurves_GetCpiForecast($B$30,J16,3)</f>
-        <v>123.79859320175402</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M16" ca="1">_xll.QCurves_GetCpiForecast($B$30,J16,-3)</f>
+        <v>124.21778335068639</v>
+      </c>
+      <c r="N16">
+        <v>123.91532411304483</v>
+      </c>
+      <c r="O16" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.30245923764155691</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="10">
-        <v>7.4999999999999997E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C17" t="str" cm="1">
-        <f t="array" aca="1" ref="C17" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A17,ComplexBuild!valDate,A17,$B$2,B17,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
-        <v>InfSwap10y¬30</v>
+        <f t="array" aca="1" ref="C17" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A17,ComplexBuild!valDate,A17,$B$2,B17,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D17)</f>
+        <v>InfSwap5y¬78</v>
+      </c>
+      <c r="D17" s="2" cm="1">
+        <f t="array" aca="1" ref="D17" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A17),$B$5)</f>
+        <v>45666</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45208</v>
       </c>
       <c r="K17" s="1">
@@ -5814,23 +6055,34 @@
         <v>6.80037086562539E-3</v>
       </c>
       <c r="M17" cm="1">
-        <f t="array" aca="1" ref="M17" ca="1">_xll.QCurves_GetCpiForecast($B$30,J17,3)</f>
-        <v>126.14512285807679</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="21">
-        <v>6.7500000000000004E-2</v>
-      </c>
-      <c r="C18" s="19" t="str" cm="1">
-        <f t="array" aca="1" ref="C18" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A18,ComplexBuild!valDate,A18,$B$2,B18,1000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI")</f>
-        <v>InfSwap4y¬19</v>
+        <f t="array" aca="1" ref="M17" ca="1">_xll.QCurves_GetCpiForecast($B$30,J17,-3)</f>
+        <v>126.61131241754792</v>
+      </c>
+      <c r="N17">
+        <v>126.3517920108352</v>
+      </c>
+      <c r="O17" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25952040671272414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C18" t="str" cm="1">
+        <f t="array" aca="1" ref="C18" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A18,ComplexBuild!valDate,A18,$B$2,B18,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D18)</f>
+        <v>InfSwap10y¬78</v>
+      </c>
+      <c r="D18" s="2" cm="1">
+        <f t="array" aca="1" ref="D18" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A18),$B$5)</f>
+        <v>47492</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45300</v>
       </c>
       <c r="K18" s="1">
@@ -5842,11 +6094,18 @@
         <v>7.0380632261232545E-3</v>
       </c>
       <c r="M18" cm="1">
-        <f t="array" aca="1" ref="M18" ca="1">_xll.QCurves_GetCpiForecast($B$30,J18,3)</f>
-        <v>128.50509420877495</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M18" ca="1">_xll.QCurves_GetCpiForecast($B$30,J18,-3)</f>
+        <v>129.03114400162772</v>
+      </c>
+      <c r="N18">
+        <v>128.81503428112876</v>
+      </c>
+      <c r="O18" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21610972049896304</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>78</v>
       </c>
@@ -5854,7 +6113,7 @@
         <v>82</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45391</v>
       </c>
       <c r="K19" s="1">
@@ -5866,17 +6125,24 @@
         <v>7.8483692645597777E-3</v>
       </c>
       <c r="M19" cm="1">
-        <f t="array" aca="1" ref="M19" ca="1">_xll.QCurves_GetCpiForecast($B$30,J19,3)</f>
-        <v>130.89357541207272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M19" ca="1">_xll.QCurves_GetCpiForecast($B$30,J19,-3)</f>
+        <v>131.45097558570751</v>
+      </c>
+      <c r="N19">
+        <v>131.27827655142232</v>
+      </c>
+      <c r="O19" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17269903428518774</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>64</v>
       </c>
       <c r="B20" t="str">
         <f ca="1">ComplexBuild!C28</f>
-        <v>FundingInstruments_USD¬2</v>
+        <v>FundingInstruments_USD¬0</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
@@ -5885,7 +6151,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45482</v>
       </c>
       <c r="K20" s="1">
@@ -5897,17 +6163,24 @@
         <v>8.1539496965475442E-3</v>
       </c>
       <c r="M20" cm="1">
-        <f t="array" aca="1" ref="M20" ca="1">_xll.QCurves_GetCpiForecast($B$30,J20,3)</f>
-        <v>133.27823562988155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M20" ca="1">_xll.QCurves_GetCpiForecast($B$30,J20,-3)</f>
+        <v>133.84450465256904</v>
+      </c>
+      <c r="N20">
+        <v>133.71474444921267</v>
+      </c>
+      <c r="O20" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.12976020335636917</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>79</v>
       </c>
       <c r="B21" t="str" cm="1">
-        <f t="array" aca="1" ref="B21" ca="1">_xll.QIns_CreateFundingInstrumentCollection(A21,C12:C17)</f>
-        <v>CPI¬30</v>
+        <f t="array" aca="1" ref="B21" ca="1">_xll.QIns_CreateFundingInstrumentCollection(A21,C12:C18)</f>
+        <v>CPI¬79</v>
       </c>
       <c r="E21" t="s">
         <v>54</v>
@@ -5916,7 +6189,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45574</v>
       </c>
       <c r="K21" s="1">
@@ -5928,17 +6201,24 @@
         <v>8.4611388513162224E-3</v>
       </c>
       <c r="M21" cm="1">
-        <f t="array" aca="1" ref="M21" ca="1">_xll.QCurves_GetCpiForecast($B$30,J21,3)</f>
-        <v>135.75660866681818</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M21" ca="1">_xll.QCurves_GetCpiForecast($B$30,J21,-3)</f>
+        <v>136.23803371943058</v>
+      </c>
+      <c r="N21">
+        <v>136.15121234700302</v>
+      </c>
+      <c r="O21" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.6821372427550614E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>81</v>
       </c>
       <c r="B22" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection(A22,B20:B21)</f>
-        <v>FicCPI¬30</v>
+        <v>FicCPI¬78</v>
       </c>
       <c r="E22" t="s">
         <v>77</v>
@@ -5947,7 +6227,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45666</v>
       </c>
       <c r="K22" s="1">
@@ -5959,34 +6239,58 @@
         <v>8.7648020218674943E-3</v>
       </c>
       <c r="M22" cm="1">
-        <f t="array" aca="1" ref="M22" ca="1">_xll.QCurves_GetCpiForecast($B$30,J22,3)</f>
-        <v>138.35111982193467</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J23" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="array" aca="1" ref="M22" ca="1">_xll.QCurves_GetCpiForecast($B$30,J22,-3)</f>
+        <v>138.65786530351036</v>
+      </c>
+      <c r="N22">
+        <v>138.61445461729659</v>
+      </c>
+      <c r="O22" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.3410686213775307E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="23">
+        <f t="shared" ca="1" si="1"/>
         <v>45756</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="24">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J23)</f>
         <v>0.97109424852837223</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="24">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J23,J24,"Linear","Act365F")</f>
         <v>8.9084999722346507E-3</v>
       </c>
-      <c r="M23" cm="1">
-        <f t="array" aca="1" ref="M23" ca="1">_xll.QCurves_GetCpiForecast($B$30,J23,3)</f>
+      <c r="M23" s="25" cm="1">
+        <f t="array" aca="1" ref="M23" ca="1">_xll.QCurves_GetCpiForecast($B$30,J23,-3)</f>
         <v>141.07769688759015</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>141.07769688759015</v>
+      </c>
+      <c r="O23" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="E24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" t="str">
+        <f ca="1">ComplexBuild!J28</f>
+        <v>fxMatrix¬0</v>
+      </c>
       <c r="J24" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45847</v>
       </c>
       <c r="K24" s="1">
@@ -5998,27 +6302,40 @@
         <v>9.1990422107138606E-3</v>
       </c>
       <c r="M24" cm="1">
-        <f t="array" aca="1" ref="M24" ca="1">_xll.QCurves_GetCpiForecast($B$30,J24,3)</f>
-        <v>143.86042465357392</v>
-      </c>
-      <c r="O24" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="P24" t="str" cm="1">
-        <f t="array" aca="1" ref="P24" ca="1">_xll.QIns_AssetPortfolioExpectedFlows("CashflowResult",B34,B33)</f>
-        <v>CashflowResult¬7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M24" ca="1">_xll.QCurves_GetCpiForecast($B$30,J24,-3)</f>
+        <v>144.3421547556126</v>
+      </c>
+      <c r="N24">
+        <v>144.3421547556126</v>
+      </c>
+      <c r="O24" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="S24" t="str" cm="1">
+        <f t="array" aca="1" ref="S24" ca="1">_xll.QRisk_PortfolioIrBenchmarkDelta(R24,B41,B33,B22,"USD")</f>
+        <v>BenchmarkRisk¬79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>80</v>
       </c>
       <c r="B25" t="str" cm="1">
-        <f t="array" aca="1" ref="B25" ca="1">_xll.QCurves_CreateFundingModel(A25,valDate,B22,E20:F22,,,F10)</f>
-        <v>ModelCPI¬31</v>
+        <f t="array" aca="1" ref="B25" ca="1">_xll.QCurves_CreateFundingModel(A25,valDate,B22,E20:F22,ComplexBuild!J28,,F10)</f>
+        <v>ModelCPI¬81</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45939</v>
       </c>
       <c r="K25" s="1">
@@ -6030,13 +6347,20 @@
         <v>9.4910842711828682E-3</v>
       </c>
       <c r="M25" cm="1">
-        <f t="array" aca="1" ref="M25" ca="1">_xll.QCurves_GetCpiForecast($B$30,J25,3)</f>
-        <v>146.82167910410232</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M25" ca="1">_xll.QCurves_GetCpiForecast($B$30,J25,-3)</f>
+        <v>147.64288437772422</v>
+      </c>
+      <c r="N25">
+        <v>147.64288437772422</v>
+      </c>
+      <c r="O25" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="J26" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46031</v>
       </c>
       <c r="K26" s="1">
@@ -6048,36 +6372,59 @@
         <v>9.7797112314272662E-3</v>
       </c>
       <c r="M26" cm="1">
-        <f t="array" aca="1" ref="M26" ca="1">_xll.QCurves_GetCpiForecast($B$30,J26,3)</f>
-        <v>149.88392218361739</v>
-      </c>
-      <c r="O26" s="14" t="str">
-        <f t="array" aca="1" ref="O26:S40" ca="1">_xll.QCube_DisplayCube(P24)</f>
+        <f t="array" aca="1" ref="M26" ca="1">_xll.QCurves_GetCpiForecast($B$30,J26,-3)</f>
+        <v>150.97988575392495</v>
+      </c>
+      <c r="N26">
+        <v>150.97988575392495</v>
+      </c>
+      <c r="O26" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="14" t="str">
+        <f t="array" aca="1" ref="Q26:Y40" ca="1">_xll.QCube_DisplayCube(S24)</f>
         <v>TradeId</v>
       </c>
-      <c r="P26" s="14" t="str">
-        <f ca="1"/>
-        <v>Currency</v>
-      </c>
-      <c r="Q26" s="14" t="str">
+      <c r="R26" s="14" t="str">
         <f ca="1"/>
         <v>TradeType</v>
       </c>
-      <c r="R26" s="14" t="str">
-        <f ca="1"/>
-        <v>PayDate</v>
-      </c>
       <c r="S26" s="14" t="str">
         <f ca="1"/>
+        <v>Curve</v>
+      </c>
+      <c r="T26" s="14" t="str">
+        <f ca="1"/>
+        <v>RiskDate</v>
+      </c>
+      <c r="U26" s="14" t="str">
+        <f ca="1"/>
+        <v>Benchmark</v>
+      </c>
+      <c r="V26" s="14" t="str">
+        <f ca="1"/>
+        <v>Metric</v>
+      </c>
+      <c r="W26" s="14" t="str">
+        <f ca="1"/>
+        <v>Units</v>
+      </c>
+      <c r="X26" s="14" t="str">
+        <f ca="1"/>
+        <v>BumpSize</v>
+      </c>
+      <c r="Y26" s="14" t="str">
+        <f ca="1"/>
         <v>Value</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>85</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46121</v>
       </c>
       <c r="K27" s="1">
@@ -6089,41 +6436,64 @@
         <v>1.0067156644269194E-2</v>
       </c>
       <c r="M27" cm="1">
-        <f t="array" aca="1" ref="M27" ca="1">_xll.QCurves_GetCpiForecast($B$30,J27,3)</f>
-        <v>153.02823461613627</v>
-      </c>
-      <c r="O27" t="str">
-        <f ca="1"/>
-        <v>InfSwap6m</v>
-      </c>
-      <c r="P27" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q27" t="str">
+        <f t="array" aca="1" ref="M27" ca="1">_xll.QCurves_GetCpiForecast($B$30,J27,-3)</f>
+        <v>154.31688713012568</v>
+      </c>
+      <c r="N27">
+        <v>154.31688713012568</v>
+      </c>
+      <c r="O27" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="13" t="str">
+        <f ca="1"/>
+        <v>TradeObj</v>
+      </c>
+      <c r="R27" s="13" t="str">
         <f ca="1"/>
         <v>InfPerfSwap</v>
       </c>
-      <c r="R27" s="2">
-        <f ca="1"/>
-        <v>44113</v>
-      </c>
-      <c r="S27" s="4">
-        <f ca="1"/>
-        <v>24695.07659595993</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S27" s="13" t="str">
+        <f ca="1"/>
+        <v>USD.CPI</v>
+      </c>
+      <c r="T27" s="19">
+        <f ca="1"/>
+        <v>45666</v>
+      </c>
+      <c r="U27" s="20" t="str">
+        <f ca="1"/>
+        <v>InfSwap5y</v>
+      </c>
+      <c r="V27" s="13" t="str">
+        <f ca="1"/>
+        <v>IrBenchmarkDelta</v>
+      </c>
+      <c r="W27" s="13" t="str">
+        <f ca="1"/>
+        <v>Nominal</v>
+      </c>
+      <c r="X27" s="13">
+        <f ca="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="Y27" s="20">
+        <f ca="1"/>
+        <v>20099019.285653304</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="array" aca="1" ref="A28:A30" ca="1">_xll.QCurves_ListCurvesInModel(B25)</f>
         <v>USD.LIBOR.3M</v>
       </c>
       <c r="B28" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A28,"curve.cpiBuild."&amp;A28)</f>
-        <v>curve.cpiBuild.USD.LIBOR.3M¬30</v>
+        <v>curve.cpiBuild.USD.LIBOR.3M¬78</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46212</v>
       </c>
       <c r="K28" s="1">
@@ -6135,41 +6505,64 @@
         <v>1.0357813597547285E-2</v>
       </c>
       <c r="M28" cm="1">
-        <f t="array" aca="1" ref="M28" ca="1">_xll.QCurves_GetCpiForecast($B$30,J28,3)</f>
-        <v>156.13676504321063</v>
-      </c>
-      <c r="O28" t="str">
-        <f ca="1"/>
-        <v>InfSwap6m</v>
-      </c>
-      <c r="P28" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q28" t="str">
+        <f t="array" aca="1" ref="M28" ca="1">_xll.QCurves_GetCpiForecast($B$30,J28,-3)</f>
+        <v>157.58134499814813</v>
+      </c>
+      <c r="N28">
+        <v>157.58134499814813</v>
+      </c>
+      <c r="O28" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="13" t="str">
+        <f ca="1"/>
+        <v>TradeObj</v>
+      </c>
+      <c r="R28" s="13" t="str">
         <f ca="1"/>
         <v>InfPerfSwap</v>
       </c>
-      <c r="R28" s="2">
-        <f ca="1"/>
-        <v>44113</v>
-      </c>
-      <c r="S28" s="4">
-        <f ca="1"/>
-        <v>-24695.07659595993</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S28" s="13" t="str">
+        <f ca="1"/>
+        <v>USD.CPI</v>
+      </c>
+      <c r="T28" s="19">
+        <f ca="1"/>
+        <v>47492</v>
+      </c>
+      <c r="U28" s="20" t="str">
+        <f ca="1"/>
+        <v>InfSwap10y</v>
+      </c>
+      <c r="V28" s="13" t="str">
+        <f ca="1"/>
+        <v>IrBenchmarkDelta</v>
+      </c>
+      <c r="W28" s="13" t="str">
+        <f ca="1"/>
+        <v>Nominal</v>
+      </c>
+      <c r="X28" s="13">
+        <f ca="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="Y28" s="20">
+        <f ca="1"/>
+        <v>5067916.5794108231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f ca="1"/>
         <v>USD.OIS.1B</v>
       </c>
       <c r="B29" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A29,"curve.cpiBuild."&amp;A29)</f>
-        <v>curve.cpiBuild.USD.OIS.1B¬30</v>
+        <v>curve.cpiBuild.USD.OIS.1B¬78</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46304</v>
       </c>
       <c r="K29" s="1">
@@ -6181,41 +6574,64 @@
         <v>1.0649940758556239E-2</v>
       </c>
       <c r="M29" cm="1">
-        <f t="array" aca="1" ref="M29" ca="1">_xll.QCurves_GetCpiForecast($B$30,J29,3)</f>
-        <v>159.36834522746165</v>
-      </c>
-      <c r="O29" t="str">
-        <f ca="1"/>
-        <v>InfSwap1y</v>
-      </c>
-      <c r="P29" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q29" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R29" s="2">
-        <f ca="1"/>
-        <v>44295</v>
-      </c>
-      <c r="S29" s="4">
-        <f ca="1"/>
-        <v>54887.533913118066</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M29" ca="1">_xll.QCurves_GetCpiForecast($B$30,J29,-3)</f>
+        <v>160.88207462025971</v>
+      </c>
+      <c r="N29">
+        <v>160.88207462025971</v>
+      </c>
+      <c r="O29" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T29" s="19" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U29" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y29" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f ca="1"/>
         <v>USD.CPI</v>
       </c>
       <c r="B30" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A30,"curve.cpiBuild."&amp;A30)</f>
-        <v>curve.cpiBuild.USD.CPI¬31</v>
+        <v>curve.cpiBuild.USD.CPI¬78</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46396</v>
       </c>
       <c r="K30" s="1">
@@ -6227,33 +6643,56 @@
         <v>1.0938586201982145E-2</v>
       </c>
       <c r="M30" cm="1">
-        <f t="array" aca="1" ref="M30" ca="1">_xll.QCurves_GetCpiForecast($B$30,J30,3)</f>
-        <v>162.6775589612019</v>
-      </c>
-      <c r="O30" t="str">
-        <f ca="1"/>
-        <v>InfSwap1y</v>
-      </c>
-      <c r="P30" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q30" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R30" s="2">
-        <f ca="1"/>
-        <v>44295</v>
-      </c>
-      <c r="S30" s="4">
-        <f ca="1"/>
-        <v>-54887.533913118066</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M30" ca="1">_xll.QCurves_GetCpiForecast($B$30,J30,-3)</f>
+        <v>164.21907599646045</v>
+      </c>
+      <c r="N30">
+        <v>164.21907599646045</v>
+      </c>
+      <c r="O30" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T30" s="19" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U30" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y30" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="J31" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46486</v>
       </c>
       <c r="K31" s="1">
@@ -6265,36 +6704,59 @@
         <v>1.174513824912918E-2</v>
       </c>
       <c r="M31" cm="1">
-        <f t="array" aca="1" ref="M31" ca="1">_xll.QCurves_GetCpiForecast($B$30,J31,3)</f>
-        <v>166.04418259794028</v>
-      </c>
-      <c r="O31" t="str">
-        <f ca="1"/>
-        <v>InfSwap2y</v>
-      </c>
-      <c r="P31" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q31" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R31" s="2">
-        <f ca="1"/>
-        <v>44659</v>
-      </c>
-      <c r="S31" s="4">
-        <f ca="1"/>
-        <v>123290.30664938733</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M31" ca="1">_xll.QCurves_GetCpiForecast($B$30,J31,-3)</f>
+        <v>167.55607737266118</v>
+      </c>
+      <c r="N31">
+        <v>167.55607737266118</v>
+      </c>
+      <c r="O31" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T31" s="19" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U31" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y31" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>89</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46577</v>
       </c>
       <c r="K32" s="1">
@@ -6306,41 +6768,66 @@
         <v>1.2071854462021157E-2</v>
       </c>
       <c r="M32" cm="1">
-        <f t="array" aca="1" ref="M32" ca="1">_xll.QCurves_GetCpiForecast($B$30,J32,3)</f>
-        <v>169.34377748516795</v>
-      </c>
-      <c r="O32" t="str">
-        <f ca="1"/>
-        <v>InfSwap2y</v>
-      </c>
-      <c r="P32" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q32" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R32" s="2">
-        <f ca="1"/>
-        <v>44659</v>
-      </c>
-      <c r="S32" s="4">
-        <f ca="1"/>
-        <v>-123290.30664938757</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M32" ca="1">_xll.QCurves_GetCpiForecast($B$30,J32,-3)</f>
+        <v>170.82053524068365</v>
+      </c>
+      <c r="N32">
+        <v>170.82053524068365</v>
+      </c>
+      <c r="O32" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T32" s="19" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U32" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y32" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f ca="1">A32</f>
         <v>AssetFxModel</v>
       </c>
       <c r="B33" t="str" cm="1">
         <f t="array" aca="1" ref="B33" ca="1">_xll.QCurves_CreateAssetFxModel(A33,valDate,,,B25)</f>
-        <v>AssetFxModel¬21</v>
-      </c>
+        <v>AssetFxModel¬78</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
       <c r="J33" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46669</v>
       </c>
       <c r="K33" s="1">
@@ -6352,40 +6839,65 @@
         <v>1.2400193204532005E-2</v>
       </c>
       <c r="M33" cm="1">
-        <f t="array" aca="1" ref="M33" ca="1">_xll.QCurves_GetCpiForecast($B$30,J33,3)</f>
-        <v>172.74570841995714</v>
-      </c>
-      <c r="O33" t="str">
-        <f ca="1"/>
-        <v>InfSwap3y</v>
-      </c>
-      <c r="P33" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q33" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R33" s="2">
-        <f ca="1"/>
-        <v>45023</v>
-      </c>
-      <c r="S33" s="4">
-        <f ca="1"/>
-        <v>207381.46579058992</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M33" ca="1">_xll.QCurves_GetCpiForecast($B$30,J33,-3)</f>
+        <v>174.12126486279524</v>
+      </c>
+      <c r="N33">
+        <v>174.12126486279524</v>
+      </c>
+      <c r="O33" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T33" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U33" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>90</v>
       </c>
       <c r="B34" t="str" cm="1">
-        <f t="array" aca="1" ref="B34" ca="1">_xll.QIns_CreatePortfolio(A34,C12:C18)</f>
-        <v>Porfolio¬22</v>
-      </c>
+        <f t="array" aca="1" ref="B34" ca="1">_xll.QIns_CreatePortfolio(A34,C13:C18)</f>
+        <v>Porfolio¬78</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
       <c r="J34" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46761</v>
       </c>
       <c r="K34" s="1">
@@ -6397,173 +6909,1039 @@
         <v>1.2726552729230234E-2</v>
       </c>
       <c r="M34" cm="1">
-        <f t="array" aca="1" ref="M34" ca="1">_xll.QCurves_GetCpiForecast($B$30,J34,3)</f>
-        <v>176.20137882673822</v>
-      </c>
-      <c r="O34" t="str">
-        <f ca="1"/>
-        <v>InfSwap3y</v>
-      </c>
-      <c r="P34" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q34" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R34" s="2">
-        <f ca="1"/>
-        <v>45023</v>
-      </c>
-      <c r="S34" s="4">
-        <f ca="1"/>
-        <v>-207381.46579058969</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="array" aca="1" ref="M34" ca="1">_xll.QCurves_GetCpiForecast($B$30,J34,-3)</f>
+        <v>177.45826623899598</v>
+      </c>
+      <c r="N34">
+        <v>177.45826623899598</v>
+      </c>
+      <c r="O34" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T34" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U34" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="H35" s="27"/>
       <c r="J35" s="2">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46852</v>
       </c>
       <c r="K35" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J35)</f>
         <v>0.94044386983374129</v>
       </c>
-      <c r="L35" s="1"/>
+      <c r="L35" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J35,J36,"Linear","Act365F")</f>
+        <v>1.3051364424061372E-2</v>
+      </c>
       <c r="M35" cm="1">
-        <f t="array" aca="1" ref="M35" ca="1">_xll.QCurves_GetCpiForecast($B$30,J35,3)</f>
-        <v>179.68947192352954</v>
-      </c>
-      <c r="O35" t="str">
-        <f ca="1"/>
-        <v>InfSwap5y</v>
-      </c>
-      <c r="P35" t="str">
+        <f t="array" aca="1" ref="M35" ca="1">_xll.QCurves_GetCpiForecast($B$30,J35,-3)</f>
+        <v>180.79526761519671</v>
+      </c>
+      <c r="N35">
+        <v>180.79526761519671</v>
+      </c>
+      <c r="O35" s="26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T35" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U35" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="H36" s="27"/>
+      <c r="J36" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>46943</v>
+      </c>
+      <c r="K36" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J36)</f>
+        <v>0.93739368282752511</v>
+      </c>
+      <c r="L36" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J36,J37,"Linear","Act365F")</f>
+        <v>1.3378232131234452E-2</v>
+      </c>
+      <c r="M36" cm="1">
+        <f t="array" aca="1" ref="M36" ca="1">_xll.QCurves_GetCpiForecast($B$30,J36,-3)</f>
+        <v>184.0959972373083</v>
+      </c>
+      <c r="N36">
+        <v>184.0959972373083</v>
+      </c>
+      <c r="O36" s="26">
+        <f t="shared" ref="O36:O50" ca="1" si="2">M36-N36</f>
+        <v>0</v>
+      </c>
+      <c r="Q36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T36" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U36" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="2">
+        <v>43923</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="H37" s="27"/>
+      <c r="J37" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47035</v>
+      </c>
+      <c r="K37" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J37)</f>
+        <v>0.93424336976059208</v>
+      </c>
+      <c r="L37" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J37,J38,"Linear","Act365F")</f>
+        <v>1.3724276514456651E-2</v>
+      </c>
+      <c r="M37" cm="1">
+        <f t="array" aca="1" ref="M37" ca="1">_xll.QCurves_GetCpiForecast($B$30,J37,-3)</f>
+        <v>187.39672685941991</v>
+      </c>
+      <c r="N37">
+        <v>187.39672685941991</v>
+      </c>
+      <c r="O37" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T37" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U37" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="2">
+        <v>46114</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="J38" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47127</v>
+      </c>
+      <c r="K38" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J38)</f>
+        <v>0.93102271110902513</v>
+      </c>
+      <c r="L38" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J38,J39,"Linear","Act365F")</f>
+        <v>1.4042264430980828E-2</v>
+      </c>
+      <c r="M38" cm="1">
+        <f t="array" aca="1" ref="M38" ca="1">_xll.QCurves_GetCpiForecast($B$30,J38,-3)</f>
+        <v>190.73372823562062</v>
+      </c>
+      <c r="N38">
+        <v>190.73372823562062</v>
+      </c>
+      <c r="O38" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T38" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U38" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="28">
+        <v>25000000</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="J39" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47217</v>
+      </c>
+      <c r="K39" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J39)</f>
+        <v>0.92781019044262547</v>
+      </c>
+      <c r="L39" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J39,J40,"Linear","Act365F")</f>
+        <v>1.406428851736794E-2</v>
+      </c>
+      <c r="M39" cm="1">
+        <f t="array" aca="1" ref="M39" ca="1">_xll.QCurves_GetCpiForecast($B$30,J39,-3)</f>
+        <v>194.07072961182138</v>
+      </c>
+      <c r="N39">
+        <v>194.07072961182138</v>
+      </c>
+      <c r="O39" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T39" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U39" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47308</v>
+      </c>
+      <c r="K40" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J40)</f>
+        <v>0.92456824822801198</v>
+      </c>
+      <c r="L40" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J40,J41,"Linear","Act365F")</f>
+        <v>1.4164353801983555E-2</v>
+      </c>
+      <c r="M40" cm="1">
+        <f t="array" aca="1" ref="M40" ca="1">_xll.QCurves_GetCpiForecast($B$30,J40,-3)</f>
+        <v>197.33518747984382</v>
+      </c>
+      <c r="N40">
+        <v>197.33518747984382</v>
+      </c>
+      <c r="O40" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T40" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U40" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="V40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" t="str" cm="1">
+        <f t="array" aca="1" ref="B41" ca="1">_xll.QIns_CreateInflationPerfSwap(A41,B37,B38,B2,B40,B39,"USD.CPI","USD.OIS.1B","Pay")</f>
+        <v>TradeObj¬81</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47400</v>
+      </c>
+      <c r="K41" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J41)</f>
+        <v>0.92127910375625865</v>
+      </c>
+      <c r="L41" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J41,J42,"Linear","Act365F")</f>
+        <v>9.6463533021110826E-3</v>
+      </c>
+      <c r="M41" cm="1">
+        <f t="array" aca="1" ref="M41" ca="1">_xll.QCurves_GetCpiForecast($B$30,J41,-3)</f>
+        <v>200.63591710195541</v>
+      </c>
+      <c r="N41">
+        <v>200.63591710195541</v>
+      </c>
+      <c r="O41" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47492</v>
+      </c>
+      <c r="K42" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J42)</f>
+        <v>0.9190445300635528</v>
+      </c>
+      <c r="L42" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J42,J43,"Linear","Act365F")</f>
+        <v>-6.4213756726114674E-3</v>
+      </c>
+      <c r="M42" cm="1">
+        <f t="array" aca="1" ref="M42" ca="1">_xll.QCurves_GetCpiForecast($B$30,J42,-3)</f>
+        <v>203.97291847815615</v>
+      </c>
+      <c r="N42">
+        <v>203.97291847815615</v>
+      </c>
+      <c r="O42" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="R42" t="str" cm="1">
+        <f t="array" aca="1" ref="R42" ca="1">_xll.QIns_AssetPortfolioExpectedFlows("CashflowResult",B41,B33)</f>
+        <v>CashflowResult¬78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I43" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="23">
+        <f t="shared" ca="1" si="1"/>
+        <v>47582</v>
+      </c>
+      <c r="K43" s="24">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J43)</f>
+        <v>0.92050200959503314</v>
+      </c>
+      <c r="L43" s="24">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J43,J44,"Linear","Act365F")</f>
+        <v>8.2876233266823661E-3</v>
+      </c>
+      <c r="M43" s="25" cm="1">
+        <f t="array" aca="1" ref="M43" ca="1">_xll.QCurves_GetCpiForecast($B$30,J43,-3)</f>
+        <v>207.30991985435688</v>
+      </c>
+      <c r="N43">
+        <v>207.30991985435688</v>
+      </c>
+      <c r="O43" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J44" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47673</v>
+      </c>
+      <c r="K44" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J44)</f>
+        <v>0.91860396310033687</v>
+      </c>
+      <c r="L44" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J44,J45,"Linear","Act365F")</f>
+        <v>8.2877173512875477E-3</v>
+      </c>
+      <c r="M44" cm="1">
+        <f t="array" aca="1" ref="M44" ca="1">_xll.QCurves_GetCpiForecast($B$30,J44,-3)</f>
+        <v>210.57437772237932</v>
+      </c>
+      <c r="N44">
+        <v>210.57437772237932</v>
+      </c>
+      <c r="O44" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="14" t="str">
+        <f t="array" aca="1" ref="Q44:U58" ca="1">_xll.QCube_DisplayCube(R42)</f>
+        <v>TradeId</v>
+      </c>
+      <c r="R44" s="14" t="str">
+        <f ca="1"/>
+        <v>Currency</v>
+      </c>
+      <c r="S44" s="14" t="str">
+        <f ca="1"/>
+        <v>TradeType</v>
+      </c>
+      <c r="T44" s="14" t="str">
+        <f ca="1"/>
+        <v>PayDate</v>
+      </c>
+      <c r="U44" s="14" t="str">
+        <f ca="1"/>
+        <v>Value</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J45" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47765</v>
+      </c>
+      <c r="K45" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J45)</f>
+        <v>0.91668903738264296</v>
+      </c>
+      <c r="L45" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J45,J46,"Linear","Act365F")</f>
+        <v>8.2877173512875477E-3</v>
+      </c>
+      <c r="M45" cm="1">
+        <f t="array" aca="1" ref="M45" ca="1">_xll.QCurves_GetCpiForecast($B$30,J45,-3)</f>
+        <v>213.87510734449094</v>
+      </c>
+      <c r="N45">
+        <v>213.87510734449094</v>
+      </c>
+      <c r="O45" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q45" t="str">
+        <f ca="1"/>
+        <v>TradeObj</v>
+      </c>
+      <c r="R45" t="str">
         <f ca="1"/>
         <v>USD</v>
       </c>
-      <c r="Q35" t="str">
+      <c r="S45" t="str">
         <f ca="1"/>
         <v>InfPerfSwap</v>
       </c>
-      <c r="R35" s="2">
-        <f ca="1"/>
-        <v>45756</v>
-      </c>
-      <c r="S35" s="4">
-        <f ca="1"/>
-        <v>402362.79212316248</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O36" t="str">
-        <f ca="1"/>
-        <v>InfSwap5y</v>
-      </c>
-      <c r="P36" t="str">
+      <c r="T45" s="2">
+        <f ca="1"/>
+        <v>46114</v>
+      </c>
+      <c r="U45" s="4">
+        <f ca="1"/>
+        <v>13464460.265854284</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J46" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47857</v>
+      </c>
+      <c r="K46" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J46)</f>
+        <v>0.91477810352722211</v>
+      </c>
+      <c r="L46" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J46,J47,"Linear","Act365F")</f>
+        <v>8.2875293034977808E-3</v>
+      </c>
+      <c r="M46" cm="1">
+        <f t="array" aca="1" ref="M46" ca="1">_xll.QCurves_GetCpiForecast($B$30,J46,-3)</f>
+        <v>217.21210872069167</v>
+      </c>
+      <c r="N46">
+        <v>217.21210872069167</v>
+      </c>
+      <c r="O46" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q46" t="str">
+        <f ca="1"/>
+        <v>TradeObj</v>
+      </c>
+      <c r="R46" t="str">
         <f ca="1"/>
         <v>USD</v>
       </c>
-      <c r="Q36" t="str">
+      <c r="S46" t="str">
         <f ca="1"/>
         <v>InfPerfSwap</v>
       </c>
-      <c r="R36" s="2">
-        <f ca="1"/>
-        <v>45756</v>
-      </c>
-      <c r="S36" s="4">
-        <f ca="1"/>
-        <v>-402362.79212316248</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O37" t="str">
-        <f ca="1"/>
-        <v>InfSwap10y</v>
-      </c>
-      <c r="P37" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q37" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R37" s="2">
-        <f ca="1"/>
-        <v>47582</v>
-      </c>
-      <c r="S37" s="4">
-        <f ca="1"/>
-        <v>1060734.7898047399</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O38" t="str">
-        <f ca="1"/>
-        <v>InfSwap10y</v>
-      </c>
-      <c r="P38" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q38" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R38" s="2">
-        <f ca="1"/>
-        <v>47582</v>
-      </c>
-      <c r="S38" s="4">
-        <f ca="1"/>
-        <v>-1060734.7898047403</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O39" s="6" t="str">
-        <f ca="1"/>
-        <v>InfSwap4y</v>
-      </c>
-      <c r="P39" s="6" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q39" s="6" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R39" s="7">
-        <f ca="1"/>
-        <v>45391</v>
-      </c>
-      <c r="S39" s="22">
-        <f ca="1"/>
-        <v>301128.98023929156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O40" s="6" t="str">
-        <f ca="1"/>
-        <v>InfSwap4y</v>
-      </c>
-      <c r="P40" s="6" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="Q40" s="6" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="R40" s="7">
-        <f ca="1"/>
-        <v>45391</v>
-      </c>
-      <c r="S40" s="22">
-        <f ca="1"/>
-        <v>-298588.44691406208</v>
+      <c r="T46" s="2">
+        <f ca="1"/>
+        <v>46114</v>
+      </c>
+      <c r="U46" s="4">
+        <f ca="1"/>
+        <v>-12513071.695675237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J47" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>47947</v>
+      </c>
+      <c r="K47" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J47)</f>
+        <v>0.91291256635443463</v>
+      </c>
+      <c r="L47" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J47,J48,"Linear","Act365F")</f>
+        <v>8.2876233266823661E-3</v>
+      </c>
+      <c r="M47" cm="1">
+        <f t="array" aca="1" ref="M47" ca="1">_xll.QCurves_GetCpiForecast($B$30,J47,-3)</f>
+        <v>220.54911009689241</v>
+      </c>
+      <c r="N47">
+        <v>220.54911009689241</v>
+      </c>
+      <c r="O47" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T47" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U47" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J48" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>48038</v>
+      </c>
+      <c r="K48" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J48)</f>
+        <v>0.91103016905549172</v>
+      </c>
+      <c r="L48" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J48,J49,"Linear","Act365F")</f>
+        <v>8.2877173512875477E-3</v>
+      </c>
+      <c r="M48" cm="1">
+        <f t="array" aca="1" ref="M48" ca="1">_xll.QCurves_GetCpiForecast($B$30,J48,-3)</f>
+        <v>223.81356796491485</v>
+      </c>
+      <c r="N48">
+        <v>223.81356796491485</v>
+      </c>
+      <c r="O48" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T48" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U48" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="J49" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>48130</v>
+      </c>
+      <c r="K49" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J49)</f>
+        <v>0.90913103170098752</v>
+      </c>
+      <c r="L49" s="1">
+        <f ca="1">_xll.QCurves_GetForwardRate($B$28,J49,J50,"Linear","Act365F")</f>
+        <v>8.2877173512875477E-3</v>
+      </c>
+      <c r="M49" cm="1">
+        <f t="array" aca="1" ref="M49" ca="1">_xll.QCurves_GetCpiForecast($B$30,J49,-3)</f>
+        <v>227.11429758702644</v>
+      </c>
+      <c r="N49">
+        <v>227.11429758702644</v>
+      </c>
+      <c r="O49" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T49" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U49" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="J50" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>48222</v>
+      </c>
+      <c r="K50" s="1">
+        <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J50)</f>
+        <v>0.90723585329626766</v>
+      </c>
+      <c r="L50" s="1"/>
+      <c r="M50" cm="1">
+        <f t="array" aca="1" ref="M50" ca="1">_xll.QCurves_GetCpiForecast($B$30,J50,-3)</f>
+        <v>230.45129896322717</v>
+      </c>
+      <c r="N50">
+        <v>230.45129896322717</v>
+      </c>
+      <c r="O50" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T50" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U50" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="Q51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T51" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U51" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="Q52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T52" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U52" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="Q53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T53" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U53" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="Q54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T54" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U54" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="Q55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T55" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U55" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="Q56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T56" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U56" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="Q57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T57" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U57" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="Q58" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R58" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S58" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T58" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U58" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transport objects for Inflation
</commit_message>
<xml_diff>
--- a/examples/Qwack - YeildCurveExample (Frozen Data).xlsx
+++ b/examples/Qwack - YeildCurveExample (Frozen Data).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Qwack\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E644BA9-7B05-452A-BF58-122B77304237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCC0119-43EF-4E4F-8365-62A480F3A509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SelfDiscounting" sheetId="1" r:id="rId1"/>
@@ -380,9 +380,9 @@
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -525,16 +525,16 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -754,22 +754,22 @@
                   <c:v>103.08432470555357</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>104.60300530860663</c:v>
+                  <c:v>104.60300530860661</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>106.12168591165968</c:v>
+                  <c:v>106.12168591165967</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>107.81948182466114</c:v>
+                  <c:v>107.81948182466112</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>109.54101684366961</c:v>
+                  <c:v>109.5410168436696</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>111.28146982991993</c:v>
+                  <c:v>111.28146982991991</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>113.02192281617025</c:v>
+                  <c:v>113.02192281617023</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>115.19136548128431</c:v>
@@ -811,13 +811,13 @@
                   <c:v>144.3421547556126</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>147.64288437772422</c:v>
+                  <c:v>147.64288437772419</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>150.97988575392495</c:v>
+                  <c:v>150.97988575392492</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>154.31688713012568</c:v>
+                  <c:v>154.31688713012565</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>157.58134499814813</c:v>
@@ -832,16 +832,16 @@
                   <c:v>167.55607737266118</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>170.82053524068365</c:v>
+                  <c:v>170.82053524068363</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>174.12126486279524</c:v>
+                  <c:v>174.12126486279521</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>177.45826623899598</c:v>
+                  <c:v>177.45826623899595</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>180.79526761519671</c:v>
+                  <c:v>180.79526761519668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3653,7 +3653,7 @@
   <dimension ref="B1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3682,14 +3682,14 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("ZAR.JIBAR.3M","ZAR","3M","Act365F","Act365F","3M","JHB","0b","MF")</f>
-        <v>ZAR.JIBAR.3M¬0</v>
+        <v>ZAR.JIBAR.3M¬3</v>
       </c>
       <c r="I2" t="s">
         <v>25</v>
       </c>
       <c r="J2" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("USD.LIBOR.3M","USD","3M","Act360","Act360","6M","NYC","2b","MF")</f>
-        <v>USD.LIBOR.3M¬0</v>
+        <v>USD.LIBOR.3M¬3</v>
       </c>
       <c r="V2" s="3"/>
     </row>
@@ -3699,14 +3699,14 @@
       </c>
       <c r="C3" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("ZAR.OIS.1B","ZAR","3M","Act365F","Act365F","3M","JHB","0b","MF")</f>
-        <v>ZAR.OIS.1B¬0</v>
+        <v>ZAR.OIS.1B¬3</v>
       </c>
       <c r="I3" t="s">
         <v>31</v>
       </c>
       <c r="J3" t="str">
         <f ca="1">_xll.QIns_CreateRateIndex("USD.OIS.1B","USD","3M","Act360","Act360","3M","NYC","0b","MF")</f>
-        <v>USD.OIS.1B¬0</v>
+        <v>USD.OIS.1B¬3</v>
       </c>
       <c r="V3" t="s">
         <v>36</v>
@@ -3791,7 +3791,7 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B6,valDate,"0x3",index,"ZAR",E6,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_3m¬0</v>
+        <v>ZAROISFra_3m¬3</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="M6" t="str">
         <f ca="1">_xll.QIns_CreateFRA("USDOISFra_"&amp;I6,valDate,"0x3",J2,"USD",L6,1,"USD.LIBOR.3M","USD.OIS.1B",,,"USD.LIBOR.3M")</f>
-        <v>USDOISFra_3m¬0</v>
+        <v>USDOISFra_3m¬3</v>
       </c>
       <c r="O6" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P6,"F","JHB+NYC")</f>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="S6" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P6,O6,"ZAR","USD",1000000,R6,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_1w¬0</v>
+        <v>ZARFwd_1w¬3</v>
       </c>
       <c r="U6" s="2">
         <f t="shared" ref="U6:U37" ca="1" si="0">EDATE(U5,3)</f>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="Y6" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U6)</f>
-        <v>0.99397688519022931</v>
+        <v>0.9939782771219795</v>
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B7,valDate,B7,index,"ZAR",E7,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_3x6¬0</v>
+        <v>ZAROISFra_3x6¬3</v>
       </c>
       <c r="I7" t="s">
         <v>39</v>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="M7" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I7,valDate,I7,$J$2,L7,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDU8¬0</v>
+        <v>EDU8¬3</v>
       </c>
       <c r="O7" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P7,"MF","JHB+NYC")</f>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="S7" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P7,O7,"ZAR","USD",1000000,R7,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_1m¬0</v>
+        <v>ZARFwd_1m¬3</v>
       </c>
       <c r="U7" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3917,11 +3917,11 @@
       </c>
       <c r="X7" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U7)</f>
-        <v>0.9656327019227805</v>
+        <v>0.96563334955776847</v>
       </c>
       <c r="Y7" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U7)</f>
-        <v>0.99187709636447929</v>
+        <v>0.99188127093428713</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B8,valDate,B8,index,"ZAR",E8,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_6x9¬0</v>
+        <v>ZAROISFra_6x9¬3</v>
       </c>
       <c r="I8" t="s">
         <v>40</v>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="M8" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I8,valDate,I8,$J$2,L8,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDZ8¬0</v>
+        <v>EDZ8¬3</v>
       </c>
       <c r="O8" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P8,"MF","JHB+NYC")</f>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="S8" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P8,O8,"ZAR","USD",1000000,R8,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_2m¬0</v>
+        <v>ZARFwd_2m¬3</v>
       </c>
       <c r="U8" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -3988,15 +3988,15 @@
       </c>
       <c r="W8" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U8,U9,"Linear","Act365F")</f>
-        <v>5.3699999999999568E-2</v>
+        <v>5.3700000000000456E-2</v>
       </c>
       <c r="X8" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U8)</f>
-        <v>0.95508414419060306</v>
+        <v>0.95502333238934101</v>
       </c>
       <c r="Y8" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U8)</f>
-        <v>0.99041855357294528</v>
+        <v>0.99042679241991194</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B9,valDate,B9,index,"ZAR",E9,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_9x12¬0</v>
+        <v>ZAROISFra_9x12¬3</v>
       </c>
       <c r="I9" t="s">
         <v>42</v>
@@ -4033,7 +4033,7 @@
       </c>
       <c r="M9" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I9,valDate,I9,$J$2,L9,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDH9¬0</v>
+        <v>EDH9¬3</v>
       </c>
       <c r="O9" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P9,"MF","JHB+NYC")</f>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="S9" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P9,O9,"ZAR","USD",1000000,R9,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_3m¬0</v>
+        <v>ZARFwd_3m¬3</v>
       </c>
       <c r="U9" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="V9" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U9)</f>
-        <v>0.93871272155929031</v>
+        <v>0.9387127215592902</v>
       </c>
       <c r="W9" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U9,U10,"Linear","Act365F")</f>
@@ -4067,11 +4067,11 @@
       </c>
       <c r="X9" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U9)</f>
-        <v>0.94327489164363509</v>
+        <v>0.94322723052657331</v>
       </c>
       <c r="Y9" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U9)</f>
-        <v>0.98954004818296748</v>
+        <v>0.98955374742453073</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B10,valDate,B10,index,"ZAR",E10,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_12x15¬0</v>
+        <v>ZAROISFra_12x15¬3</v>
       </c>
       <c r="I10" t="s">
         <v>41</v>
@@ -4108,7 +4108,7 @@
       </c>
       <c r="M10" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I10,valDate,I10,$J$2,L10,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDM9¬0</v>
+        <v>EDM9¬3</v>
       </c>
       <c r="O10" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P10,"MF","JHB+NYC")</f>
@@ -4126,7 +4126,7 @@
       </c>
       <c r="S10" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P10,O10,"ZAR","USD",1000000,R10,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_6m¬0</v>
+        <v>ZARFwd_6m¬3</v>
       </c>
       <c r="U10" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4134,19 +4134,19 @@
       </c>
       <c r="V10" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U10)</f>
-        <v>0.92560750704156458</v>
+        <v>0.92560750704156447</v>
       </c>
       <c r="W10" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U10,U11,"Linear","Act365F")</f>
-        <v>6.0714308999312856E-2</v>
+        <v>6.0390129186780286E-2</v>
       </c>
       <c r="X10" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U10)</f>
-        <v>0.9311124050637537</v>
+        <v>0.9310886947492667</v>
       </c>
       <c r="Y10" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U10)</f>
-        <v>0.98925973228493413</v>
+        <v>0.98928033925064329</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -4165,7 +4165,7 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">_xll.QIns_CreateFRA("ZAROISFra_"&amp;B11,valDate,B11,index,"ZAR",E11,1,"ZAR.JIBAR.3M","ZAR.OIS.1B",,,"ZAR.JIBAR.3M")</f>
-        <v>ZAROISFra_15x18¬0</v>
+        <v>ZAROISFra_15x18¬3</v>
       </c>
       <c r="I11" t="s">
         <v>43</v>
@@ -4183,7 +4183,7 @@
       </c>
       <c r="M11" t="str">
         <f ca="1">_xll.QIns_CreateSTIRFromCode(I11,valDate,I11,$J$2,L11,1,0,"USD.LIBOR.3M","USD.LIBOR.3M")</f>
-        <v>EDU9¬0</v>
+        <v>EDU9¬3</v>
       </c>
       <c r="O11" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P11,"MF","JHB+NYC")</f>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="S11" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P11,O11,"ZAR","USD",1000000,R11,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_9m¬0</v>
+        <v>ZARFwd_9m¬3</v>
       </c>
       <c r="U11" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4209,19 +4209,19 @@
       </c>
       <c r="V11" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U11)</f>
-        <v>0.91165612999514489</v>
+        <v>0.91172950550426635</v>
       </c>
       <c r="W11" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U11,U12,"Linear","Act365F")</f>
-        <v>6.3305511654691615E-2</v>
+        <v>6.2880802889422938E-2</v>
       </c>
       <c r="X11" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U11)</f>
-        <v>0.91799187684709571</v>
+        <v>0.91804261250887176</v>
       </c>
       <c r="Y11" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U11)</f>
-        <v>0.9895900670759552</v>
+        <v>0.98961898828383377</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -4240,7 +4240,7 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B12,valDate,B12,index,E12,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_2y¬0</v>
+        <v>ZAROISSwap_2y¬3</v>
       </c>
       <c r="I12" t="s">
         <v>12</v>
@@ -4256,8 +4256,8 @@
         <v>4.6769999999999997E-3</v>
       </c>
       <c r="M12" t="str">
-        <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I12,valDate,I12,$J$2,L12,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_2y¬0</v>
+        <f ca="1">_xll.QIns_CreateIRS("USDSwap_"&amp;I12,valDate,I12,$J$2,L12,1000000,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
+        <v>USDSwap_2y¬3</v>
       </c>
       <c r="O12" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P12,"MF","JHB+NYC")</f>
@@ -4275,7 +4275,7 @@
       </c>
       <c r="S12" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P12,O12,"ZAR","USD",1000000,R12,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_12m¬0</v>
+        <v>ZARFwd_12m¬3</v>
       </c>
       <c r="U12" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4283,19 +4283,19 @@
       </c>
       <c r="V12" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U12)</f>
-        <v>0.89764428137467944</v>
+        <v>0.89780910505749789</v>
       </c>
       <c r="W12" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U12,U13,"Linear","Act365F")</f>
-        <v>6.6022872672555147E-2</v>
+        <v>6.5944876986154352E-2</v>
       </c>
       <c r="X12" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U12)</f>
-        <v>0.90476115186497996</v>
+        <v>0.90490500036226329</v>
       </c>
       <c r="Y12" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U12)</f>
-        <v>0.99050468498643585</v>
+        <v>0.9905431168206783</v>
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B13,valDate,B13,index,E13,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_3y¬0</v>
+        <v>ZAROISSwap_3y¬3</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -4330,8 +4330,8 @@
         <v>4.7160000000000006E-3</v>
       </c>
       <c r="M13" t="str">
-        <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I13,valDate,I13,$J$2,L13,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_3y¬0</v>
+        <f ca="1">_xll.QIns_CreateIRS("USDSwap_"&amp;I13,valDate,I13,$J$2,L13,1000000,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
+        <v>USDSwap_3y¬1</v>
       </c>
       <c r="O13" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P13,"MF","JHB+NYC")</f>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="S13" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P13,O13,"ZAR","USD",1000000,R13,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_15m¬0</v>
+        <v>ZARFwd_15m¬3</v>
       </c>
       <c r="U13" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4357,19 +4357,19 @@
       </c>
       <c r="V13" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U13)</f>
-        <v>0.88310788663618245</v>
+        <v>0.88328693898443689</v>
       </c>
       <c r="W13" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U13,U14,"Linear","Act365F")</f>
-        <v>6.8638838016895798E-2</v>
+        <v>6.8575221920884222E-2</v>
       </c>
       <c r="X13" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U13)</f>
-        <v>0.89061526662429957</v>
+        <v>0.89077018584097667</v>
       </c>
       <c r="Y13" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U13)</f>
-        <v>0.98936595621968537</v>
+        <v>0.98940202322815007</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B14,valDate,B14,index,E14,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_4y¬0</v>
+        <v>ZAROISSwap_4y¬3</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
@@ -4404,8 +4404,8 @@
         <v>5.1839999999999994E-3</v>
       </c>
       <c r="M14" t="str">
-        <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I14,valDate,I14,$J$2,L14,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_4y¬0</v>
+        <f ca="1">_xll.QIns_CreateIRS("USDSwap_"&amp;I14,valDate,I14,$J$2,L14,1000000,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
+        <v>USDSwap_4y¬1</v>
       </c>
       <c r="O14" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P14,"MF","JHB+NYC")</f>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="S14" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P14,O14,"ZAR","USD",1000000,R14,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_18m¬0</v>
+        <v>ZARFwd_18m¬3</v>
       </c>
       <c r="U14" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4431,19 +4431,19 @@
       </c>
       <c r="V14" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U14)</f>
-        <v>0.86808929236306109</v>
+        <v>0.8682789855075097</v>
       </c>
       <c r="W14" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U14,U15,"Linear","Act365F")</f>
-        <v>7.126129505508913E-2</v>
+        <v>7.1203298914752119E-2</v>
       </c>
       <c r="X14" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U14)</f>
-        <v>0.87588056205160736</v>
+        <v>0.87604267910963551</v>
       </c>
       <c r="Y14" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U14)</f>
-        <v>0.98815770009348602</v>
+        <v>0.98818944595200109</v>
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
@@ -4462,7 +4462,7 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B15,valDate,B15,index,E15,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_5y¬0</v>
+        <v>ZAROISSwap_5y¬3</v>
       </c>
       <c r="I15" t="s">
         <v>15</v>
@@ -4478,8 +4478,8 @@
         <v>5.7820000000000007E-3</v>
       </c>
       <c r="M15" t="str">
-        <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I15,valDate,I15,$J$2,L15,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_5y¬0</v>
+        <f ca="1">_xll.QIns_CreateIRS("USDSwap_"&amp;I15,valDate,I15,$J$2,L15,1000000,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
+        <v>USDSwap_5y¬1</v>
       </c>
       <c r="O15" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P15,"MF","JHB+NYC")</f>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="S15" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P15,O15,"ZAR","USD",1000000,R15,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_2y¬0</v>
+        <v>ZARFwd_2y¬3</v>
       </c>
       <c r="U15" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4505,19 +4505,19 @@
       </c>
       <c r="V15" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U15)</f>
-        <v>0.85277201372255773</v>
+        <v>0.85297060865370422</v>
       </c>
       <c r="W15" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U15,U16,"Linear","Act365F")</f>
-        <v>7.3842072502186704E-2</v>
+        <v>7.3789663461394345E-2</v>
       </c>
       <c r="X15" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U15)</f>
-        <v>0.86074727431237563</v>
+        <v>0.86091473422367226</v>
       </c>
       <c r="Y15" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U15)</f>
-        <v>0.98694615116806661</v>
+        <v>0.98697191281199692</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B16,valDate,B16,index,E16,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_7y¬0</v>
+        <v>ZAROISSwap_7y¬3</v>
       </c>
       <c r="I16" t="s">
         <v>16</v>
@@ -4552,8 +4552,8 @@
         <v>6.927E-3</v>
       </c>
       <c r="M16" t="str">
-        <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I16,valDate,I16,$J$2,L16,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_7y¬0</v>
+        <f ca="1">_xll.QIns_CreateIRS("USDSwap_"&amp;I16,valDate,I16,$J$2,L16,1000000,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
+        <v>USDSwap_7y¬1</v>
       </c>
       <c r="O16" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P16,"MF","JHB+NYC")</f>
@@ -4571,7 +4571,7 @@
       </c>
       <c r="S16" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P16,O16,"ZAR","USD",1000000,R16,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_3y¬0</v>
+        <v>ZARFwd_3y¬3</v>
       </c>
       <c r="U16" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4579,19 +4579,19 @@
       </c>
       <c r="V16" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U16)</f>
-        <v>0.83752270655066519</v>
+        <v>0.8377283823885916</v>
       </c>
       <c r="W16" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U16,U17,"Linear","Act365F")</f>
-        <v>7.857175418754106E-2</v>
+        <v>7.865262674858732E-2</v>
       </c>
       <c r="X16" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U16)</f>
-        <v>0.84558539907893437</v>
+        <v>0.84575635889675416</v>
       </c>
       <c r="Y16" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U16)</f>
-        <v>0.98575776917644486</v>
+        <v>0.98577607347647955</v>
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="F17" t="str">
         <f ca="1">_xll.QIns_CreateIRS("ZAROISSwap_"&amp;B17,valDate,B17,index,E17,1,"ZAR.JIBAR.3M","ZAR.OIS.1B","Pay","ZAR.JIBAR.3M")</f>
-        <v>ZAROISSwap_10y¬0</v>
+        <v>ZAROISSwap_10y¬3</v>
       </c>
       <c r="I17" t="s">
         <v>17</v>
@@ -4626,8 +4626,8 @@
         <v>8.1550000000000008E-3</v>
       </c>
       <c r="M17" t="str">
-        <f ca="1">_xll.QIns_CreateIRS("USDOISSwap_"&amp;I17,valDate,I17,$J$2,L17,1,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
-        <v>USDOISSwap_10y¬0</v>
+        <f ca="1">_xll.QIns_CreateIRS("USDSwap_"&amp;I17,valDate,I17,$J$2,L17,1000000,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
+        <v>USDSwap_10y¬1</v>
       </c>
       <c r="O17" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P17,"MF","JHB+NYC")</f>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="S17" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P17,O17,"ZAR","USD",1000000,R17,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_4y¬0</v>
+        <v>ZARFwd_4y¬3</v>
       </c>
       <c r="U17" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4653,19 +4653,19 @@
       </c>
       <c r="V17" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U17)</f>
-        <v>0.82143158283245765</v>
+        <v>0.82161705929154938</v>
       </c>
       <c r="W17" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U17,U18,"Linear","Act365F")</f>
-        <v>8.1577207989190395E-2</v>
+        <v>8.1686634800363755E-2</v>
       </c>
       <c r="X17" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U17)</f>
-        <v>0.82992395098678051</v>
+        <v>0.8300967860738232</v>
       </c>
       <c r="Y17" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U17)</f>
-        <v>0.98420963731310829</v>
+        <v>0.98422717366878043</v>
       </c>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
@@ -4677,7 +4677,7 @@
       </c>
       <c r="F18" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B18,valDate,B18,oisIndex,index,E18,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_3m¬0</v>
+        <v>ZAROISBasis_3m¬3</v>
       </c>
       <c r="I18" t="s">
         <v>0</v>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="M18" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I18,valDate,I18,$J$3,$J$2,L18,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_3m¬0</v>
+        <v>USDOISBasis_3m¬3</v>
       </c>
       <c r="O18" s="2">
         <f ca="1">_xll.QDates_AddPeriod($R$5,P18,"MF","JHB+NYC")</f>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="S18" s="5" t="str">
         <f ca="1">_xll.QIns_CreateFxForward("ZARFwd_"&amp;P18,O18,"ZAR","USD",1000000,R18,"ZAR.DISC.[USD.OIS.1B]","ZAR.DISC.[USD.OIS.1B]")</f>
-        <v>ZARFwd_5y¬0</v>
+        <v>ZARFwd_5y¬3</v>
       </c>
       <c r="U18" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4713,19 +4713,19 @@
       </c>
       <c r="V18" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U18)</f>
-        <v>0.80488166527260585</v>
+        <v>0.80504164788264565</v>
       </c>
       <c r="W18" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U18,U19,"Linear","Act365F")</f>
-        <v>8.4548149616066187E-2</v>
+        <v>8.4683640526620002E-2</v>
       </c>
       <c r="X18" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U18)</f>
-        <v>0.81378124182284473</v>
+        <v>0.81395435108703718</v>
       </c>
       <c r="Y18" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U18)</f>
-        <v>0.98258462547215442</v>
+        <v>0.98260113641887803</v>
       </c>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
@@ -4737,7 +4737,7 @@
       </c>
       <c r="F19" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B19,valDate,B19,oisIndex,index,E19,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_6m¬0</v>
+        <v>ZAROISBasis_6m¬3</v>
       </c>
       <c r="I19" t="s">
         <v>32</v>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="M19" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I19,valDate,I19,$J$3,$J$2,L19,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_6m¬0</v>
+        <v>USDOISBasis_6m¬3</v>
       </c>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
@@ -4757,19 +4757,19 @@
       </c>
       <c r="V19" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U19)</f>
-        <v>0.78808692876880038</v>
+        <v>0.78821721633937258</v>
       </c>
       <c r="W19" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U19,U20,"Linear","Act365F")</f>
-        <v>8.7494694879952345E-2</v>
+        <v>8.7656107965939062E-2</v>
       </c>
       <c r="X19" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U19)</f>
-        <v>0.79735746824190035</v>
+        <v>0.79752930457893967</v>
       </c>
       <c r="Y19" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U19)</f>
-        <v>0.98090329240969876</v>
+        <v>0.98091844194025224</v>
       </c>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="F20" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B20,valDate,B20,oisIndex,index,E20,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_9m¬0</v>
+        <v>ZAROISBasis_9m¬3</v>
       </c>
       <c r="I20" t="s">
         <v>33</v>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="M20" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I20,valDate,I20,$J$3,$J$2,L20,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_9m¬0</v>
+        <v>USDOISBasis_9m¬3</v>
       </c>
       <c r="U20" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4799,19 +4799,19 @@
       </c>
       <c r="V20" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U20)</f>
-        <v>0.77126279810975573</v>
+        <v>0.77135992535398656</v>
       </c>
       <c r="W20" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U20,U21,"Linear","Act365F")</f>
-        <v>9.4941632972784462E-2</v>
+        <v>9.4832662664627754E-2</v>
       </c>
       <c r="X20" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U20)</f>
-        <v>0.78086504341135521</v>
+        <v>0.7810341839908691</v>
       </c>
       <c r="Y20" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U20)</f>
-        <v>0.97918512096307153</v>
+        <v>0.97919859526263953</v>
       </c>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
@@ -4823,7 +4823,7 @@
       </c>
       <c r="F21" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B21,valDate,B21,oisIndex,index,E21,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_1y¬0</v>
+        <v>ZAROISBasis_1y¬3</v>
       </c>
       <c r="I21" t="s">
         <v>34</v>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="M21" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I21,valDate,I21,$J$3,$J$2,L21,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_1y¬0</v>
+        <v>USDOISBasis_1y¬3</v>
       </c>
       <c r="U21" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4841,19 +4841,19 @@
       </c>
       <c r="V21" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U21)</f>
-        <v>0.75342885110644131</v>
+        <v>0.75354373132308183</v>
       </c>
       <c r="W21" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U21,U22,"Linear","Act365F")</f>
-        <v>9.8450448476763722E-2</v>
+        <v>9.8332294651314087E-2</v>
       </c>
       <c r="X21" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U21)</f>
-        <v>0.76415580420091456</v>
+        <v>0.76432090740954051</v>
       </c>
       <c r="Y21" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U21)</f>
-        <v>0.97727287478823477</v>
+        <v>0.97728822179602359</v>
       </c>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="F22" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B22,valDate,B22,oisIndex,index,E22,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_18m¬0</v>
+        <v>ZAROISBasis_18m¬3</v>
       </c>
       <c r="I22" t="s">
         <v>35</v>
@@ -4875,7 +4875,7 @@
       </c>
       <c r="M22" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I22,valDate,I22,$J$3,$J$2,L22,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_18m¬0</v>
+        <v>USDOISBasis_18m¬3</v>
       </c>
       <c r="U22" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4883,19 +4883,19 @@
       </c>
       <c r="V22" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U22)</f>
-        <v>0.73518529594711146</v>
+        <v>0.73531876289695641</v>
       </c>
       <c r="W22" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U22,U23,"Linear","Act365F")</f>
-        <v>0.10196915259017414</v>
+        <v>0.10184177743101935</v>
       </c>
       <c r="X22" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U22)</f>
-        <v>0.74707188897943855</v>
+        <v>0.7472316374930501</v>
       </c>
       <c r="Y22" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U22)</f>
-        <v>0.97526846197147277</v>
+        <v>0.97528581972614004</v>
       </c>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
@@ -4907,7 +4907,7 @@
       </c>
       <c r="F23" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B23,valDate,B23,oisIndex,index,E23,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_2y¬0</v>
+        <v>ZAROISBasis_2y¬3</v>
       </c>
       <c r="I23" t="s">
         <v>12</v>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="M23" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I23,valDate,I23,$J$3,$J$2,L23,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_2y¬0</v>
+        <v>USDOISBasis_2y¬3</v>
       </c>
       <c r="U23" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4925,19 +4925,19 @@
       </c>
       <c r="V23" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U23)</f>
-        <v>0.71676318209954837</v>
+        <v>0.71691574486215071</v>
       </c>
       <c r="W23" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U23,U24,"Linear","Act365F")</f>
-        <v>0.10542241134319731</v>
+        <v>0.10528597726554249</v>
       </c>
       <c r="X23" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U23)</f>
-        <v>0.72982525635703765</v>
+        <v>0.72997846365860708</v>
       </c>
       <c r="Y23" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U23)</f>
-        <v>0.97319296193923055</v>
+        <v>0.97321244732404855</v>
       </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="F24" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B24,valDate,B24,oisIndex,index,E24,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_5y¬0</v>
+        <v>ZAROISBasis_5y¬3</v>
       </c>
       <c r="I24" t="s">
         <v>15</v>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="M24" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I24,valDate,I24,$J$3,$J$2,L24,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_5y¬0</v>
+        <v>USDOISBasis_5y¬3</v>
       </c>
       <c r="U24" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -4967,19 +4967,19 @@
       </c>
       <c r="V24" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U24)</f>
-        <v>0.69860329189583359</v>
+        <v>0.69877490142472021</v>
       </c>
       <c r="W24" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U24,U25,"Linear","Act365F")</f>
-        <v>0.10491977430031936</v>
+        <v>0.10510287105152567</v>
       </c>
       <c r="X24" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U24)</f>
-        <v>0.7128241353515089</v>
+        <v>0.71296988674522044</v>
       </c>
       <c r="Y24" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U24)</f>
-        <v>0.97109424852837223</v>
+        <v>0.97111592716689865</v>
       </c>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="F25" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("ZAROISBasis_"&amp;B25,valDate,B25,oisIndex,index,E25,TRUE,1,"ZAR.OIS.1B","ZAR.JIBAR.3M","ZAR.OIS.1B","ZAR.OIS.1B")</f>
-        <v>ZAROISBasis_10y¬0</v>
+        <v>ZAROISBasis_10y¬3</v>
       </c>
       <c r="I25" t="s">
         <v>17</v>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="M25" t="str">
         <f ca="1">_xll.QIns_CreateIRBasisSwap("USDOISBasis_"&amp;I25,valDate,I25,$J$3,$J$2,L25,TRUE,1,"USD.OIS.1B","USD.LIBOR.3M","USD.OIS.1B","USD.OIS.1B")</f>
-        <v>USDOISBasis_10y¬0</v>
+        <v>USDOISBasis_10y¬3</v>
       </c>
       <c r="U25" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5009,19 +5009,19 @@
       </c>
       <c r="V25" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U25)</f>
-        <v>0.68079500130077886</v>
+        <v>0.68093194493511044</v>
       </c>
       <c r="W25" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U25,U26,"Linear","Act365F")</f>
-        <v>0.1080593266864182</v>
+        <v>0.10826492821737227</v>
       </c>
       <c r="X25" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U25)</f>
-        <v>0.69644975390208053</v>
+        <v>0.69658949782740331</v>
       </c>
       <c r="Y25" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U25)</f>
-        <v>0.9689422053326282</v>
+        <v>0.96895696385680063</v>
       </c>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
@@ -5031,19 +5031,19 @@
       </c>
       <c r="V26" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U26)</f>
-        <v>0.66274393011570798</v>
+        <v>0.66284380306723867</v>
       </c>
       <c r="W26" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U26,U27,"Linear","Act365F")</f>
-        <v>0.11120341922427235</v>
+        <v>0.11143163097328238</v>
       </c>
       <c r="X26" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U26)</f>
-        <v>0.67985976179011709</v>
+        <v>0.67999263313482983</v>
       </c>
       <c r="Y26" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U26)</f>
-        <v>0.96670075236166508</v>
+        <v>0.96670777979465861</v>
       </c>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
@@ -5052,7 +5052,7 @@
       </c>
       <c r="C27" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_ZAR",F6:F25)</f>
-        <v>FundingInstruments_ZAR¬0</v>
+        <v>FundingInstruments_ZAR¬3</v>
       </c>
       <c r="G27" t="s">
         <v>53</v>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="J27" t="str">
         <f ca="1">_xll.QIns_CreateFxPair("USDZAR","ZAR","USD","NYC+JHB","2b")</f>
-        <v>USDZAR¬0</v>
+        <v>USDZAR¬3</v>
       </c>
       <c r="L27" t="s">
         <v>63</v>
@@ -5077,19 +5077,19 @@
       </c>
       <c r="V27" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U27)</f>
-        <v>0.64467413007574426</v>
+        <v>0.64473520477122048</v>
       </c>
       <c r="W27" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U27,U28,"Linear","Act365F")</f>
-        <v>0.11428026635733614</v>
+        <v>0.11453072200221853</v>
       </c>
       <c r="X27" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U27)</f>
-        <v>0.66325493574990402</v>
+        <v>0.66338020301094713</v>
       </c>
       <c r="Y27" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U27)</f>
-        <v>0.96439365916425557</v>
+        <v>0.96439222348453846</v>
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
@@ -5098,7 +5098,7 @@
       </c>
       <c r="C28" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_USD",M6:M25)</f>
-        <v>FundingInstruments_USD¬0</v>
+        <v>FundingInstruments_USD¬4</v>
       </c>
       <c r="G28" t="s">
         <v>54</v>
@@ -5108,7 +5108,7 @@
       </c>
       <c r="J28" t="str">
         <f ca="1">_xll.QIns_CreateFxMatrix("fxMatrix","USD",valDate,L27:M27,J27,L29:M30)</f>
-        <v>fxMatrix¬0</v>
+        <v>fxMatrix¬3</v>
       </c>
       <c r="U28" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5116,19 +5116,19 @@
       </c>
       <c r="V28" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U28)</f>
-        <v>0.62700592095547669</v>
+        <v>0.62702766022949408</v>
       </c>
       <c r="W28" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U28,U29,"Linear","Act365F")</f>
-        <v>0.11739458242899767</v>
+        <v>0.11766741594568447</v>
       </c>
       <c r="X28" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U28)</f>
-        <v>0.64701654978952006</v>
+        <v>0.6471337393882084</v>
       </c>
       <c r="Y28" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U28)</f>
-        <v>0.96207368039716601</v>
+        <v>0.96206326422356037</v>
       </c>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
@@ -5137,7 +5137,7 @@
       </c>
       <c r="C29" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstruments_XCY",S6:S18)</f>
-        <v>FundingInstruments_XCY¬0</v>
+        <v>FundingInstruments_XCY¬3</v>
       </c>
       <c r="G29" t="s">
         <v>55</v>
@@ -5157,19 +5157,19 @@
       </c>
       <c r="V29" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U29)</f>
-        <v>0.60917640085263758</v>
+        <v>0.60915726442122597</v>
       </c>
       <c r="W29" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U29,U30,"Linear","Act365F")</f>
-        <v>0.12054745722348974</v>
+        <v>0.12084296785545989</v>
       </c>
       <c r="X29" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U29)</f>
-        <v>0.63062259340956817</v>
+        <v>0.6307310415303149</v>
       </c>
       <c r="Y29" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U29)</f>
-        <v>0.95966502305936319</v>
+        <v>0.95964482860679623</v>
       </c>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
@@ -5178,7 +5178,7 @@
       </c>
       <c r="C30" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection("FundingInstrumentsComplex",C27:C29)</f>
-        <v>FundingInstrumentsComplex¬0</v>
+        <v>FundingInstrumentsComplex¬3</v>
       </c>
       <c r="G30" t="s">
         <v>56</v>
@@ -5198,19 +5198,19 @@
       </c>
       <c r="V30" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U30)</f>
-        <v>0.59121266156826624</v>
+        <v>0.59115135604560298</v>
       </c>
       <c r="W30" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U30,U31,"Linear","Act365F")</f>
-        <v>0.12370118399362764</v>
+        <v>0.1240194434946833</v>
       </c>
       <c r="X30" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U30)</f>
-        <v>0.61409313718099956</v>
+        <v>0.61419222990008104</v>
       </c>
       <c r="Y30" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U30)</f>
-        <v>0.95716611447307476</v>
+        <v>0.95713532851836425</v>
       </c>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
@@ -5226,19 +5226,19 @@
       </c>
       <c r="V31" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U31)</f>
-        <v>0.57333633478356749</v>
+        <v>0.57323228931866455</v>
       </c>
       <c r="W31" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U31,U32,"Linear","Act365F")</f>
-        <v>0.12677943077668374</v>
+        <v>0.12711999300751539</v>
       </c>
       <c r="X31" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U31)</f>
-        <v>0.59762748966727686</v>
+        <v>0.59771677487976194</v>
       </c>
       <c r="Y31" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U31)</f>
-        <v>0.95460360649813214</v>
+        <v>0.95456152749551193</v>
       </c>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
@@ -5247,7 +5247,7 @@
       </c>
       <c r="C32" t="str">
         <f ca="1">_xll.QCurves_CreateFundingModel("ModelComplex",valDate,C30,G27:H31,J28)</f>
-        <v>ModelComplex¬0</v>
+        <v>ModelComplex¬12</v>
       </c>
       <c r="U32" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5255,19 +5255,19 @@
       </c>
       <c r="V32" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U32)</f>
-        <v>0.55595674792479344</v>
+        <v>0.55581059744612504</v>
       </c>
       <c r="W32" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U32,U33,"Linear","Act365F")</f>
-        <v>0.11324381779953492</v>
+        <v>0.11317255021449089</v>
       </c>
       <c r="X32" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U32)</f>
-        <v>0.58159917600275446</v>
+        <v>0.58167849418104156</v>
       </c>
       <c r="Y32" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U32)</f>
-        <v>0.95203578923972831</v>
+        <v>0.9519819919124336</v>
       </c>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
       </c>
       <c r="D33" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C33,"curve.complex."&amp;C33)</f>
-        <v>curve.complex.ZAR.JIBAR.3M¬0</v>
+        <v>curve.complex.ZAR.JIBAR.3M¬3</v>
       </c>
       <c r="U33" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5288,19 +5288,19 @@
       </c>
       <c r="V33" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U33)</f>
-        <v>0.54069120223907352</v>
+        <v>0.54055840574225256</v>
       </c>
       <c r="W33" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U33,U34,"Linear","Act365F")</f>
-        <v>0.11524144192979881</v>
+        <v>0.1151625160290714</v>
       </c>
       <c r="X33" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U33)</f>
-        <v>0.56548965287335351</v>
+        <v>0.56555858172537254</v>
       </c>
       <c r="Y33" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U33)</f>
-        <v>0.94925613949209153</v>
+        <v>0.94920195317394584</v>
       </c>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="D34" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C34,"curve.complex."&amp;C34)</f>
-        <v>curve.complex.ZAR.OIS.1B¬0</v>
+        <v>curve.complex.ZAR.OIS.1B¬3</v>
       </c>
       <c r="U34" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5321,19 +5321,19 @@
       </c>
       <c r="V34" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U34)</f>
-        <v>0.5254289835539373</v>
+        <v>0.5253100908871664</v>
       </c>
       <c r="W34" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U34,U35,"Linear","Act365F")</f>
-        <v>0.11723344966439958</v>
+        <v>0.11714683807864844</v>
       </c>
       <c r="X34" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U34)</f>
-        <v>0.54931891008299771</v>
+        <v>0.54937707981928041</v>
       </c>
       <c r="Y34" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U34)</f>
-        <v>0.94637653450372528</v>
+        <v>0.94632205719360685</v>
       </c>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
@@ -5346,7 +5346,11 @@
       </c>
       <c r="D35" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C35,"curve.complex."&amp;C35)</f>
-        <v>curve.complex.USD.LIBOR.3M¬0</v>
+        <v>curve.complex.USD.LIBOR.3M¬3</v>
+      </c>
+      <c r="M35" t="str">
+        <f ca="1">_xll.QIns_CreateIRS("USDSwap_X",valDate,"6y",$J$2,L14,1000000,"USD.LIBOR.3M","USD.OIS.1B","Pay","USD.LIBOR.3M")</f>
+        <v>USDSwap_X¬0</v>
       </c>
       <c r="U35" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5354,19 +5358,19 @@
       </c>
       <c r="V35" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U35)</f>
-        <v>0.51034856466474043</v>
+        <v>0.51024390371681438</v>
       </c>
       <c r="W35" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U35,U36,"Linear","Act365F")</f>
-        <v>0.11919632052293011</v>
+        <v>0.11910208793379656</v>
       </c>
       <c r="X35" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U35)</f>
-        <v>0.53328091430168234</v>
+        <v>0.53332812950621078</v>
       </c>
       <c r="Y35" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U35)</f>
-        <v>0.94342782428126781</v>
+        <v>0.94337315800310673</v>
       </c>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
@@ -5379,7 +5383,7 @@
       </c>
       <c r="D36" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C36,"curve.complex."&amp;C36)</f>
-        <v>curve.complex.USD.OIS.1B¬0</v>
+        <v>curve.complex.USD.OIS.1B¬3</v>
       </c>
       <c r="U36" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5387,19 +5391,19 @@
       </c>
       <c r="V36" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$33,valDate,U36)</f>
-        <v>0.49562000741863571</v>
+        <v>0.49552967276340659</v>
       </c>
       <c r="W36" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($D$33,U36,U37,"Linear","Act365F")</f>
-        <v>0.12116794901357843</v>
+        <v>0.12106610256586189</v>
       </c>
       <c r="X36" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$34,valDate,U36)</f>
-        <v>0.51756317891717318</v>
+        <v>0.51759942485096522</v>
       </c>
       <c r="Y36" s="1">
         <f ca="1">_xll.QCurves_GetDF($D$35,valDate,U36)</f>
-        <v>0.94044386983374129</v>
+        <v>0.94038911616997289</v>
       </c>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
@@ -5412,7 +5416,7 @@
       </c>
       <c r="D37" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($C$32,C37,"curve.complex."&amp;C37)</f>
-        <v>curve.complex.ZAR.DISC.[USD.OIS.1B]¬0</v>
+        <v>curve.complex.ZAR.DISC.[USD.OIS.1B]¬3</v>
       </c>
       <c r="U37" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -5433,10 +5437,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8176C107-E78D-42F6-9C95-7C92D15AD2A8}">
-  <dimension ref="A1:Y58"/>
+  <dimension ref="A1:AE57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U30" sqref="Q30:U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5455,14 +5459,16 @@
     <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" customWidth="1"/>
-    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.42578125" customWidth="1"/>
-    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -5476,10 +5482,10 @@
         <f ca="1">valDate</f>
         <v>43930</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="21"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -5487,7 +5493,7 @@
       </c>
       <c r="B2" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_xll.QIns_CreateInflationIndex(B3,B4,"Linear",B6,B7,"1y","USD",B5,"P")</f>
-        <v>USD.CPI¬79</v>
+        <v>USD.CPI¬19</v>
       </c>
       <c r="E2" s="2">
         <f ca="1">EDATE(E1,-3)</f>
@@ -5540,7 +5546,7 @@
       <c r="N3">
         <v>100.6</v>
       </c>
-      <c r="O3" s="26">
+      <c r="O3" s="25">
         <f ca="1">M3-N3</f>
         <v>0</v>
       </c>
@@ -5566,7 +5572,7 @@
       </c>
       <c r="L4" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J4,J5,"Linear","Act365F")</f>
-        <v>1.0853461188319216E-2</v>
+        <v>1.084789019614822E-2</v>
       </c>
       <c r="M4" cm="1">
         <f t="array" aca="1" ref="M4" ca="1">_xll.QCurves_GetCpiForecast($B$30,J4,-3)</f>
@@ -5575,7 +5581,7 @@
       <c r="N4">
         <v>101.84216235277678</v>
       </c>
-      <c r="O4" s="26">
+      <c r="O4" s="25">
         <f t="shared" ref="O4:O35" ca="1" si="0">M4-N4</f>
         <v>0</v>
       </c>
@@ -5594,11 +5600,11 @@
       </c>
       <c r="K5" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J5)</f>
-        <v>0.99397688519022931</v>
+        <v>0.9939782771219795</v>
       </c>
       <c r="L5" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J5,J6,"Linear","Act365F")</f>
-        <v>8.3989074440587643E-3</v>
+        <v>8.3877419183225159E-3</v>
       </c>
       <c r="M5" cm="1">
         <f t="array" aca="1" ref="M5" ca="1">_xll.QCurves_GetCpiForecast($B$30,J5,-3)</f>
@@ -5607,7 +5613,7 @@
       <c r="N5">
         <v>103.08432470555357</v>
       </c>
-      <c r="O5" s="26">
+      <c r="O5" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -5625,20 +5631,20 @@
       </c>
       <c r="K6" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J6)</f>
-        <v>0.99187709636447929</v>
+        <v>0.99188127093428713</v>
       </c>
       <c r="L6" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J6,J7,"Linear","Act365F")</f>
-        <v>5.9724257990548448E-3</v>
+        <v>5.9557338962919299E-3</v>
       </c>
       <c r="M6" cm="1">
         <f t="array" aca="1" ref="M6" ca="1">_xll.QCurves_GetCpiForecast($B$30,J6,-3)</f>
-        <v>104.60300530860663</v>
+        <v>104.60300530860661</v>
       </c>
       <c r="N6">
         <v>104.60300530860663</v>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -5654,29 +5660,29 @@
         <f ca="1">M7/M3-1</f>
         <v>5.488753391311807E-2</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="22">
         <f t="shared" ca="1" si="1"/>
         <v>44295</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="23">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J7)</f>
-        <v>0.99041855357294528</v>
-      </c>
-      <c r="L7" s="24">
+        <v>0.99042679241991194</v>
+      </c>
+      <c r="L7" s="23">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J7,J8,"Linear","Act365F")</f>
-        <v>3.5609225435252819E-3</v>
-      </c>
-      <c r="M7" s="25" cm="1">
+        <v>3.5387404592084897E-3</v>
+      </c>
+      <c r="M7" s="24" cm="1">
         <f t="array" aca="1" ref="M7" ca="1">_xll.QCurves_GetCpiForecast($B$30,J7,-3)</f>
-        <v>106.12168591165968</v>
+        <v>106.12168591165967</v>
       </c>
       <c r="N7">
         <v>106.12168591165968</v>
       </c>
-      <c r="O7" s="26">
+      <c r="O7" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -5688,20 +5694,20 @@
       </c>
       <c r="K8" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J8)</f>
-        <v>0.98954004818296748</v>
+        <v>0.98955374742453073</v>
       </c>
       <c r="L8" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J8,J9,"Linear","Act365F")</f>
-        <v>1.1241970334315312E-3</v>
+        <v>1.0964710088553679E-3</v>
       </c>
       <c r="M8" cm="1">
         <f t="array" aca="1" ref="M8" ca="1">_xll.QCurves_GetCpiForecast($B$30,J8,-3)</f>
-        <v>107.81948182466114</v>
+        <v>107.81948182466112</v>
       </c>
       <c r="N8">
         <v>107.81948182466114</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -5713,20 +5719,20 @@
       </c>
       <c r="K9" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J9)</f>
-        <v>0.98925973228493413</v>
+        <v>0.98928033925064329</v>
       </c>
       <c r="L9" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J9,J10,"Linear","Act365F")</f>
-        <v>-1.3243538117687285E-3</v>
+        <v>-1.3576469786977421E-3</v>
       </c>
       <c r="M9" cm="1">
         <f t="array" aca="1" ref="M9" ca="1">_xll.QCurves_GetCpiForecast($B$30,J9,-3)</f>
-        <v>109.54101684366961</v>
+        <v>109.5410168436696</v>
       </c>
       <c r="N9">
         <v>109.54101684366961</v>
       </c>
-      <c r="O9" s="26">
+      <c r="O9" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -5740,7 +5746,7 @@
       </c>
       <c r="F10" t="str" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">_xll.QCurves_CreateFixingDictionary(E10,"USD.CPI",E12:F14)</f>
-        <v>CPI Fixings¬78</v>
+        <v>CPI Fixings¬19</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -5748,20 +5754,20 @@
       </c>
       <c r="K10" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J10)</f>
-        <v>0.9895900670759552</v>
+        <v>0.98961898828383377</v>
       </c>
       <c r="L10" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J10,J11,"Linear","Act365F")</f>
-        <v>-3.7448422044676728E-3</v>
+        <v>-3.783636025533567E-3</v>
       </c>
       <c r="M10" cm="1">
         <f t="array" aca="1" ref="M10" ca="1">_xll.QCurves_GetCpiForecast($B$30,J10,-3)</f>
-        <v>111.28146982991993</v>
+        <v>111.28146982991991</v>
       </c>
       <c r="N10">
         <v>111.28146982991993</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -5782,29 +5788,29 @@
       <c r="F11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="22">
         <f t="shared" ca="1" si="1"/>
         <v>44660</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="23">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J11)</f>
-        <v>0.99050468498643585</v>
-      </c>
-      <c r="L11" s="24">
+        <v>0.9905431168206783</v>
+      </c>
+      <c r="L11" s="23">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J11,J12,"Linear","Act365F")</f>
-        <v>4.6165208548161734E-3</v>
-      </c>
-      <c r="M11" s="25" cm="1">
+        <v>4.6259394590755206E-3</v>
+      </c>
+      <c r="M11" s="24" cm="1">
         <f t="array" aca="1" ref="M11" ca="1">_xll.QCurves_GetCpiForecast($B$30,J11,-3)</f>
-        <v>113.02192281617025</v>
+        <v>113.02192281617023</v>
       </c>
       <c r="N11">
         <v>113.02192281617025</v>
       </c>
-      <c r="O11" s="26">
+      <c r="O11" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -5820,7 +5826,7 @@
       </c>
       <c r="C12" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xll.QIns_CreateInflationFwd("InfFwd0",A12,B2,B12,100000000,"USD.CPI","USD.OIS.1B","USD.CPI",D12)</f>
-        <v>InfFwd0¬82</v>
+        <v>InfFwd0¬19</v>
       </c>
       <c r="D12" s="2" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">_xll.QDates_AddPeriod(valDate,$B$5,"P","USD")</f>
@@ -5838,11 +5844,11 @@
       </c>
       <c r="K12" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J12)</f>
-        <v>0.98936595621968537</v>
+        <v>0.98940202322815007</v>
       </c>
       <c r="L12" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J12,J13,"Linear","Act365F")</f>
-        <v>4.8510727063655334E-3</v>
+        <v>4.868265453501895E-3</v>
       </c>
       <c r="M12" cm="1">
         <f t="array" aca="1" ref="M12" ca="1">_xll.QCurves_GetCpiForecast($B$30,J12,-3)</f>
@@ -5851,7 +5857,7 @@
       <c r="N12">
         <v>115.10809080132813</v>
       </c>
-      <c r="O12" s="26">
+      <c r="O12" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>8.3274679956176101E-2</v>
       </c>
@@ -5865,7 +5871,7 @@
       </c>
       <c r="C13" t="str" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A13,ComplexBuild!valDate,A13,$B$2,B13,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D13)</f>
-        <v>InfSwap6m¬79</v>
+        <v>InfSwap6m¬9</v>
       </c>
       <c r="D13" s="2" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A13),$B$5)</f>
@@ -5883,11 +5889,11 @@
       </c>
       <c r="K13" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J13)</f>
-        <v>0.98815770009348602</v>
+        <v>0.98818944595200109</v>
       </c>
       <c r="L13" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J13,J14,"Linear","Act365F")</f>
-        <v>4.8702643663097681E-3</v>
+        <v>4.8941923571514962E-3</v>
       </c>
       <c r="M13" cm="1">
         <f t="array" aca="1" ref="M13" ca="1">_xll.QCurves_GetCpiForecast($B$30,J13,-3)</f>
@@ -5896,7 +5902,7 @@
       <c r="N13">
         <v>117.22625235372986</v>
       </c>
-      <c r="O13" s="26">
+      <c r="O13" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0.16938826945630581</v>
       </c>
@@ -5910,7 +5916,7 @@
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A14,ComplexBuild!valDate,A14,$B$2,B14,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D14)</f>
-        <v>InfSwap1y¬78</v>
+        <v>InfSwap1y¬19</v>
       </c>
       <c r="D14" s="2" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A14),$B$5)</f>
@@ -5928,11 +5934,11 @@
       </c>
       <c r="K14" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J14)</f>
-        <v>0.98694615116806661</v>
+        <v>0.98697191281199692</v>
       </c>
       <c r="L14" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J14,J15,"Linear","Act365F")</f>
-        <v>4.8891820475031661E-3</v>
+        <v>4.9197713265708432E-3</v>
       </c>
       <c r="M14" cm="1">
         <f t="array" aca="1" ref="M14" ca="1">_xll.QCurves_GetCpiForecast($B$30,J14,-3)</f>
@@ -5941,7 +5947,7 @@
       <c r="N14">
         <v>119.36769040670744</v>
       </c>
-      <c r="O14" s="26">
+      <c r="O14" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0.25644816213775812</v>
       </c>
@@ -5955,35 +5961,35 @@
       </c>
       <c r="C15" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A15,ComplexBuild!valDate,A15,$B$2,B15,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D15)</f>
-        <v>InfSwap2y¬78</v>
+        <v>InfSwap2y¬19</v>
       </c>
       <c r="D15" s="2" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A15),$B$5)</f>
         <v>44572</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="22">
         <f t="shared" ca="1" si="1"/>
         <v>45025</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="23">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J15)</f>
-        <v>0.98575776917644486</v>
-      </c>
-      <c r="L15" s="24">
+        <v>0.98577607347647955</v>
+      </c>
+      <c r="L15" s="23">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J15,J16,"Linear","Act365F")</f>
-        <v>6.3091638772783849E-3</v>
-      </c>
-      <c r="M15" s="25" cm="1">
+        <v>6.3121810431694941E-3</v>
+      </c>
+      <c r="M15" s="24" cm="1">
         <f t="array" aca="1" ref="M15" ca="1">_xll.QCurves_GetCpiForecast($B$30,J15,-3)</f>
         <v>121.85263651450421</v>
       </c>
       <c r="N15">
         <v>121.509128459685</v>
       </c>
-      <c r="O15" s="26">
+      <c r="O15" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0.34350805481921043</v>
       </c>
@@ -5997,7 +6003,7 @@
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A16,ComplexBuild!valDate,A16,$B$2,B16,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D16)</f>
-        <v>InfSwap3y¬78</v>
+        <v>InfSwap3y¬19</v>
       </c>
       <c r="D16" s="2" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A16),$B$5)</f>
@@ -6009,11 +6015,11 @@
       </c>
       <c r="K16" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J16)</f>
-        <v>0.98420963731310829</v>
+        <v>0.98422717366878043</v>
       </c>
       <c r="L16" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J16,J17,"Linear","Act365F")</f>
-        <v>6.5613257933532371E-3</v>
+        <v>6.5653557753045134E-3</v>
       </c>
       <c r="M16" cm="1">
         <f t="array" aca="1" ref="M16" ca="1">_xll.QCurves_GetCpiForecast($B$30,J16,-3)</f>
@@ -6022,12 +6028,12 @@
       <c r="N16">
         <v>123.91532411304483</v>
       </c>
-      <c r="O16" s="26">
+      <c r="O16" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0.30245923764155691</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
@@ -6036,7 +6042,7 @@
       </c>
       <c r="C17" t="str" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A17,ComplexBuild!valDate,A17,$B$2,B17,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D17)</f>
-        <v>InfSwap5y¬78</v>
+        <v>InfSwap5y¬19</v>
       </c>
       <c r="D17" s="2" cm="1">
         <f t="array" aca="1" ref="D17" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A17),$B$5)</f>
@@ -6048,11 +6054,11 @@
       </c>
       <c r="K17" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J17)</f>
-        <v>0.98258462547215442</v>
+        <v>0.98260113641887803</v>
       </c>
       <c r="L17" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J17,J18,"Linear","Act365F")</f>
-        <v>6.80037086562539E-3</v>
+        <v>6.8057721793557636E-3</v>
       </c>
       <c r="M17" cm="1">
         <f t="array" aca="1" ref="M17" ca="1">_xll.QCurves_GetCpiForecast($B$30,J17,-3)</f>
@@ -6061,12 +6067,12 @@
       <c r="N17">
         <v>126.3517920108352</v>
       </c>
-      <c r="O17" s="26">
+      <c r="O17" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0.25952040671272414</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -6075,7 +6081,7 @@
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">_xll.QIns_CreateInflationBenchmarkSwap("InfSwap" &amp;A18,ComplexBuild!valDate,A18,$B$2,B18,100000000,"USD.CPI","USD.OIS.1B","Pay","USD.CPI",D18)</f>
-        <v>InfSwap10y¬78</v>
+        <v>InfSwap10y¬19</v>
       </c>
       <c r="D18" s="2" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">_xll.QDates_AddPeriod(_xll.QDates_AddPeriod(valDate,A18),$B$5)</f>
@@ -6087,11 +6093,11 @@
       </c>
       <c r="K18" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J18)</f>
-        <v>0.98090329240969876</v>
+        <v>0.98091844194025224</v>
       </c>
       <c r="L18" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J18,J19,"Linear","Act365F")</f>
-        <v>7.0380632261232545E-3</v>
+        <v>7.044828452434487E-3</v>
       </c>
       <c r="M18" cm="1">
         <f t="array" aca="1" ref="M18" ca="1">_xll.QCurves_GetCpiForecast($B$30,J18,-3)</f>
@@ -6100,12 +6106,12 @@
       <c r="N18">
         <v>128.81503428112876</v>
       </c>
-      <c r="O18" s="26">
+      <c r="O18" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0.21610972049896304</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>78</v>
       </c>
@@ -6118,11 +6124,11 @@
       </c>
       <c r="K19" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J19)</f>
-        <v>0.97918512096307153</v>
+        <v>0.97919859526263953</v>
       </c>
       <c r="L19" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J19,J20,"Linear","Act365F")</f>
-        <v>7.8483692645597777E-3</v>
+        <v>7.8405600421535028E-3</v>
       </c>
       <c r="M19" cm="1">
         <f t="array" aca="1" ref="M19" ca="1">_xll.QCurves_GetCpiForecast($B$30,J19,-3)</f>
@@ -6131,18 +6137,18 @@
       <c r="N19">
         <v>131.27827655142232</v>
       </c>
-      <c r="O19" s="26">
+      <c r="O19" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0.17269903428518774</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>64</v>
       </c>
       <c r="B20" t="str">
         <f ca="1">ComplexBuild!C28</f>
-        <v>FundingInstruments_USD¬0</v>
+        <v>FundingInstruments_USD¬4</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
@@ -6156,11 +6162,11 @@
       </c>
       <c r="K20" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J20)</f>
-        <v>0.97727287478823477</v>
+        <v>0.97728822179602359</v>
       </c>
       <c r="L20" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J20,J21,"Linear","Act365F")</f>
-        <v>8.1539496965475442E-3</v>
+        <v>8.1456250046731786E-3</v>
       </c>
       <c r="M20" cm="1">
         <f t="array" aca="1" ref="M20" ca="1">_xll.QCurves_GetCpiForecast($B$30,J20,-3)</f>
@@ -6169,18 +6175,18 @@
       <c r="N20">
         <v>133.71474444921267</v>
       </c>
-      <c r="O20" s="26">
+      <c r="O20" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0.12976020335636917</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>79</v>
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" aca="1" ref="B21" ca="1">_xll.QIns_CreateFundingInstrumentCollection(A21,C12:C18)</f>
-        <v>CPI¬79</v>
+        <v>CPI¬9</v>
       </c>
       <c r="E21" t="s">
         <v>54</v>
@@ -6194,11 +6200,11 @@
       </c>
       <c r="K21" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J21)</f>
-        <v>0.97526846197147277</v>
+        <v>0.97528581972614004</v>
       </c>
       <c r="L21" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J21,J22,"Linear","Act365F")</f>
-        <v>8.4611388513162224E-3</v>
+        <v>8.4522959620484915E-3</v>
       </c>
       <c r="M21" cm="1">
         <f t="array" aca="1" ref="M21" ca="1">_xll.QCurves_GetCpiForecast($B$30,J21,-3)</f>
@@ -6207,18 +6213,18 @@
       <c r="N21">
         <v>136.15121234700302</v>
       </c>
-      <c r="O21" s="26">
+      <c r="O21" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>8.6821372427550614E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>81</v>
       </c>
       <c r="B22" t="str">
         <f ca="1">_xll.QIns_CreateFundingInstrumentCollection(A22,B20:B21)</f>
-        <v>FicCPI¬78</v>
+        <v>FicCPI¬9</v>
       </c>
       <c r="E22" t="s">
         <v>77</v>
@@ -6232,11 +6238,11 @@
       </c>
       <c r="K22" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J22)</f>
-        <v>0.97319296193923055</v>
+        <v>0.97321244732404855</v>
       </c>
       <c r="L22" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J22,J23,"Linear","Act365F")</f>
-        <v>8.7648020218674943E-3</v>
+        <v>8.7554469376984866E-3</v>
       </c>
       <c r="M22" cm="1">
         <f t="array" aca="1" ref="M22" ca="1">_xll.QCurves_GetCpiForecast($B$30,J22,-3)</f>
@@ -6245,40 +6251,40 @@
       <c r="N22">
         <v>138.61445461729659</v>
       </c>
-      <c r="O22" s="26">
+      <c r="O22" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>4.3410686213775307E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I23" s="22" t="s">
+    <row r="23" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="22">
         <f t="shared" ca="1" si="1"/>
         <v>45756</v>
       </c>
-      <c r="K23" s="24">
+      <c r="K23" s="23">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J23)</f>
-        <v>0.97109424852837223</v>
-      </c>
-      <c r="L23" s="24">
+        <v>0.97111592716689865</v>
+      </c>
+      <c r="L23" s="23">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J23,J24,"Linear","Act365F")</f>
-        <v>8.9084999722346507E-3</v>
-      </c>
-      <c r="M23" s="25" cm="1">
+        <v>8.9370100375391979E-3</v>
+      </c>
+      <c r="M23" s="24" cm="1">
         <f t="array" aca="1" ref="M23" ca="1">_xll.QCurves_GetCpiForecast($B$30,J23,-3)</f>
         <v>141.07769688759015</v>
       </c>
       <c r="N23">
         <v>141.07769688759015</v>
       </c>
-      <c r="O23" s="26">
+      <c r="O23" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>27</v>
       </c>
@@ -6287,7 +6293,7 @@
       </c>
       <c r="F24" t="str">
         <f ca="1">ComplexBuild!J28</f>
-        <v>fxMatrix¬0</v>
+        <v>fxMatrix¬3</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -6295,11 +6301,11 @@
       </c>
       <c r="K24" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J24)</f>
-        <v>0.9689422053326282</v>
+        <v>0.96895696385680063</v>
       </c>
       <c r="L24" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J24,J25,"Linear","Act365F")</f>
-        <v>9.1990422107138606E-3</v>
+        <v>9.2307039174912755E-3</v>
       </c>
       <c r="M24" cm="1">
         <f t="array" aca="1" ref="M24" ca="1">_xll.QCurves_GetCpiForecast($B$30,J24,-3)</f>
@@ -6308,25 +6314,32 @@
       <c r="N24">
         <v>144.3421547556126</v>
       </c>
-      <c r="O24" s="26">
+      <c r="O24" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="R24" s="8" t="s">
+      <c r="Q24" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="R24" t="str" cm="1">
+        <f t="array" aca="1" ref="R24" ca="1">_xll.QIns_AssetPortfolioExpectedFlows("CashflowResult",B41,B33)</f>
+        <v>CashflowResult¬25</v>
+      </c>
+      <c r="W24" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="S24" t="str" cm="1">
-        <f t="array" aca="1" ref="S24" ca="1">_xll.QRisk_PortfolioIrBenchmarkDelta(R24,B41,B33,B22,"USD")</f>
-        <v>BenchmarkRisk¬79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X24" t="str" cm="1">
+        <f t="array" aca="1" ref="X24" ca="1">_xll.QRisk_PortfolioIrBenchmarkDelta(W24,B41,B33,B22,"USD")</f>
+        <v>BenchmarkRisk¬28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>80</v>
       </c>
       <c r="B25" t="str" cm="1">
         <f t="array" aca="1" ref="B25" ca="1">_xll.QCurves_CreateFundingModel(A25,valDate,B22,E20:F22,ComplexBuild!J28,,F10)</f>
-        <v>ModelCPI¬81</v>
+        <v>ModelCPI¬9</v>
       </c>
       <c r="E25" t="s">
         <v>64</v>
@@ -6340,86 +6353,106 @@
       </c>
       <c r="K25" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J25)</f>
-        <v>0.96670075236166508</v>
+        <v>0.96670777979465861</v>
       </c>
       <c r="L25" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J25,J26,"Linear","Act365F")</f>
-        <v>9.4910842711828682E-3</v>
+        <v>9.5259146079641564E-3</v>
       </c>
       <c r="M25" cm="1">
         <f t="array" aca="1" ref="M25" ca="1">_xll.QCurves_GetCpiForecast($B$30,J25,-3)</f>
-        <v>147.64288437772422</v>
+        <v>147.64288437772419</v>
       </c>
       <c r="N25">
         <v>147.64288437772422</v>
       </c>
-      <c r="O25" s="26">
+      <c r="O25" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J26" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>46031</v>
       </c>
       <c r="K26" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J26)</f>
-        <v>0.96439365916425557</v>
+        <v>0.96439222348453846</v>
       </c>
       <c r="L26" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J26,J27,"Linear","Act365F")</f>
-        <v>9.7797112314272662E-3</v>
+        <v>9.8176741808606461E-3</v>
       </c>
       <c r="M26" cm="1">
         <f t="array" aca="1" ref="M26" ca="1">_xll.QCurves_GetCpiForecast($B$30,J26,-3)</f>
-        <v>150.97988575392495</v>
+        <v>150.97988575392492</v>
       </c>
       <c r="N26">
         <v>150.97988575392495</v>
       </c>
-      <c r="O26" s="26">
+      <c r="O26" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="Q26" s="14" t="str">
-        <f t="array" aca="1" ref="Q26:Y40" ca="1">_xll.QCube_DisplayCube(S24)</f>
+        <f t="array" aca="1" ref="Q26:U40" ca="1">_xll.QCube_DisplayCube(R24)</f>
         <v>TradeId</v>
       </c>
       <c r="R26" s="14" t="str">
         <f ca="1"/>
+        <v>Currency</v>
+      </c>
+      <c r="S26" s="14" t="str">
+        <f ca="1"/>
         <v>TradeType</v>
       </c>
-      <c r="S26" s="14" t="str">
+      <c r="T26" s="14" t="str">
+        <f ca="1"/>
+        <v>PayDate</v>
+      </c>
+      <c r="U26" s="14" t="str">
+        <f ca="1"/>
+        <v>Value</v>
+      </c>
+      <c r="W26" s="14" t="str">
+        <f t="array" aca="1" ref="W26:AE57" ca="1">_xll.QCube_DisplayCube(X24)</f>
+        <v>TradeId</v>
+      </c>
+      <c r="X26" s="14" t="str">
+        <f ca="1"/>
+        <v>TradeType</v>
+      </c>
+      <c r="Y26" s="14" t="str">
         <f ca="1"/>
         <v>Curve</v>
       </c>
-      <c r="T26" s="14" t="str">
+      <c r="Z26" s="14" t="str">
         <f ca="1"/>
         <v>RiskDate</v>
       </c>
-      <c r="U26" s="14" t="str">
+      <c r="AA26" s="14" t="str">
         <f ca="1"/>
         <v>Benchmark</v>
       </c>
-      <c r="V26" s="14" t="str">
+      <c r="AB26" s="14" t="str">
         <f ca="1"/>
         <v>Metric</v>
       </c>
-      <c r="W26" s="14" t="str">
+      <c r="AC26" s="14" t="str">
         <f ca="1"/>
         <v>Units</v>
       </c>
-      <c r="X26" s="14" t="str">
+      <c r="AD26" s="14" t="str">
         <f ca="1"/>
         <v>BumpSize</v>
       </c>
-      <c r="Y26" s="14" t="str">
+      <c r="AE26" s="14" t="str">
         <f ca="1"/>
         <v>Value</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>85</v>
       </c>
@@ -6429,68 +6462,88 @@
       </c>
       <c r="K27" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J27)</f>
-        <v>0.96207368039716601</v>
+        <v>0.96206326422356037</v>
       </c>
       <c r="L27" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J27,J28,"Linear","Act365F")</f>
-        <v>1.0067156644269194E-2</v>
+        <v>1.0108238374720333E-2</v>
       </c>
       <c r="M27" cm="1">
         <f t="array" aca="1" ref="M27" ca="1">_xll.QCurves_GetCpiForecast($B$30,J27,-3)</f>
-        <v>154.31688713012568</v>
+        <v>154.31688713012565</v>
       </c>
       <c r="N27">
         <v>154.31688713012568</v>
       </c>
-      <c r="O27" s="26">
+      <c r="O27" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="13" t="str">
+      <c r="Q27" t="str">
         <f ca="1"/>
         <v>TradeObj</v>
       </c>
-      <c r="R27" s="13" t="str">
+      <c r="R27" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="S27" t="str">
         <f ca="1"/>
         <v>InfPerfSwap</v>
       </c>
-      <c r="S27" s="13" t="str">
+      <c r="T27" s="2">
+        <f ca="1"/>
+        <v>46114</v>
+      </c>
+      <c r="U27" s="4">
+        <f ca="1"/>
+        <v>13464460.265854279</v>
+      </c>
+      <c r="W27" s="13" t="str">
+        <f ca="1"/>
+        <v>TradeObj</v>
+      </c>
+      <c r="X27" s="13" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="Y27" s="13" t="str">
         <f ca="1"/>
         <v>USD.CPI</v>
       </c>
-      <c r="T27" s="19">
+      <c r="Z27" s="19">
         <f ca="1"/>
         <v>45666</v>
       </c>
-      <c r="U27" s="20" t="str">
+      <c r="AA27" s="20" t="str">
         <f ca="1"/>
         <v>InfSwap5y</v>
       </c>
-      <c r="V27" s="13" t="str">
+      <c r="AB27" s="13" t="str">
         <f ca="1"/>
         <v>IrBenchmarkDelta</v>
       </c>
-      <c r="W27" s="13" t="str">
+      <c r="AC27" s="13" t="str">
         <f ca="1"/>
         <v>Nominal</v>
       </c>
-      <c r="X27" s="13">
+      <c r="AD27" s="13">
         <f ca="1"/>
         <v>0.01</v>
       </c>
-      <c r="Y27" s="20">
-        <f ca="1"/>
-        <v>20099019.285653304</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AE27" s="20">
+        <f ca="1"/>
+        <v>20098639.799651146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="array" aca="1" ref="A28:A30" ca="1">_xll.QCurves_ListCurvesInModel(B25)</f>
         <v>USD.LIBOR.3M</v>
       </c>
       <c r="B28" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A28,"curve.cpiBuild."&amp;A28)</f>
-        <v>curve.cpiBuild.USD.LIBOR.3M¬78</v>
+        <v>curve.cpiBuild.USD.LIBOR.3M¬9</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -6498,11 +6551,11 @@
       </c>
       <c r="K28" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J28)</f>
-        <v>0.95966502305936319</v>
+        <v>0.95964482860679623</v>
       </c>
       <c r="L28" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J28,J29,"Linear","Act365F")</f>
-        <v>1.0357813597547285E-2</v>
+        <v>1.0402049253073921E-2</v>
       </c>
       <c r="M28" cm="1">
         <f t="array" aca="1" ref="M28" ca="1">_xll.QCurves_GetCpiForecast($B$30,J28,-3)</f>
@@ -6511,55 +6564,75 @@
       <c r="N28">
         <v>157.58134499814813</v>
       </c>
-      <c r="O28" s="26">
+      <c r="O28" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="13" t="str">
+      <c r="Q28" t="str">
         <f ca="1"/>
         <v>TradeObj</v>
       </c>
-      <c r="R28" s="13" t="str">
+      <c r="R28" t="str">
+        <f ca="1"/>
+        <v>USD</v>
+      </c>
+      <c r="S28" t="str">
         <f ca="1"/>
         <v>InfPerfSwap</v>
       </c>
-      <c r="S28" s="13" t="str">
+      <c r="T28" s="2">
+        <f ca="1"/>
+        <v>46114</v>
+      </c>
+      <c r="U28" s="4">
+        <f ca="1"/>
+        <v>-12513071.695675237</v>
+      </c>
+      <c r="W28" s="13" t="str">
+        <f ca="1"/>
+        <v>TradeObj</v>
+      </c>
+      <c r="X28" s="13" t="str">
+        <f ca="1"/>
+        <v>InfPerfSwap</v>
+      </c>
+      <c r="Y28" s="13" t="str">
         <f ca="1"/>
         <v>USD.CPI</v>
       </c>
-      <c r="T28" s="19">
+      <c r="Z28" s="19">
         <f ca="1"/>
         <v>47492</v>
       </c>
-      <c r="U28" s="20" t="str">
+      <c r="AA28" s="20" t="str">
         <f ca="1"/>
         <v>InfSwap10y</v>
       </c>
-      <c r="V28" s="13" t="str">
+      <c r="AB28" s="13" t="str">
         <f ca="1"/>
         <v>IrBenchmarkDelta</v>
       </c>
-      <c r="W28" s="13" t="str">
+      <c r="AC28" s="13" t="str">
         <f ca="1"/>
         <v>Nominal</v>
       </c>
-      <c r="X28" s="13">
+      <c r="AD28" s="13">
         <f ca="1"/>
         <v>0.01</v>
       </c>
-      <c r="Y28" s="20">
-        <f ca="1"/>
-        <v>5067916.5794108231</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="AE28" s="20">
+        <f ca="1"/>
+        <v>5068687.6511816857</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f ca="1"/>
         <v>USD.OIS.1B</v>
       </c>
       <c r="B29" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A29,"curve.cpiBuild."&amp;A29)</f>
-        <v>curve.cpiBuild.USD.OIS.1B¬78</v>
+        <v>curve.cpiBuild.USD.OIS.1B¬9</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -6567,11 +6640,11 @@
       </c>
       <c r="K29" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J29)</f>
-        <v>0.95716611447307476</v>
+        <v>0.95713532851836425</v>
       </c>
       <c r="L29" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J29,J30,"Linear","Act365F")</f>
-        <v>1.0649940758556239E-2</v>
+        <v>1.0697346900180484E-2</v>
       </c>
       <c r="M29" cm="1">
         <f t="array" aca="1" ref="M29" ca="1">_xll.QCurves_GetCpiForecast($B$30,J29,-3)</f>
@@ -6580,31 +6653,27 @@
       <c r="N29">
         <v>160.88207462025971</v>
       </c>
-      <c r="O29" s="26">
+      <c r="O29" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q29" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R29" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S29" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T29" s="19" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U29" s="20" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V29" s="13" t="e">
+      <c r="Q29" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R29" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S29" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T29" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U29" s="4" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -6616,19 +6685,43 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="Y29" s="20" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z29" s="19" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA29" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD29" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE29" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f ca="1"/>
         <v>USD.CPI</v>
       </c>
       <c r="B30" t="str">
         <f ca="1">_xll.QCurves_ExtractCurveFromModel($B$25,A30,"curve.cpiBuild."&amp;A30)</f>
-        <v>curve.cpiBuild.USD.CPI¬78</v>
+        <v>curve.cpiBuild.USD.CPI¬9</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -6636,11 +6729,11 @@
       </c>
       <c r="K30" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J30)</f>
-        <v>0.95460360649813214</v>
+        <v>0.95456152749551193</v>
       </c>
       <c r="L30" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J30,J31,"Linear","Act365F")</f>
-        <v>1.0938586201982145E-2</v>
+        <v>1.0989125796056969E-2</v>
       </c>
       <c r="M30" cm="1">
         <f t="array" aca="1" ref="M30" ca="1">_xll.QCurves_GetCpiForecast($B$30,J30,-3)</f>
@@ -6649,31 +6742,27 @@
       <c r="N30">
         <v>164.21907599646045</v>
       </c>
-      <c r="O30" s="26">
+      <c r="O30" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R30" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S30" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T30" s="19" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U30" s="20" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V30" s="13" t="e">
+      <c r="Q30" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R30" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S30" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T30" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U30" s="4" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -6685,23 +6774,47 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="Y30" s="20" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z30" s="19" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA30" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD30" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE30" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J31" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>46486</v>
       </c>
       <c r="K31" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J31)</f>
-        <v>0.95203578923972831</v>
+        <v>0.9519819919124336</v>
       </c>
       <c r="L31" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J31,J32,"Linear","Act365F")</f>
-        <v>1.174513824912918E-2</v>
+        <v>1.1747452470901648E-2</v>
       </c>
       <c r="M31" cm="1">
         <f t="array" aca="1" ref="M31" ca="1">_xll.QCurves_GetCpiForecast($B$30,J31,-3)</f>
@@ -6710,31 +6823,27 @@
       <c r="N31">
         <v>167.55607737266118</v>
       </c>
-      <c r="O31" s="26">
+      <c r="O31" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q31" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R31" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S31" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T31" s="19" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U31" s="20" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V31" s="13" t="e">
+      <c r="Q31" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R31" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S31" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T31" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U31" s="4" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -6746,12 +6855,36 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="Y31" s="20" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z31" s="19" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA31" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD31" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE31" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>89</v>
       </c>
@@ -6761,44 +6894,40 @@
       </c>
       <c r="K32" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J32)</f>
-        <v>0.94925613949209153</v>
+        <v>0.94920195317394584</v>
       </c>
       <c r="L32" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J32,J33,"Linear","Act365F")</f>
-        <v>1.2071854462021157E-2</v>
+        <v>1.2073769371609916E-2</v>
       </c>
       <c r="M32" cm="1">
         <f t="array" aca="1" ref="M32" ca="1">_xll.QCurves_GetCpiForecast($B$30,J32,-3)</f>
-        <v>170.82053524068365</v>
+        <v>170.82053524068363</v>
       </c>
       <c r="N32">
         <v>170.82053524068365</v>
       </c>
-      <c r="O32" s="26">
+      <c r="O32" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R32" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S32" s="13" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T32" s="19" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U32" s="20" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V32" s="13" t="e">
+      <c r="Q32" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R32" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="S32" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T32" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U32" s="4" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>
@@ -6810,19 +6939,43 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="Y32" s="20" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z32" s="19" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA32" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD32" s="13" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE32" s="20" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f ca="1">A32</f>
         <v>AssetFxModel</v>
       </c>
       <c r="B33" t="str" cm="1">
         <f t="array" aca="1" ref="B33" ca="1">_xll.QCurves_CreateAssetFxModel(A33,valDate,,,B25)</f>
-        <v>AssetFxModel¬78</v>
+        <v>AssetFxModel¬25</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -6832,20 +6985,20 @@
       </c>
       <c r="K33" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J33)</f>
-        <v>0.94637653450372528</v>
+        <v>0.94632205719360685</v>
       </c>
       <c r="L33" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J33,J34,"Linear","Act365F")</f>
-        <v>1.2400193204532005E-2</v>
+        <v>1.2401706479070606E-2</v>
       </c>
       <c r="M33" cm="1">
         <f t="array" aca="1" ref="M33" ca="1">_xll.QCurves_GetCpiForecast($B$30,J33,-3)</f>
-        <v>174.12126486279524</v>
+        <v>174.12126486279521</v>
       </c>
       <c r="N33">
         <v>174.12126486279524</v>
       </c>
-      <c r="O33" s="26">
+      <c r="O33" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -6869,10 +7022,6 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="V33" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="W33" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6885,14 +7034,38 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z33" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA33" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD33" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE33" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>90</v>
       </c>
       <c r="B34" t="str" cm="1">
         <f t="array" aca="1" ref="B34" ca="1">_xll.QIns_CreatePortfolio(A34,C13:C18)</f>
-        <v>Porfolio¬78</v>
+        <v>Porfolio¬9</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -6902,20 +7075,20 @@
       </c>
       <c r="K34" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J34)</f>
-        <v>0.94342782428126781</v>
+        <v>0.94337315800310673</v>
       </c>
       <c r="L34" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J34,J35,"Linear","Act365F")</f>
-        <v>1.2726552729230234E-2</v>
+        <v>1.2727666447033307E-2</v>
       </c>
       <c r="M34" cm="1">
         <f t="array" aca="1" ref="M34" ca="1">_xll.QCurves_GetCpiForecast($B$30,J34,-3)</f>
-        <v>177.45826623899598</v>
+        <v>177.45826623899595</v>
       </c>
       <c r="N34">
         <v>177.45826623899598</v>
       </c>
-      <c r="O34" s="26">
+      <c r="O34" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -6939,10 +7112,6 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="V34" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="W34" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -6955,31 +7124,55 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z34" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA34" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD34" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE34" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="H35" s="27"/>
+      <c r="H35" s="26"/>
       <c r="J35" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>46852</v>
       </c>
       <c r="K35" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J35)</f>
-        <v>0.94044386983374129</v>
+        <v>0.94038911616997289</v>
       </c>
       <c r="L35" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J35,J36,"Linear","Act365F")</f>
-        <v>1.3051364424061372E-2</v>
+        <v>1.305208075525594E-2</v>
       </c>
       <c r="M35" cm="1">
         <f t="array" aca="1" ref="M35" ca="1">_xll.QCurves_GetCpiForecast($B$30,J35,-3)</f>
-        <v>180.79526761519671</v>
+        <v>180.79526761519668</v>
       </c>
       <c r="N35">
         <v>180.79526761519671</v>
       </c>
-      <c r="O35" s="26">
+      <c r="O35" s="25">
         <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
@@ -7003,10 +7196,6 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="V35" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="W35" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -7019,34 +7208,58 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z35" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA35" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD35" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE35" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="H36" s="27"/>
+      <c r="H36" s="26"/>
       <c r="J36" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>46943</v>
       </c>
       <c r="K36" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J36)</f>
-        <v>0.93739368282752511</v>
+        <v>0.93733893989051209</v>
       </c>
       <c r="L36" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J36,J37,"Linear","Act365F")</f>
-        <v>1.3378232131234452E-2</v>
+        <v>1.3378548839313199E-2</v>
       </c>
       <c r="M36" cm="1">
         <f t="array" aca="1" ref="M36" ca="1">_xll.QCurves_GetCpiForecast($B$30,J36,-3)</f>
-        <v>184.0959972373083</v>
+        <v>184.09599723730827</v>
       </c>
       <c r="N36">
         <v>184.0959972373083</v>
       </c>
-      <c r="O36" s="26">
+      <c r="O36" s="25">
         <f t="shared" ref="O36:O50" ca="1" si="2">M36-N36</f>
         <v>0</v>
       </c>
@@ -7070,10 +7283,6 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="V36" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="W36" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -7086,8 +7295,32 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z36" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA36" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD36" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE36" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>93</v>
       </c>
@@ -7097,27 +7330,27 @@
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="H37" s="27"/>
+      <c r="H37" s="26"/>
       <c r="J37" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>47035</v>
       </c>
       <c r="K37" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J37)</f>
-        <v>0.93424336976059208</v>
+        <v>0.93418873647539247</v>
       </c>
       <c r="L37" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J37,J38,"Linear","Act365F")</f>
-        <v>1.3724276514456651E-2</v>
+        <v>1.3724275432627111E-2</v>
       </c>
       <c r="M37" cm="1">
         <f t="array" aca="1" ref="M37" ca="1">_xll.QCurves_GetCpiForecast($B$30,J37,-3)</f>
-        <v>187.39672685941991</v>
+        <v>187.39672685941986</v>
       </c>
       <c r="N37">
         <v>187.39672685941991</v>
       </c>
-      <c r="O37" s="26">
+      <c r="O37" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
@@ -7141,10 +7374,6 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="V37" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="W37" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -7157,8 +7386,32 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z37" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA37" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD37" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE37" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -7174,11 +7427,11 @@
       </c>
       <c r="K38" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J38)</f>
-        <v>0.93102271110902513</v>
+        <v>0.93096826641655694</v>
       </c>
       <c r="L38" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J38,J39,"Linear","Act365F")</f>
-        <v>1.4042264430980828E-2</v>
+        <v>1.4042264407516129E-2</v>
       </c>
       <c r="M38" cm="1">
         <f t="array" aca="1" ref="M38" ca="1">_xll.QCurves_GetCpiForecast($B$30,J38,-3)</f>
@@ -7187,7 +7440,7 @@
       <c r="N38">
         <v>190.73372823562062</v>
       </c>
-      <c r="O38" s="26">
+      <c r="O38" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
@@ -7211,10 +7464,6 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="V38" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="W38" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -7227,12 +7476,36 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z38" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA38" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD38" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE38" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>100</v>
       </c>
-      <c r="B39" s="28">
+      <c r="B39" s="27">
         <v>25000000</v>
       </c>
       <c r="D39" s="2"/>
@@ -7243,20 +7516,20 @@
       </c>
       <c r="K39" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J39)</f>
-        <v>0.92781019044262547</v>
+        <v>0.9277559336184853</v>
       </c>
       <c r="L39" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J39,J40,"Linear","Act365F")</f>
-        <v>1.406428851736794E-2</v>
+        <v>1.4064285836837904E-2</v>
       </c>
       <c r="M39" cm="1">
         <f t="array" aca="1" ref="M39" ca="1">_xll.QCurves_GetCpiForecast($B$30,J39,-3)</f>
-        <v>194.07072961182138</v>
+        <v>194.07072961182132</v>
       </c>
       <c r="N39">
         <v>194.07072961182138</v>
       </c>
-      <c r="O39" s="26">
+      <c r="O39" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
@@ -7280,10 +7553,6 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="V39" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="W39" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -7296,8 +7565,32 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z39" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA39" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD39" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE39" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -7310,20 +7603,20 @@
       </c>
       <c r="K40" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J40)</f>
-        <v>0.92456824822801198</v>
+        <v>0.92451418160304677</v>
       </c>
       <c r="L40" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J40,J41,"Linear","Act365F")</f>
-        <v>1.4164353801983555E-2</v>
+        <v>1.4164355045629925E-2</v>
       </c>
       <c r="M40" cm="1">
         <f t="array" aca="1" ref="M40" ca="1">_xll.QCurves_GetCpiForecast($B$30,J40,-3)</f>
-        <v>197.33518747984382</v>
+        <v>197.3351874798438</v>
       </c>
       <c r="N40">
         <v>197.33518747984382</v>
       </c>
-      <c r="O40" s="26">
+      <c r="O40" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
@@ -7347,10 +7640,6 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-      <c r="V40" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
       <c r="W40" t="e">
         <f ca="1"/>
         <v>#N/A</v>
@@ -7363,14 +7652,38 @@
         <f ca="1"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z40" s="2" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA40" s="18" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD40" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE40" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>96</v>
       </c>
       <c r="B41" t="str" cm="1">
         <f t="array" aca="1" ref="B41" ca="1">_xll.QIns_CreateInflationPerfSwap(A41,B37,B38,B2,B40,B39,"USD.CPI","USD.OIS.1B","Pay")</f>
-        <v>TradeObj¬81</v>
+        <v>TradeObj¬25</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -7378,568 +7691,871 @@
       </c>
       <c r="K41" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J41)</f>
-        <v>0.92127910375625865</v>
+        <v>0.92122522918515171</v>
       </c>
       <c r="L41" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J41,J42,"Linear","Act365F")</f>
-        <v>9.6463533021110826E-3</v>
+        <v>9.7378719579023429E-3</v>
       </c>
       <c r="M41" cm="1">
         <f t="array" aca="1" ref="M41" ca="1">_xll.QCurves_GetCpiForecast($B$30,J41,-3)</f>
-        <v>200.63591710195541</v>
+        <v>200.63591710195539</v>
       </c>
       <c r="N41">
         <v>200.63591710195541</v>
       </c>
-      <c r="O41" s="26">
+      <c r="O41" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W41" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X41" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y41" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z41" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA41" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB41" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC41" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD41" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE41" s="4" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J42" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>47492</v>
       </c>
       <c r="K42" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J42)</f>
-        <v>0.9190445300635528</v>
+        <v>0.9189696390525407</v>
       </c>
       <c r="L42" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J42,J43,"Linear","Act365F")</f>
-        <v>-6.4213756726114674E-3</v>
+        <v>-6.0096606368741558E-3</v>
       </c>
       <c r="M42" cm="1">
         <f t="array" aca="1" ref="M42" ca="1">_xll.QCurves_GetCpiForecast($B$30,J42,-3)</f>
-        <v>203.97291847815615</v>
+        <v>203.97291847815612</v>
       </c>
       <c r="N42">
         <v>203.97291847815615</v>
       </c>
-      <c r="O42" s="26">
+      <c r="O42" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q42" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="R42" t="str" cm="1">
-        <f t="array" aca="1" ref="R42" ca="1">_xll.QIns_AssetPortfolioExpectedFlows("CashflowResult",B41,B33)</f>
-        <v>CashflowResult¬78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I43" s="22" t="s">
+      <c r="W42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE42" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I43" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="23">
+      <c r="J43" s="22">
         <f t="shared" ca="1" si="1"/>
         <v>47582</v>
       </c>
-      <c r="K43" s="24">
+      <c r="K43" s="23">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J43)</f>
-        <v>0.92050200959503314</v>
-      </c>
-      <c r="L43" s="24">
+        <v>0.9203334205257242</v>
+      </c>
+      <c r="L43" s="23">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J43,J44,"Linear","Act365F")</f>
-        <v>8.2876233266823661E-3</v>
-      </c>
-      <c r="M43" s="25" cm="1">
+        <v>8.3059677455544871E-3</v>
+      </c>
+      <c r="M43" s="24" cm="1">
         <f t="array" aca="1" ref="M43" ca="1">_xll.QCurves_GetCpiForecast($B$30,J43,-3)</f>
-        <v>207.30991985435688</v>
+        <v>207.30991985435685</v>
       </c>
       <c r="N43">
         <v>207.30991985435688</v>
       </c>
-      <c r="O43" s="26">
+      <c r="O43" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="W43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE43" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J44" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>47673</v>
       </c>
       <c r="K44" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J44)</f>
-        <v>0.91860396310033687</v>
+        <v>0.91843152983432508</v>
       </c>
       <c r="L44" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J44,J45,"Linear","Act365F")</f>
-        <v>8.2877173512875477E-3</v>
+        <v>8.3060621867200989E-3</v>
       </c>
       <c r="M44" cm="1">
         <f t="array" aca="1" ref="M44" ca="1">_xll.QCurves_GetCpiForecast($B$30,J44,-3)</f>
-        <v>210.57437772237932</v>
+        <v>210.5743777223793</v>
       </c>
       <c r="N44">
         <v>210.57437772237932</v>
       </c>
-      <c r="O44" s="26">
+      <c r="O44" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q44" s="14" t="str">
-        <f t="array" aca="1" ref="Q44:U58" ca="1">_xll.QCube_DisplayCube(R42)</f>
-        <v>TradeId</v>
-      </c>
-      <c r="R44" s="14" t="str">
-        <f ca="1"/>
-        <v>Currency</v>
-      </c>
-      <c r="S44" s="14" t="str">
-        <f ca="1"/>
-        <v>TradeType</v>
-      </c>
-      <c r="T44" s="14" t="str">
-        <f ca="1"/>
-        <v>PayDate</v>
-      </c>
-      <c r="U44" s="14" t="str">
-        <f ca="1"/>
-        <v>Value</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="W44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE44" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J45" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>47765</v>
       </c>
       <c r="K45" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J45)</f>
-        <v>0.91668903738264296</v>
+        <v>0.91651273453937587</v>
       </c>
       <c r="L45" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J45,J46,"Linear","Act365F")</f>
-        <v>8.2877173512875477E-3</v>
+        <v>8.3060621867200989E-3</v>
       </c>
       <c r="M45" cm="1">
         <f t="array" aca="1" ref="M45" ca="1">_xll.QCurves_GetCpiForecast($B$30,J45,-3)</f>
-        <v>213.87510734449094</v>
+        <v>213.87510734449089</v>
       </c>
       <c r="N45">
         <v>213.87510734449094</v>
       </c>
-      <c r="O45" s="26">
+      <c r="O45" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q45" t="str">
-        <f ca="1"/>
-        <v>TradeObj</v>
-      </c>
-      <c r="R45" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="S45" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="T45" s="2">
-        <f ca="1"/>
-        <v>46114</v>
-      </c>
-      <c r="U45" s="4">
-        <f ca="1"/>
-        <v>13464460.265854284</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="W45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE45" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J46" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>47857</v>
       </c>
       <c r="K46" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J46)</f>
-        <v>0.91477810352722211</v>
+        <v>0.91459794800856886</v>
       </c>
       <c r="L46" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J46,J47,"Linear","Act365F")</f>
-        <v>8.2875293034977808E-3</v>
+        <v>8.3058733058206657E-3</v>
       </c>
       <c r="M46" cm="1">
         <f t="array" aca="1" ref="M46" ca="1">_xll.QCurves_GetCpiForecast($B$30,J46,-3)</f>
-        <v>217.21210872069167</v>
+        <v>217.21210872069162</v>
       </c>
       <c r="N46">
         <v>217.21210872069167</v>
       </c>
-      <c r="O46" s="26">
+      <c r="O46" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q46" t="str">
-        <f ca="1"/>
-        <v>TradeObj</v>
-      </c>
-      <c r="R46" t="str">
-        <f ca="1"/>
-        <v>USD</v>
-      </c>
-      <c r="S46" t="str">
-        <f ca="1"/>
-        <v>InfPerfSwap</v>
-      </c>
-      <c r="T46" s="2">
-        <f ca="1"/>
-        <v>46114</v>
-      </c>
-      <c r="U46" s="4">
-        <f ca="1"/>
-        <v>-12513071.695675237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="W46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE46" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J47" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>47947</v>
       </c>
       <c r="K47" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J47)</f>
-        <v>0.91291256635443463</v>
+        <v>0.91272865821734406</v>
       </c>
       <c r="L47" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J47,J48,"Linear","Act365F")</f>
-        <v>8.2876233266823661E-3</v>
+        <v>8.3059677455544871E-3</v>
       </c>
       <c r="M47" cm="1">
         <f t="array" aca="1" ref="M47" ca="1">_xll.QCurves_GetCpiForecast($B$30,J47,-3)</f>
-        <v>220.54911009689241</v>
+        <v>220.54911009689235</v>
       </c>
       <c r="N47">
         <v>220.54911009689241</v>
       </c>
-      <c r="O47" s="26">
+      <c r="O47" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q47" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R47" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S47" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T47" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U47" s="4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="W47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE47" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="J48" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>48038</v>
       </c>
       <c r="K48" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J48)</f>
-        <v>0.91103016905549172</v>
+        <v>0.9108424829463807</v>
       </c>
       <c r="L48" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J48,J49,"Linear","Act365F")</f>
-        <v>8.2877173512875477E-3</v>
+        <v>8.3060621867200989E-3</v>
       </c>
       <c r="M48" cm="1">
         <f t="array" aca="1" ref="M48" ca="1">_xll.QCurves_GetCpiForecast($B$30,J48,-3)</f>
-        <v>223.81356796491485</v>
+        <v>223.81356796491482</v>
       </c>
       <c r="N48">
         <v>223.81356796491485</v>
       </c>
-      <c r="O48" s="26">
+      <c r="O48" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q48" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R48" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S48" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T48" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U48" s="4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="49" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="W48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE48" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="10:31" x14ac:dyDescent="0.25">
       <c r="J49" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>48130</v>
       </c>
       <c r="K49" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J49)</f>
-        <v>0.90913103170098752</v>
+        <v>0.90893954275547428</v>
       </c>
       <c r="L49" s="1">
         <f ca="1">_xll.QCurves_GetForwardRate($B$28,J49,J50,"Linear","Act365F")</f>
-        <v>8.2877173512875477E-3</v>
+        <v>8.3060621867200989E-3</v>
       </c>
       <c r="M49" cm="1">
         <f t="array" aca="1" ref="M49" ca="1">_xll.QCurves_GetCpiForecast($B$30,J49,-3)</f>
-        <v>227.11429758702644</v>
+        <v>227.11429758702641</v>
       </c>
       <c r="N49">
         <v>227.11429758702644</v>
       </c>
-      <c r="O49" s="26">
+      <c r="O49" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q49" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R49" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S49" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T49" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U49" s="4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="50" spans="10:21" x14ac:dyDescent="0.25">
+      <c r="W49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE49" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="10:31" x14ac:dyDescent="0.25">
       <c r="J50" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>48222</v>
       </c>
       <c r="K50" s="1">
         <f ca="1">_xll.QCurves_GetDF($B$28,valDate,J50)</f>
-        <v>0.90723585329626766</v>
+        <v>0.90704057820408612</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" cm="1">
         <f t="array" aca="1" ref="M50" ca="1">_xll.QCurves_GetCpiForecast($B$30,J50,-3)</f>
-        <v>230.45129896322717</v>
+        <v>230.45129896322715</v>
       </c>
       <c r="N50">
         <v>230.45129896322717</v>
       </c>
-      <c r="O50" s="26">
+      <c r="O50" s="25">
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q50" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R50" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S50" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T50" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U50" s="4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="51" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="Q51" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R51" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S51" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T51" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U51" s="4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="52" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="Q52" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R52" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S52" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T52" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U52" s="4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="53" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="Q53" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R53" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S53" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T53" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U53" s="4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="54" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="Q54" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R54" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S54" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T54" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U54" s="4" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="55" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="Q55" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R55" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S55" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T55" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U55" s="18" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="56" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="Q56" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R56" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S56" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T56" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U56" s="18" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="57" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="Q57" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R57" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S57" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T57" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U57" s="18" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="58" spans="10:21" x14ac:dyDescent="0.25">
-      <c r="Q58" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R58" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="S58" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T58" s="2" t="e">
-        <f ca="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U58" s="18" t="e">
+      <c r="W50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE50" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="10:31" x14ac:dyDescent="0.25">
+      <c r="W51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE51" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="10:31" x14ac:dyDescent="0.25">
+      <c r="W52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE52" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="10:31" x14ac:dyDescent="0.25">
+      <c r="W53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE53" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="10:31" x14ac:dyDescent="0.25">
+      <c r="W54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE54" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="10:31" x14ac:dyDescent="0.25">
+      <c r="W55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE55" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="10:31" x14ac:dyDescent="0.25">
+      <c r="W56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE56" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="10:31" x14ac:dyDescent="0.25">
+      <c r="W57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Y57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Z57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AA57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AB57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AC57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AD57" t="e">
+        <f ca="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AE57" t="e">
         <f ca="1"/>
         <v>#N/A</v>
       </c>

</xml_diff>